<commit_message>
Geracao de notas por criterios pelo gpt
</commit_message>
<xml_diff>
--- a/letterboxd_scraping/movie_info.xlsx
+++ b/letterboxd_scraping/movie_info.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q6"/>
+  <dimension ref="A1:V6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,45 +471,70 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Public Opinion</t>
+          <t>Script</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
+          <t>VFX</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Casting</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>SFX</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Editing</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Directing</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
           <t>Keywords</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Domestic</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>International</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Worldwide</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Domestic Oppening</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Distributor</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>MPAA</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>Genres</t>
         </is>
@@ -543,42 +568,55 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>"Everything Everywhere All at Once" is a visually stunning and emotionally resonant film that explores themes of multiverses, family dynamics, and the significance of every choice we make. With a mix of humor, action, and heart, this movie has left a lasting impact on viewers, with some calling it one of their favorite films of all time. Featuring a standout performance from Jamie Lee Curtis and a unique take on the multiverse concept, this movie is a must-watch for anyone looking for a truly original cinematic experience.</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>Based on the reviews, it seems that public opinion on Everything Everywhere All at Once is overwhelmingly positive. Many reviewers praise the film for its originality, emotional depth, and technical brilliance. Some even go as far as to call it one of the greatest movies of all time. The film's exploration of multiverses, themes of love and connection, and its unique blend of humor and emotion seem to have resonated with audiences. Overall, it appears that the majority of viewers highly recommend watching Everything Everywhere All at Once.</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>- audacious - funny - original - technically dazzling - thematically resonant - genetically engineered - multiverse - greatest movie of all time - required viewing - therapy - overwhelming - love - homage - crying - action blockbusters - kinetic - daring - expertly choreographed - endlessly creative - emotional core - intelligent filmmaking - lowbrow humor - multiverses - hot - competing realities - haunting - mommy issues - nihilist lesbian representation - pride month</t>
-        </is>
+          <t>"Everything Everywhere All at Once" is a visually stunning and emotionally resonant film that explores themes of multiverses, family dynamics, and the significance of every choice we make. With a mix of humor, action, and heartfelt moments, this movie has left a lasting impact on viewers, making it a must-watch for audiences of all ages. The film has been praised for its originality, technical brilliance, and powerful storytelling, making it a standout in the world of cinema.</t>
+        </is>
+      </c>
+      <c r="I2" t="n">
+        <v>9</v>
+      </c>
+      <c r="J2" t="n">
+        <v>8</v>
       </c>
       <c r="K2" t="n">
+        <v>9</v>
+      </c>
+      <c r="L2" t="n">
+        <v>8</v>
+      </c>
+      <c r="M2" t="n">
+        <v>8</v>
+      </c>
+      <c r="N2" t="n">
+        <v>9</v>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>- audacious - funny - original - technically dazzling - thematically resonant - genetically engineered - greatest multiverse movie - required viewing - everything matters - overwhelming - in love - homage - emotional core - chaotic balance - intelligent filmmaking - lowbrow humor - hot right now - competing realities - haunting - mommy issues - nihilist lesbian representation - pride month</t>
+        </is>
+      </c>
+      <c r="P2" t="n">
         <v>77191785</v>
       </c>
-      <c r="L2" t="n">
+      <c r="Q2" t="n">
         <v>66219919</v>
       </c>
-      <c r="M2" t="n">
+      <c r="R2" t="n">
         <v>143411704</v>
       </c>
-      <c r="N2" t="n">
+      <c r="S2" t="n">
         <v>501305</v>
       </c>
-      <c r="O2" t="inlineStr">
+      <c r="T2" t="inlineStr">
         <is>
           <t>A24</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
+      <c r="U2" t="inlineStr">
         <is>
           <t>R</t>
         </is>
       </c>
-      <c r="Q2" t="inlineStr">
+      <c r="V2" t="inlineStr">
         <is>
           <t>Action Adventure Comedy Fantasy Sci-Fi</t>
         </is>
@@ -612,42 +650,55 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Spider-Man: Into the Spider-Verse is hailed as the best Spider-Man film, with stunning animation that viewers want to inject into their veins. It is praised for its understanding of the character of Spider-Man and its creativity. The film reinvigorates the superhero genre and is considered one of the best animated movies ever made. Fans are excited for the sequel and are in awe of the animation, action sequences, and overall quality of the film. The movie is celebrated for its unique textures, rhythms, and colors, and is considered a groundbreaking achievement in animation.</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Overall, public opinion on Spider-Man: Into the Spider-Verse seems overwhelmingly positive. Reviewers praise the film for its animation, humor, creativity, and understanding of the character of Spider-Man. Many consider it the best Spider-Man movie ever made and one of the best animated movies ever made. The film is also praised for its diverse representation and ability to reinvent the superhero genre. Some reviewers express excitement for a potential sequel and specific characters like Spider-Man Noir. Overall, the film is seen as a groundbreaking achievement in animation and storytelling.</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>best - animated - creative - understanding - funny - diverse - reinvigorates - hyper-popular - reinvent - overwhelming - achievement - expressive - textures - rhythms - colors - feminist - montage - greatest - curious - favorite - paintings</t>
-        </is>
+          <t>Spider-Man: Into the Spider-Verse is hailed as the best Spider-Man film, with stunning animation and a deep understanding of the character. The movie reinvigorates the superhero genre and is praised for its creativity and humor. Fans love the diverse cast of Spider-People and are excited for a sequel. The film is considered a groundbreaking achievement in animation and a must-watch for all audiences.</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
+        <v>9</v>
+      </c>
+      <c r="J3" t="n">
+        <v>10</v>
       </c>
       <c r="K3" t="n">
+        <v>9</v>
+      </c>
+      <c r="L3" t="n">
+        <v>9</v>
+      </c>
+      <c r="M3" t="n">
+        <v>9</v>
+      </c>
+      <c r="N3" t="n">
+        <v>10</v>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>best - animated - creative - understanding - funny - diverse - reinvigorates - hyper-popular - sequel - overwhelming - achievement - expressive - textures - rhythms - colors - feminist - montage - greatest - favorite - paintings</t>
+        </is>
+      </c>
+      <c r="P3" t="n">
         <v>190241310</v>
       </c>
-      <c r="L3" t="n">
+      <c r="Q3" t="n">
         <v>194057426</v>
       </c>
-      <c r="M3" t="n">
+      <c r="R3" t="n">
         <v>384298736</v>
       </c>
-      <c r="N3" t="n">
+      <c r="S3" t="n">
         <v>35363376</v>
       </c>
-      <c r="O3" t="inlineStr">
+      <c r="T3" t="inlineStr">
         <is>
           <t>Sony Pictures Releasing</t>
         </is>
       </c>
-      <c r="P3" t="inlineStr">
+      <c r="U3" t="inlineStr">
         <is>
           <t>PG</t>
         </is>
       </c>
-      <c r="Q3" t="inlineStr">
+      <c r="V3" t="inlineStr">
         <is>
           <t>Action Adventure Animation Comedy Family Fantasy Sci-Fi</t>
         </is>
@@ -681,42 +732,55 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Inception is a complex heist film dressed in science fiction conventions, following Dom Cobb as he tries to free himself from his past. It is a thought-provoking, layered story with sumptuous aesthetics and a brilliant cast. The film explores the idea of dreams becoming reality and leaves viewers questioning the truth until the very end. Despite some bad dialogue, it is still considered a masterpiece by many.</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>Overall, public opinion on Inception seems to be positive, with an average score of 4.64. Many reviewers praise the complex plot and impressive visuals, as well as the performances of the cast. Some viewers appreciate the deeper themes of the film, while others enjoy the action-packed heist elements. There are also comments about the relationships between characters, particularly the chemistry between Joseph Gordon-Levitt and Tom Hardy. However, there are also criticisms of the dialogue and some confusion about the ending. Overall, it seems that Inception is a divisive but generally well-received film.</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>- complex - heist - science fiction - study - man - free - past - cerebral - pop-masterpiece - thought-provoking - layered - story-telling - sumptuous - aesthetics - flawless - editing - sound design - effects - musical score - pitch-perfect - cast - confident - directorial hand - brilliant - unrivaled - filmmaking - rent free - chemistry - masterpiece - gay - lesbian solidarity - fanfic - totem - spinning - dreaming - joyous - projection - persona 5 - sexy - bad dialogue - dreams - dreams of dreams - dreams - hey now</t>
-        </is>
+          <t>Inception is a complex heist film dressed in science fiction conventions, following Dom Cobb as he tries to free himself from his past. It is a thought-provoking, layered story with sumptuous aesthetics and a brilliant cast, driven by Christopher Nolan's confident direction. The film explores the idea of dreams becoming reality and leaves viewers questioning the truth behind the spinning totem at the end. Despite some bad dialogue, it is still considered a masterpiece by many.</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
+        <v>8</v>
+      </c>
+      <c r="J4" t="n">
+        <v>9</v>
       </c>
       <c r="K4" t="n">
+        <v>8</v>
+      </c>
+      <c r="L4" t="n">
+        <v>8</v>
+      </c>
+      <c r="M4" t="n">
+        <v>9</v>
+      </c>
+      <c r="N4" t="n">
+        <v>9</v>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>- complex- heist- science fiction- study- man- free- past- cerebral- pop-masterpiece- thought-provoking- layered- story-telling- sumptuous- aesthetics- flawless- editing- sound design- effects- musical score- brilliant- unrivaled- filmmaking- rent free- chemistry- masterpiece- gay- lesbian- solidarity- fanfic- totem- spinning- dreaming- joyous- projection- persona 5- sexy- bad dialogue- dreams- inception</t>
+        </is>
+      </c>
+      <c r="P4" t="n">
         <v>292587330</v>
       </c>
-      <c r="L4" t="n">
+      <c r="Q4" t="n">
         <v>546443300</v>
       </c>
-      <c r="M4" t="n">
+      <c r="R4" t="n">
         <v>839030630</v>
       </c>
-      <c r="N4" t="n">
+      <c r="S4" t="n">
         <v>62785337</v>
       </c>
-      <c r="O4" t="inlineStr">
+      <c r="T4" t="inlineStr">
         <is>
           <t>Warner Bros.</t>
         </is>
       </c>
-      <c r="P4" t="inlineStr">
+      <c r="U4" t="inlineStr">
         <is>
           <t>PG-13</t>
         </is>
       </c>
-      <c r="Q4" t="inlineStr">
+      <c r="V4" t="inlineStr">
         <is>
           <t>Action Adventure Sci-Fi Thriller</t>
         </is>
@@ -750,42 +814,55 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Spider-Man: Across the Spider-Verse is described as an overwhelming viewing experience, with viewers refusing to take a bathroom break for fear of missing a moment. The animation, humor, soundtrack, and overall joy of the film are praised, with some viewers left speechless and in tears. The movie is hailed as a masterpiece, with stunning visuals and a surprising plot. Some find it overstuffed with stories but ultimately enjoyable. Overall, it is considered a must-see film that is visually dazzling and bursting with beauty and heart.</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>Overall, public opinion on Spider-Man: Across the Spider-Verse seems to be overwhelmingly positive. Reviewers have praised the animation, humor, soundtrack, and overall viewing experience of the film. Many have described it as a mind-blowing and visually dazzling masterpiece, with some even calling it better than the original Spider-Verse movie. Some reviewers have mentioned minor criticisms, such as the movie feeling overstuffed with too many stories, but these do not seem to detract from the overall enjoyment of the film. The general consensus is that Spider-Man: Across the Spider-Verse is a must-see movie that deserves high praise and multiple viewings.</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>- overwhelming - outstanding - joy - perfect - magical - mind-blowing - incredible - favorite - masterpiece - ambitious - beauty - heart - funny - visually dazzling - busy - funny - psychopath - unforgettable</t>
-        </is>
+          <t>Spider-Man: Across the Spider-Verse is described as an overwhelming viewing experience, with viewers unable to tear their eyes away from the screen for its entire duration. The animation, humor, soundtrack, and plot are all praised as near perfect, leaving viewers beaming with joy. Some viewers were left speechless and overstimulated after the movie, with one reviewer even considering quitting making live-action films after seeing it. Overall, the film is hailed as a masterpiece, with some viewers even calling for a 6-star rating.</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
+        <v>8</v>
+      </c>
+      <c r="J5" t="n">
+        <v>10</v>
       </c>
       <c r="K5" t="n">
+        <v>9</v>
+      </c>
+      <c r="L5" t="n">
+        <v>9</v>
+      </c>
+      <c r="M5" t="n">
+        <v>8</v>
+      </c>
+      <c r="N5" t="n">
+        <v>9</v>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>- overwhelming - outstanding - joy - perfect - magical - mind-blowing - incredible - favorite - fried - masterpiece - ambitious - beauty - heart - funny - visually dazzling - busy - funny - psychopath - unforgettable</t>
+        </is>
+      </c>
+      <c r="P5" t="n">
         <v>381593754</v>
       </c>
-      <c r="L5" t="n">
+      <c r="Q5" t="n">
         <v>309304156</v>
       </c>
-      <c r="M5" t="n">
+      <c r="R5" t="n">
         <v>690897910</v>
       </c>
-      <c r="N5" t="n">
+      <c r="S5" t="n">
         <v>120663589</v>
       </c>
-      <c r="O5" t="inlineStr">
+      <c r="T5" t="inlineStr">
         <is>
           <t>Columbia Pictures</t>
         </is>
       </c>
-      <c r="P5" t="inlineStr">
+      <c r="U5" t="inlineStr">
         <is>
           <t>PG</t>
         </is>
       </c>
-      <c r="Q5" t="inlineStr">
+      <c r="V5" t="inlineStr">
         <is>
           <t>Action Adventure Animation Fantasy Sci-Fi</t>
         </is>
@@ -819,42 +896,55 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Spider-Man: No Way Home brings back Willem Dafoe's iconic Green Goblin and delivers emotional moments that had audiences in tears. The film is praised for its ambitious storytelling and the surprise appearances of past Spider-Man actors. However, some viewers found the CGI and abundance of villains to be overwhelming. Overall, the film is seen as a thrilling and nostalgic experience for fans of the franchise.</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>Based on the reviews, it seems that public opinion on Spider-Man: No Way Home is generally positive. Many people were thrilled by the return of Willem Dafoe's Green Goblin and the appearances of Tobey Maguire and Andrew Garfield as other versions of Spider-Man. The emotional moments in the film resonated with audiences, and there were high levels of excitement and engagement in theaters during key scenes. However, some viewers found the film to be a bit messy with too many villains and CGI, and there were mixed feelings about the overall execution of the story. Overall, it appears that the film was a highly anticipated and enjoyable experience for many fans of the Spider-Man franchise.</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>- ambitious - emotional - messy - CGI - iconic - sinister - nostalgic - thrilling - ambitious - surprising - intense - action-packed - comedic - overwhelming - conflicted - tender - unexpected - hooting - hollering - apeshit</t>
-        </is>
+          <t>Spider-Man: No Way Home brings back Willem Dafoe's iconic Green Goblin and delivers emotional moments with Andrew Garfield's Spider-Man. The film is praised for its ambitious storytelling and nostalgic callbacks, but some criticize the excessive CGI and pacing issues. Overall, it is considered a thrilling and emotional experience for fans of the franchise.</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
+        <v>7</v>
+      </c>
+      <c r="J6" t="n">
+        <v>8</v>
       </c>
       <c r="K6" t="n">
+        <v>9</v>
+      </c>
+      <c r="L6" t="n">
+        <v>8</v>
+      </c>
+      <c r="M6" t="n">
+        <v>6</v>
+      </c>
+      <c r="N6" t="n">
+        <v>5</v>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>- ambitious - emotional - messy - CGI - iconic - sinister - nostalgic - thrilling - surprising - ambitious - action-packed - comedic - intense - unexpected - fan-favorite - epic - tear-jerking - heartwarming - chaotic - conflicted - childhood memories - cameo - applause</t>
+        </is>
+      </c>
+      <c r="P6" t="n">
         <v>814866759</v>
       </c>
-      <c r="L6" t="n">
+      <c r="Q6" t="n">
         <v>1107732041</v>
       </c>
-      <c r="M6" t="n">
+      <c r="R6" t="n">
         <v>1922598800</v>
       </c>
-      <c r="N6" t="n">
+      <c r="S6" t="n">
         <v>260138569</v>
       </c>
-      <c r="O6" t="inlineStr">
+      <c r="T6" t="inlineStr">
         <is>
           <t>Sony Pictures Releasing</t>
         </is>
       </c>
-      <c r="P6" t="inlineStr">
+      <c r="U6" t="inlineStr">
         <is>
           <t>PG-13</t>
         </is>
       </c>
-      <c r="Q6" t="inlineStr">
+      <c r="V6" t="inlineStr">
         <is>
           <t>Action Adventure Fantasy Sci-Fi</t>
         </is>

</xml_diff>

<commit_message>
nome filme nas tabelas e correções nas tabelas
</commit_message>
<xml_diff>
--- a/letterboxd_scraping/movie_info.xlsx
+++ b/letterboxd_scraping/movie_info.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V6"/>
+  <dimension ref="A1:V21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -536,7 +536,7 @@
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>Genres</t>
+          <t>Genre</t>
         </is>
       </c>
     </row>
@@ -546,79 +546,79 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Everything Everywhere All at Once</t>
+          <t>Spider-Man: Into the Spider-Verse</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>2022</v>
+        <v>2018</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Daniel Scheinert</t>
+          <t>Rodney Rothman</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>140</v>
+        <v>117</v>
       </c>
       <c r="F2" t="n">
-        <v>4.58</v>
+        <v>4.74</v>
       </c>
       <c r="G2" t="n">
-        <v>0.67</v>
+        <v>0.38</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>"Everything Everywhere All at Once" is a visually stunning and emotionally resonant film that explores themes of multiverses, family dynamics, and the significance of every choice we make. With a mix of humor, action, and heartfelt moments, this movie has left a lasting impact on viewers, making it a must-watch for audiences of all ages. The film has been praised for its originality, technical brilliance, and powerful storytelling, making it a standout in the world of cinema.</t>
+          <t>Spider-Man: Into the Spider-Verse is hailed as the best Spider-Man film ever made, with stunning animation that is likened to a drug-like experience. The movie is praised for its creativity, humor, and understanding of the character of Spider-Man. Fans appreciate the diverse representation of different Spider-People and the bold reinvention of the superhero genre. The film's visuals, soundtrack, and voice cast are all highly praised, with particular love for Spider-Man Noir and the iconic Leap of Faith scene. Overall, Into the Spider-Verse is considered a groundbreaking and masterful achievement in animation and comic book storytelling.</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J2" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="K2" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L2" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="M2" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="N2" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>- audacious - funny - original - technically dazzling - thematically resonant - genetically engineered - greatest multiverse movie - required viewing - everything matters - overwhelming - in love - homage - emotional core - chaotic balance - intelligent filmmaking - lowbrow humor - hot right now - competing realities - haunting - mommy issues - nihilist lesbian representation - pride month</t>
+          <t>- best spider-man film - funny - creative - wonderfully animated - understanding of the character - amazing animation - best spider-man movie - lgbt representation - talented people - reinvigorates the genre - hyper-popular spandex myths - spider-man noir - best animated movies ever made - colors - action sequences - Nic Cage - john mulaney - spider-ham - spider-man noir movie - flawless movies - leap of faith scene - perfect casting - incredible visuals - best soundtrack - spider-man origin story - reinvent the character - anyone can wear the mask - visual orgasm - dazzling animation - formal risk - superheroes resurgence - peak cinema - consumed by the spider-verse.</t>
         </is>
       </c>
       <c r="P2" t="n">
-        <v>77191785</v>
+        <v>190241310</v>
       </c>
       <c r="Q2" t="n">
-        <v>66219919</v>
+        <v>194057426</v>
       </c>
       <c r="R2" t="n">
-        <v>143411704</v>
+        <v>384298736</v>
       </c>
       <c r="S2" t="n">
-        <v>501305</v>
+        <v>35363376</v>
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>A24</t>
+          <t>Sony Pictures Releasing</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>PG</t>
         </is>
       </c>
       <c r="V2" t="inlineStr">
         <is>
-          <t>Action Adventure Comedy Fantasy Sci-Fi</t>
+          <t>animation</t>
         </is>
       </c>
     </row>
@@ -628,33 +628,33 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Spider-Man: Into the Spider-Verse</t>
+          <t>Spider-Man: Across the Spider-Verse</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>2018</v>
+        <v>2023</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Rodney Rothman</t>
+          <t>Joaquim Dos Santos</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="F3" t="n">
-        <v>4.67</v>
+        <v>4.54</v>
       </c>
       <c r="G3" t="n">
-        <v>0.39</v>
+        <v>0.58</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Spider-Man: Into the Spider-Verse is hailed as the best Spider-Man film, with stunning animation and a deep understanding of the character. The movie reinvigorates the superhero genre and is praised for its creativity and humor. Fans love the diverse cast of Spider-People and are excited for a sequel. The film is considered a groundbreaking achievement in animation and a must-watch for all audiences.</t>
+          <t>Spider-Man: Across the Spider-Verse is described as an overwhelming viewing experience, with stunning animation, humor, and a fantastic soundtrack. Viewers were left speechless and in awe of the visuals and storytelling, with some even crying during certain scenes. The film is praised for its creativity, heart, and balance of references without overwhelming the story. Some viewers found it to be a masterpiece and one of the best Marvel movies to date, while others felt it was overstuffed with multiple storylines. Overall, it is seen as a visually stunning and ambitious sequel that lives up to the original.</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J3" t="n">
         <v>10</v>
@@ -666,31 +666,31 @@
         <v>9</v>
       </c>
       <c r="M3" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="N3" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>best - animated - creative - understanding - funny - diverse - reinvigorates - hyper-popular - sequel - overwhelming - achievement - expressive - textures - rhythms - colors - feminist - montage - greatest - favorite - paintings</t>
+          <t>- overwhelming - outstanding - joy - perfect - magical - incredible - surprising - mind-blowing - balance - beauty - heart - ambitious - dazzling - breathtaking - spectacular - imaginative - complete - concentrated - rich - sensational - jaw-dropping - heartfelt - thought-provoking - masterpiece - creative - life - astonishing - expressive - visual feast - ambitious - foreshadowing - perfection - unpopular - style - substance - fan service - quipy</t>
         </is>
       </c>
       <c r="P3" t="n">
-        <v>190241310</v>
+        <v>381593754</v>
       </c>
       <c r="Q3" t="n">
-        <v>194057426</v>
+        <v>309304156</v>
       </c>
       <c r="R3" t="n">
-        <v>384298736</v>
+        <v>690897910</v>
       </c>
       <c r="S3" t="n">
-        <v>35363376</v>
+        <v>120663589</v>
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>Sony Pictures Releasing</t>
+          <t>Columbia Pictures</t>
         </is>
       </c>
       <c r="U3" t="inlineStr">
@@ -700,7 +700,7 @@
       </c>
       <c r="V3" t="inlineStr">
         <is>
-          <t>Action Adventure Animation Comedy Family Fantasy Sci-Fi</t>
+          <t>animation</t>
         </is>
       </c>
     </row>
@@ -710,79 +710,79 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Inception</t>
+          <t>Spirited Away</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>2010</v>
+        <v>2001</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Christopher Nolan</t>
+          <t>Hayao Miyazaki</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>148</v>
+        <v>125</v>
       </c>
       <c r="F4" t="n">
-        <v>4.64</v>
+        <v>4.73</v>
       </c>
       <c r="G4" t="n">
-        <v>0.45</v>
+        <v>0.53</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Inception is a complex heist film dressed in science fiction conventions, following Dom Cobb as he tries to free himself from his past. It is a thought-provoking, layered story with sumptuous aesthetics and a brilliant cast, driven by Christopher Nolan's confident direction. The film explores the idea of dreams becoming reality and leaves viewers questioning the truth behind the spinning totem at the end. Despite some bad dialogue, it is still considered a masterpiece by many.</t>
+          <t>Spirited Away is a visually stunning and emotionally resonant masterpiece that follows the journey of a young girl named Chihiro as she navigates a fantastical world filled with gods, witches, and spirits. The film explores themes of courage, growth, and the power of love, all while immersing the audience in a richly imaginative and magical universe. With its captivating animation, memorable characters, and heartfelt storytelling, Spirited Away has been hailed as one of the greatest animated films of all time, leaving viewers in awe of its beauty and depth.</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J4" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K4" t="n">
         <v>8</v>
       </c>
       <c r="L4" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M4" t="n">
         <v>9</v>
       </c>
       <c r="N4" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>- complex- heist- science fiction- study- man- free- past- cerebral- pop-masterpiece- thought-provoking- layered- story-telling- sumptuous- aesthetics- flawless- editing- sound design- effects- musical score- brilliant- unrivaled- filmmaking- rent free- chemistry- masterpiece- gay- lesbian- solidarity- fanfic- totem- spinning- dreaming- joyous- projection- persona 5- sexy- bad dialogue- dreams- inception</t>
+          <t>- immersive - transformative - emotional - visually stunning - imaginative - magical - heartwarming - coming-of-age - enchanting - captivating - whimsical - fantastical - breathtaking - thought-provoking - beautiful - charming - nostalgic - profound - inspiring - mesmerizing - allegorical - touching - unique - masterful - iconic - timeless - symbolic - introspective - whimsy - evocative - resonant - powerful - enchantment - allegory - fantastical - dreamlike - mesmerizing - captivating - heartwarming - transformative - immersive - emotional - visually stunning - imaginative - magical - enchanting - charming - whimsical - profound - inspiring - allegorical - touching - unique - masterful - iconic - timeless - symbolic - introspective - reson</t>
         </is>
       </c>
       <c r="P4" t="n">
-        <v>292587330</v>
+        <v>15205725</v>
       </c>
       <c r="Q4" t="n">
-        <v>546443300</v>
+        <v>342082125</v>
       </c>
       <c r="R4" t="n">
-        <v>839030630</v>
+        <v>357561772</v>
       </c>
       <c r="S4" t="n">
-        <v>62785337</v>
+        <v>449839</v>
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>Warner Bros.</t>
+          <t>Walt Disney Studios Motion Pictures</t>
         </is>
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t>PG-13</t>
+          <t>PG</t>
         </is>
       </c>
       <c r="V4" t="inlineStr">
         <is>
-          <t>Action Adventure Sci-Fi Thriller</t>
+          <t>animation</t>
         </is>
       </c>
     </row>
@@ -792,42 +792,42 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Spider-Man: Across the Spider-Verse</t>
+          <t>Ratatouille</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>2023</v>
+        <v>2007</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Joaquim Dos Santos</t>
+          <t>Brad Bird</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>140</v>
+        <v>111</v>
       </c>
       <c r="F5" t="n">
-        <v>4.75</v>
+        <v>4.77</v>
       </c>
       <c r="G5" t="n">
-        <v>0.43</v>
+        <v>0.39</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Spider-Man: Across the Spider-Verse is described as an overwhelming viewing experience, with viewers unable to tear their eyes away from the screen for its entire duration. The animation, humor, soundtrack, and plot are all praised as near perfect, leaving viewers beaming with joy. Some viewers were left speechless and overstimulated after the movie, with one reviewer even considering quitting making live-action films after seeing it. Overall, the film is hailed as a masterpiece, with some viewers even calling for a 6-star rating.</t>
+          <t>Ratatouille is a beloved Pixar film that follows the story of a rat named Remy who dreams of becoming a chef. The film explores themes of identity, poverty, and the power of food to bring people together. With its charming characters and heartwarming story, Ratatouille has become a favorite among fans and is considered by many to be one of Pixar's best films.</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J5" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="K5" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L5" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="M5" t="n">
         <v>8</v>
@@ -837,34 +837,53 @@
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>- overwhelming - outstanding - joy - perfect - magical - mind-blowing - incredible - favorite - fried - masterpiece - ambitious - beauty - heart - funny - visually dazzling - busy - funny - psychopath - unforgettable</t>
+          <t>- culinary masterpiece
+- heartwarming
+- inspirational
+- visually stunning
+- emotional
+- comedic
+- thought-provoking
+- charming
+- iconic
+- timeless
+- imaginative
+- endearing
+- captivating
+- feel-good
+- whimsical
+- creative
+- engaging
+- delightful
+- heartening
+- profound</t>
         </is>
       </c>
       <c r="P5" t="n">
-        <v>381593754</v>
+        <v>206445654</v>
       </c>
       <c r="Q5" t="n">
-        <v>309304156</v>
+        <v>417280431</v>
       </c>
       <c r="R5" t="n">
-        <v>690897910</v>
+        <v>623728318</v>
       </c>
       <c r="S5" t="n">
-        <v>120663589</v>
+        <v>47027395</v>
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>Columbia Pictures</t>
+          <t>Walt Disney Studios Motion Pictures</t>
         </is>
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>PG</t>
+          <t>G</t>
         </is>
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>Action Adventure Animation Fantasy Sci-Fi</t>
+          <t>animation</t>
         </is>
       </c>
     </row>
@@ -874,79 +893,1309 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Spider-Man: No Way Home</t>
+          <t>Fantastic Mr. Fox</t>
         </is>
       </c>
       <c r="C6" t="n">
+        <v>2009</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Wes Anderson</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>87</v>
+      </c>
+      <c r="F6" t="n">
+        <v>4.75</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Fantastic Mr. Fox is a stop-motion puppet animation film directed by Wes Anderson that follows the story of Mr. Fox, voiced by George Clooney, as he assembles a team for elaborate heists. The film features a diverse group of characters, including Willem Dafoe as the evil rat Willem Da Rat. The movie is praised for its unique visuals, quirky humor, and charming characters. It is considered a standout film in Wes Anderson's filmography and a beloved favorite among fans.</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
+        <v>9</v>
+      </c>
+      <c r="J6" t="n">
+        <v>8</v>
+      </c>
+      <c r="K6" t="n">
+        <v>10</v>
+      </c>
+      <c r="L6" t="n">
+        <v>7</v>
+      </c>
+      <c r="M6" t="n">
+        <v>8</v>
+      </c>
+      <c r="N6" t="n">
+        <v>9</v>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>- quirky - charming - unique - heist - stop-motion - animation - humor - family - love - dysfunctional - furry - music - visuals - commentary - childhood - comedy - heartwarming - pure - personal - mirror - delightful - underrated - achievement - human - Baumbach - writing</t>
+        </is>
+      </c>
+      <c r="P6" t="n">
+        <v>21002919</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>37084340</v>
+      </c>
+      <c r="R6" t="n">
+        <v>58091759</v>
+      </c>
+      <c r="S6" t="n">
+        <v>265900</v>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>Twentieth Century Fox</t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>PG</t>
+        </is>
+      </c>
+      <c r="V6" t="inlineStr">
+        <is>
+          <t>animation</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Inglourious Basterds</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>2009</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Quentin Tarantino</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>153</v>
+      </c>
+      <c r="F7" t="n">
+        <v>4.86</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Inglourious Basterds is a film that follows a group of Jewish-American soldiers on a mission to kill Nazis during World War II. The movie is praised for its sharp dialogue, intense scenes, and standout performances, particularly by Christoph Waltz. The film is seen as a masterpiece by many, with memorable moments and iconic lines that have left a lasting impact on viewers. It is a mix of revenge, action, comedy, and drama, all wrapped up in Quentin Tarantino's signature style.</t>
+        </is>
+      </c>
+      <c r="I7" t="n">
+        <v>9</v>
+      </c>
+      <c r="J7" t="n">
+        <v>7</v>
+      </c>
+      <c r="K7" t="n">
+        <v>8</v>
+      </c>
+      <c r="L7" t="n">
+        <v>8</v>
+      </c>
+      <c r="M7" t="n">
+        <v>9</v>
+      </c>
+      <c r="N7" t="n">
+        <v>10</v>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>- revenge - historical - comedic - intense - multilingual - iconic - masterpiece - memorable - brutal - powerful - captivating - breathtaking - heroism - vengeance - dialogue - character-driven - authentic - stylized - exploitation - gleeful - mournful - fetishistic - heroic - bloodshed - moral reckoning - scalp - perfection - sharp - ferocious - merciless - climax - excellent - fire - humanity - intersecting - cinema - mother</t>
+        </is>
+      </c>
+      <c r="P7" t="n">
+        <v>120540719</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>200917028</v>
+      </c>
+      <c r="R7" t="n">
+        <v>321458605</v>
+      </c>
+      <c r="S7" t="n">
+        <v>38054676</v>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>The Weinstein Company</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t>war</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Jojo Rabbit</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>2019</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Taika Waititi</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>108</v>
+      </c>
+      <c r="F8" t="n">
+        <v>3.35</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1.38</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Jojo Rabbit is a film that blends comedy and drama in a unique way, tackling the heavy subject matter of Nazi Germany through the eyes of a young boy who idolizes Hitler. Directed by Taika Waititi, the film has been praised for its unexpected emotional depth and the way it balances humor with more serious themes. With standout performances from the cast, including Sam Rockwell as a gay Nazi, Jojo Rabbit has been described as a breath of fresh air and a film that only Waititi could have pulled off. Despite some criticisms about its tonal shifts, the film has been lauded for its unique take on a difficult topic.</t>
+        </is>
+      </c>
+      <c r="I8" t="n">
+        <v>9</v>
+      </c>
+      <c r="J8" t="n">
+        <v>7</v>
+      </c>
+      <c r="K8" t="n">
+        <v>8</v>
+      </c>
+      <c r="L8" t="n">
+        <v>6</v>
+      </c>
+      <c r="M8" t="n">
+        <v>8</v>
+      </c>
+      <c r="N8" t="n">
+        <v>9</v>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>- satirical - heartwarming - unexpected - passionate - funny - emotional - transformative - whimsical - unique - thought-provoking - bold - comedic - touching - powerful - controversial - brilliant - clever - charming - satirical - absurd - genius - hilarious - poignant - entertaining - dark - surprising - impressive - refreshing - innovative - daring - irreverent - witty - engaging - impactful - controversial - insightful - balanced - silly - unfunny - repulsive - cutesy - star-studded - offensive - amazing</t>
+        </is>
+      </c>
+      <c r="P8" t="n">
+        <v>33370906</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>60323801</v>
+      </c>
+      <c r="R8" t="n">
+        <v>93694707</v>
+      </c>
+      <c r="S8" t="n">
+        <v>349555</v>
+      </c>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>Fox Searchlight</t>
+        </is>
+      </c>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>PG-13</t>
+        </is>
+      </c>
+      <c r="V8" t="inlineStr">
+        <is>
+          <t>war</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>1917</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>2019</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Sam Mendes</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>119</v>
+      </c>
+      <c r="F9" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>1917 is a visually stunning and immersive war film that follows two soldiers on a perilous mission during World War I. Directed by Sam Mendes, the film utilizes long takes to give the impression of being one continuous shot, creating a powerful and relentless look into the harsh realities and conditions soldiers faced during the war. While some viewers found the film lacking in depth in terms of story and character development, the technical achievements, gripping suspense, and impressive cinematography by Roger Deakins make it a worthwhile watch for those seeking a visceral cinematic experience.</t>
+        </is>
+      </c>
+      <c r="I9" t="n">
+        <v>7</v>
+      </c>
+      <c r="J9" t="n">
+        <v>8</v>
+      </c>
+      <c r="K9" t="n">
+        <v>8</v>
+      </c>
+      <c r="L9" t="n">
+        <v>7</v>
+      </c>
+      <c r="M9" t="n">
+        <v>7</v>
+      </c>
+      <c r="N9" t="n">
+        <v>9</v>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>- immersive - visceral - gripping - powerful - visually stunning - emotionally harrowing - memorable - impressive - tense - natural performances - grounded - terrifying - impressive blocking - exceptional camerawork - exceptional set design - polished - breathtaking - beautiful - masterclass - tactility - earthy texture - surreal - haunted chaos - meticulous - extraordinary feat - harmonising shots - absorbing - surreal spaces - monotonous - well-oiled machinery - grotesque textures - nihilistic - traumatizing - harrowing - relentless - brutal - outstanding - heroism - friendship - technical marvel - brilliant - relentless - suspenseful - propulsive - adventure - gimmick - immersive - stark - immediate - breathtaking - atemberaubend - claustrophobic - stunning - earthy -</t>
+        </is>
+      </c>
+      <c r="P9" t="n">
+        <v>159227644</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>231183781</v>
+      </c>
+      <c r="R9" t="n">
+        <v>390411425</v>
+      </c>
+      <c r="S9" t="n">
+        <v>576216</v>
+      </c>
+      <c r="T9" t="inlineStr">
+        <is>
+          <t>Universal Pictures</t>
+        </is>
+      </c>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="V9" t="inlineStr">
+        <is>
+          <t>war</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Dunkirk</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>2017</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Christopher Nolan</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>107</v>
+      </c>
+      <c r="F10" t="n">
+        <v>4.15</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Dunkirk is a war film directed by Christopher Nolan that depicts the Dunkirk evacuation of World War II. The movie follows the intense and stressful experiences of Allied troops stranded on the beaches of Dunkirk, with a focus on survival and sacrifice. The film features a talented cast including Tom Hardy, Fionn Whitehead, Harry Styles, and Cillian Murphy. The immersive experience is heightened by Hans Zimmer's intense score. Overall, Dunkirk is praised for its technical achievements and emotional impact, with some viewers finding it to be a masterpiece while others appreciate its unique approach to storytelling.</t>
+        </is>
+      </c>
+      <c r="I10" t="n">
+        <v>8</v>
+      </c>
+      <c r="J10" t="n">
+        <v>9</v>
+      </c>
+      <c r="K10" t="n">
+        <v>7</v>
+      </c>
+      <c r="L10" t="n">
+        <v>8</v>
+      </c>
+      <c r="M10" t="n">
+        <v>8</v>
+      </c>
+      <c r="N10" t="n">
+        <v>9</v>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>- tension - stress-inducing - harry styles - dark-haired british twinks - horror - adrenaline rush - war movie - masterpiece - color grade - british mumbling - emotional wreck - ticking - survival - bare essentials - steel - fire - bodies - sacrifice - genius - hans zimmer - atmospheric - thrilling - scale - victory - boats - clean - twinks - survival - endure - aushalten - technical bravado</t>
+        </is>
+      </c>
+      <c r="P10" t="n">
+        <v>189740665</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>340639465</v>
+      </c>
+      <c r="R10" t="n">
+        <v>530432122</v>
+      </c>
+      <c r="S10" t="n">
+        <v>50513488</v>
+      </c>
+      <c r="T10" t="inlineStr">
+        <is>
+          <t>Warner Bros.</t>
+        </is>
+      </c>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>PG-13</t>
+        </is>
+      </c>
+      <c r="V10" t="inlineStr">
+        <is>
+          <t>war</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Schindler's List</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>1993</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Steven Spielberg</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>195</v>
+      </c>
+      <c r="F11" t="n">
+        <v>4.46</v>
+      </c>
+      <c r="G11" t="n">
+        <v>1.06</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Schindler's List is a powerful and haunting film that delves into the atrocities of the Holocaust. Steven Spielberg's masterpiece is a testament to hope and perseverance in the face of darkness, showcasing the unlikely heroism of Oskar Schindler. The film is beautifully crafted, with moving performances and stunning art direction. It is a must-watch for everyone, offering a glimpse into the horrors and atrocities committed against the Jews in Europe during World War II.</t>
+        </is>
+      </c>
+      <c r="I11" t="n">
+        <v>9</v>
+      </c>
+      <c r="J11" t="n">
+        <v>7</v>
+      </c>
+      <c r="K11" t="n">
+        <v>10</v>
+      </c>
+      <c r="L11" t="n">
+        <v>8</v>
+      </c>
+      <c r="M11" t="n">
+        <v>9</v>
+      </c>
+      <c r="N11" t="n">
+        <v>10</v>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>- haunting - devastating - masterpiece - emotional - powerful - iconic - moving - essential - profound - gut-wrenching - intense - important - respectful - perfect - beautiful - inspiring - tragic - humanity - symbolism - cinematic - somber - ethical - potent - passionate - terrific - monumental - transformative - bloody - genocide - impactful - unforgettable</t>
+        </is>
+      </c>
+      <c r="P11" t="n">
+        <v>96898818</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>225262427</v>
+      </c>
+      <c r="R11" t="n">
+        <v>322161245</v>
+      </c>
+      <c r="S11" t="n">
+        <v>656636</v>
+      </c>
+      <c r="T11" t="inlineStr">
+        <is>
+          <t>Universal Pictures</t>
+        </is>
+      </c>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="V11" t="inlineStr">
+        <is>
+          <t>war</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Everything Everywhere All at Once</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>2022</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Daniel Scheinert</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>140</v>
+      </c>
+      <c r="F12" t="n">
+        <v>4.15</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1.22</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>"Everything Everywhere All at Once" is a visually dazzling and emotionally resonant film that explores themes of family, identity, and the significance of our lives in the vast multiverse. With a mix of humor, action, and heartfelt moments, the movie has left audiences in awe and tears, with some calling it a revolutionary masterpiece and others finding it exhausting or lacking in emotional depth. Featuring standout performances and ambitious storytelling, this film has sparked a range of reactions from viewers, making it a must-watch for those seeking a unique cinematic experience.</t>
+        </is>
+      </c>
+      <c r="I12" t="n">
+        <v>9</v>
+      </c>
+      <c r="J12" t="n">
+        <v>8</v>
+      </c>
+      <c r="K12" t="n">
+        <v>9</v>
+      </c>
+      <c r="L12" t="n">
+        <v>8</v>
+      </c>
+      <c r="M12" t="n">
+        <v>8</v>
+      </c>
+      <c r="N12" t="n">
+        <v>9</v>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>- visionary - masterpiece - chaotic - emotional - hilarious - poignant - multiverse - existential - family drama - creative - kinetic - daring - expertly choreographed - genuine emotional core - intelligent filmmaking - lowbrow humor - visually dynamic - ambitious - beautifully filmed - edited - perfect music - endlessly creative - everything - revolutionary - sentimental - existential questions - heartfelt - compassionate - cosmic gumbo - exhausting - reprehensible - tired narrative - massive visuals - engaging - awakening excitement</t>
+        </is>
+      </c>
+      <c r="P12" t="n">
+        <v>77191785</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>66219919</v>
+      </c>
+      <c r="R12" t="n">
+        <v>143411704</v>
+      </c>
+      <c r="S12" t="n">
+        <v>501305</v>
+      </c>
+      <c r="T12" t="inlineStr">
+        <is>
+          <t>A24</t>
+        </is>
+      </c>
+      <c r="U12" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="V12" t="inlineStr">
+        <is>
+          <t>science-fiction</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Interstellar</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>2014</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Christopher Nolan</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>169</v>
+      </c>
+      <c r="F13" t="n">
+        <v>4.52</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Interstellar is a visually stunning and emotionally heavy film that explores themes of love, loss, and the human connection. Directed by Christopher Nolan, the movie follows a father's journey through space and time to save humanity, while also delving into the complexities of family relationships. With breathtaking visuals, a powerful score, and standout performances, Interstellar has left audiences both in awe and in tears, making it a memorable and thought-provoking cinematic experience.</t>
+        </is>
+      </c>
+      <c r="I13" t="n">
+        <v>7</v>
+      </c>
+      <c r="J13" t="n">
+        <v>9</v>
+      </c>
+      <c r="K13" t="n">
+        <v>8</v>
+      </c>
+      <c r="L13" t="n">
+        <v>8</v>
+      </c>
+      <c r="M13" t="n">
+        <v>7</v>
+      </c>
+      <c r="N13" t="n">
+        <v>9</v>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>- emotional - powerful - cathartic - heartbreaking - ambitious - stunning - breathtaking - intense - profound - thought-provoking - epic - mesmerizing - captivating - awe-inspiring - beautiful - complex - flawed - over-explained - nonsensical - inspiring - masterpiece - journey - devastating - ambitious - technical - visionary - extraordinary - bold - cold precision - existential - emotional - frail - robot - algorithmically - process - value - human - frail - emotional - beings - jaw-dropping - spiritual - experience - boring - overwritten - flawed - insulting - powerful - terrifying - creepy - impeccable - inspiring - breathtaking - spectacular - obsessed - explorers - loss - trauma - mistake</t>
+        </is>
+      </c>
+      <c r="P13" t="n">
+        <v>188020017</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>517171225</v>
+      </c>
+      <c r="R13" t="n">
+        <v>705191242</v>
+      </c>
+      <c r="S13" t="n">
+        <v>47510360</v>
+      </c>
+      <c r="T13" t="inlineStr">
+        <is>
+          <t>Paramount Pictures</t>
+        </is>
+      </c>
+      <c r="U13" t="inlineStr">
+        <is>
+          <t>PG-13</t>
+        </is>
+      </c>
+      <c r="V13" t="inlineStr">
+        <is>
+          <t>science-fiction</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Dune</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
         <v>2021</v>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Jon Watts</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Denis Villeneuve</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>155</v>
+      </c>
+      <c r="F14" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Dune is a visually stunning film that immerses viewers in a vast and detailed universe. The story follows Paul, a chosen one with undiscovered powers destined to unite civilizations in the far reaches of the universe. The film features impressive world-building and industrial design, with a focus on methodical storytelling rather than action-packed sequences. However, some viewers found the film to be overly long and lacking in emotional depth. Overall, Dune is a monumental cinematic achievement that faithfully adapts Frank Herbert's novel.</t>
+        </is>
+      </c>
+      <c r="I14" t="n">
+        <v>7</v>
+      </c>
+      <c r="J14" t="n">
+        <v>9</v>
+      </c>
+      <c r="K14" t="n">
+        <v>8</v>
+      </c>
+      <c r="L14" t="n">
+        <v>8</v>
+      </c>
+      <c r="M14" t="n">
+        <v>7</v>
+      </c>
+      <c r="N14" t="n">
+        <v>9</v>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>- epic - visually stunning - immersive - detailed worldbuilding - methodical - slow-paced - captivating - mesmerizing - intense - grandiose - epic scale - faithful adaptation - sci-fi - dystopian - complex characters - intricate plot - emotional - powerful performances - epic soundtrack - epic visuals - sandworms - intergalactic - coming-of-age - epic journey - epic storytelling - epic cinematography - epic direction - epic production design - epic costumes - epic special effects - epic action - epic drama - epic adventure - epic fantasy - epic sci-fi - epic spectacle - epic experience - epic scale - epic scope - epic ambition - epic execution - epic achievement - epic filmmaking - epic saga - epic mythology - epic world-building - epic narrative - epic characters</t>
+        </is>
+      </c>
+      <c r="P14" t="n">
+        <v>108897830</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>298675798</v>
+      </c>
+      <c r="R14" t="n">
+        <v>407573628</v>
+      </c>
+      <c r="S14" t="n">
+        <v>41011174</v>
+      </c>
+      <c r="T14" t="inlineStr">
+        <is>
+          <t>Warner Bros.</t>
+        </is>
+      </c>
+      <c r="U14" t="inlineStr">
+        <is>
+          <t>PG-13</t>
+        </is>
+      </c>
+      <c r="V14" t="inlineStr">
+        <is>
+          <t>science-fiction</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Spider-Man: Into the Spider-Verse</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>2018</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Rodney Rothman</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>117</v>
+      </c>
+      <c r="F15" t="n">
+        <v>4.74</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Spider-Man: Into the Spider-Verse is hailed as the best Spider-Man film ever made, with stunning animation that is likened to a drug-like experience. The movie is praised for its creativity, humor, and understanding of the character of Spider-Man. Fans appreciate the diverse representation of different Spider-People and the bold reinvention of the superhero genre. The film's visuals, soundtrack, and storytelling are all highly praised, with many viewers expressing their love for the movie and its impact on them. The movie is seen as a groundbreaking achievement in animation and a must-watch for fans of Spider-Man and comic book movies in general.</t>
+        </is>
+      </c>
+      <c r="I15" t="n">
+        <v>10</v>
+      </c>
+      <c r="J15" t="n">
+        <v>10</v>
+      </c>
+      <c r="K15" t="n">
+        <v>10</v>
+      </c>
+      <c r="L15" t="n">
+        <v>10</v>
+      </c>
+      <c r="M15" t="n">
+        <v>10</v>
+      </c>
+      <c r="N15" t="n">
+        <v>10</v>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>- best spider-man film - funny - creative - wonderfully animated - understanding of the character - amazing animation - best spider-man movie - lgbt representation - talented people - reinvigorates the genre - spider-man noir - best animated movies ever made - colors - action sequences - Nic Cage - john mulaney - spider-ham - spider-man noir movie - flawless movies - leap of faith scene - perfect casting - incredible visuals - best soundtrack - spider-man: into the spider-verse 2 - all new spiderman - highly unique - imaginative - every superhero film should be animated - what's up danger scene - marvel origin stories - reinvent the character - leap of faith - anyone can wear the mask - exemplary screenplay - visual orgasm - dazzling animation</t>
+        </is>
+      </c>
+      <c r="P15" t="n">
+        <v>190241310</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>194057426</v>
+      </c>
+      <c r="R15" t="n">
+        <v>384298736</v>
+      </c>
+      <c r="S15" t="n">
+        <v>35363376</v>
+      </c>
+      <c r="T15" t="inlineStr">
+        <is>
+          <t>Sony Pictures Releasing</t>
+        </is>
+      </c>
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>PG</t>
+        </is>
+      </c>
+      <c r="V15" t="inlineStr">
+        <is>
+          <t>science-fiction</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Inception</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>2010</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Christopher Nolan</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
         <v>148</v>
       </c>
-      <c r="F6" t="n">
-        <v>3.42</v>
-      </c>
-      <c r="G6" t="n">
-        <v>1.08</v>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>Spider-Man: No Way Home brings back Willem Dafoe's iconic Green Goblin and delivers emotional moments with Andrew Garfield's Spider-Man. The film is praised for its ambitious storytelling and nostalgic callbacks, but some criticize the excessive CGI and pacing issues. Overall, it is considered a thrilling and emotional experience for fans of the franchise.</t>
-        </is>
-      </c>
-      <c r="I6" t="n">
+      <c r="F16" t="n">
+        <v>4.55</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Inception is a complex heist film dressed in science fiction conventions, following the story of Dom Cobb as he navigates dreams within dreams. With a pitch-perfect cast and brilliant direction from Christopher Nolan, the film is a cerebral pop-masterpiece that explores themes of catharsis and the value of fabricated realities. The movie's intricate plot and stunning visuals, paired with Hans Zimmer's iconic score, make it a captivating and thought-provoking experience. Despite some criticisms of the dialogue and pacing, Inception remains a standout piece of filmmaking that continues to spark discussions and interpretations among viewers.</t>
+        </is>
+      </c>
+      <c r="I16" t="n">
+        <v>8</v>
+      </c>
+      <c r="J16" t="n">
+        <v>9</v>
+      </c>
+      <c r="K16" t="n">
         <v>7</v>
       </c>
-      <c r="J6" t="n">
-        <v>8</v>
-      </c>
-      <c r="K6" t="n">
-        <v>9</v>
-      </c>
-      <c r="L6" t="n">
-        <v>8</v>
-      </c>
-      <c r="M6" t="n">
+      <c r="L16" t="n">
+        <v>8</v>
+      </c>
+      <c r="M16" t="n">
+        <v>9</v>
+      </c>
+      <c r="N16" t="n">
+        <v>9</v>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>- complex - heist - science fiction - study - man - free - past - cerebral - thought-provoking - layered - story-telling - sumptuous - aesthetics - flawless - editing - sound design - effects - musical score - pitch-perfect - cast - brilliant - unrivaled - filmmaking - dream - gay - lesbian - solidarity - fanfic - totem - spinning - spinning - dreaming - reality - masterpiece - gay - lesbian - solidarity - fanfic - spinning - dreaming - reality - masterpiece - personal - technical feat - collaborative - vision - design - workaholic - craft - loved ones - fabricated - simulated - catharsis - therapy - film editing - creativity - cleverness - scope - ideas - deliberate ambiguity - rules</t>
+        </is>
+      </c>
+      <c r="P16" t="n">
+        <v>292587330</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>546443300</v>
+      </c>
+      <c r="R16" t="n">
+        <v>839030630</v>
+      </c>
+      <c r="S16" t="n">
+        <v>62785337</v>
+      </c>
+      <c r="T16" t="inlineStr">
+        <is>
+          <t>Warner Bros.</t>
+        </is>
+      </c>
+      <c r="U16" t="inlineStr">
+        <is>
+          <t>PG-13</t>
+        </is>
+      </c>
+      <c r="V16" t="inlineStr">
+        <is>
+          <t>science-fiction</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>La La Land</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>2016</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Damien Chazelle</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>129</v>
+      </c>
+      <c r="F17" t="n">
+        <v>4.77</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>La La Land is a film that has divided audiences, with some finding it to be a magical and uplifting experience, while others have been left feeling depressed and despondent. The movie, directed by Damien Chazelle, follows the love story between Mia and Sebastian, played by Emma Stone and Ryan Gosling, as they navigate the challenges of pursuing their dreams in Hollywood. The film is praised for its stunning cinematography, beautiful musical numbers, and the electric chemistry between the two leads. Despite some criticisms of the storyline and pacing, La La Land has been hailed as a reinvention of the musical genre and a celebration of love and dreams.</t>
+        </is>
+      </c>
+      <c r="I17" t="n">
+        <v>8</v>
+      </c>
+      <c r="J17" t="n">
         <v>6</v>
       </c>
-      <c r="N6" t="n">
-        <v>5</v>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>- ambitious - emotional - messy - CGI - iconic - sinister - nostalgic - thrilling - surprising - ambitious - action-packed - comedic - intense - unexpected - fan-favorite - epic - tear-jerking - heartwarming - chaotic - conflicted - childhood memories - cameo - applause</t>
-        </is>
-      </c>
-      <c r="P6" t="n">
-        <v>814866759</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>1107732041</v>
-      </c>
-      <c r="R6" t="n">
-        <v>1922598800</v>
-      </c>
-      <c r="S6" t="n">
-        <v>260138569</v>
-      </c>
-      <c r="T6" t="inlineStr">
-        <is>
-          <t>Sony Pictures Releasing</t>
-        </is>
-      </c>
-      <c r="U6" t="inlineStr">
+      <c r="K17" t="n">
+        <v>9</v>
+      </c>
+      <c r="L17" t="n">
+        <v>7</v>
+      </c>
+      <c r="M17" t="n">
+        <v>8</v>
+      </c>
+      <c r="N17" t="n">
+        <v>9</v>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>- emotional - magical - bittersweet - captivating - romantic - impactful - mesmerizing - beautiful - electrifying - colorful - vibrant - nostalgic - heartbreaking - awe-inspiring - tender - dreamy - celebratory - exuberant - bold - rewarding - influential - masterful - corny - fantastic - fantastic - fantastic - fantastic - fantastic - fantastic - fantastic - fantastic - fantastic - fantastic - fantastic - fantastic - fantastic - fantastic - fantastic - fantastic - fantastic - fantastic - fantastic - fantastic - fantastic - fantastic - fantastic - fantastic - fantastic - fantastic - fantastic - fantastic - fantastic - fantastic - fantastic - fantastic - fantastic - fantastic - fantastic - fantastic - fantastic - fantastic - fantastic - fantastic - fantastic - fantastic - fantastic - fantastic - fantastic - fantastic</t>
+        </is>
+      </c>
+      <c r="P17" t="n">
+        <v>151101803</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>320887518</v>
+      </c>
+      <c r="R17" t="n">
+        <v>471991358</v>
+      </c>
+      <c r="S17" t="n">
+        <v>881104</v>
+      </c>
+      <c r="T17" t="inlineStr">
+        <is>
+          <t>Lionsgate Films</t>
+        </is>
+      </c>
+      <c r="U17" t="inlineStr">
         <is>
           <t>PG-13</t>
         </is>
       </c>
-      <c r="V6" t="inlineStr">
-        <is>
-          <t>Action Adventure Fantasy Sci-Fi</t>
+      <c r="V17" t="inlineStr">
+        <is>
+          <t>music</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Whiplash</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>2014</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Damien Chazelle</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>107</v>
+      </c>
+      <c r="F18" t="n">
+        <v>4.83</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Whiplash is a film about a young drummer named Andrew who is pushed to his limits by his intense and abusive music teacher, Terence Fletcher. The movie is known for its heart-pounding intensity, incredible performances by Miles Teller and J.K. Simmons, and its exploration of the quest for greatness in the world of jazz music. The film has been described as anxiety-inducing, captivating, and a cinematic masterpiece by many viewers.</t>
+        </is>
+      </c>
+      <c r="I18" t="n">
+        <v>8</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0</v>
+      </c>
+      <c r="K18" t="n">
+        <v>9</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0</v>
+      </c>
+      <c r="M18" t="n">
+        <v>9</v>
+      </c>
+      <c r="N18" t="n">
+        <v>10</v>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>- intense - anxiety-inducing - passionate - powerful - mesmerizing - energetic - riveting - flawless - incredible - heart-pounding - breathtaking - prodigious - stupefying - invigorating - romantic - perfect - goosebumps-inducing - taut - engrossing - crackling - authentic - percussive - brilliant - psychopath</t>
+        </is>
+      </c>
+      <c r="P18" t="n">
+        <v>13092000</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>36348474</v>
+      </c>
+      <c r="R18" t="n">
+        <v>49449489</v>
+      </c>
+      <c r="S18" t="n">
+        <v>135388</v>
+      </c>
+      <c r="T18" t="inlineStr">
+        <is>
+          <t>Sony Pictures Classics</t>
+        </is>
+      </c>
+      <c r="U18" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="V18" t="inlineStr">
+        <is>
+          <t>music</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Coco</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>2017</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Lee Unkrich</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>105</v>
+      </c>
+      <c r="F19" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.58</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Coco is a visually stunning and emotionally powerful animated film that explores themes of family, memory, and the afterlife. It follows the story of a young boy named Miguel who embarks on a journey to the Land of the Dead to uncover his family's history and pursue his passion for music. The film has been praised for its vibrant animation, heartfelt storytelling, and memorable music, making it a must-watch for audiences of all ages.</t>
+        </is>
+      </c>
+      <c r="I19" t="n">
+        <v>9</v>
+      </c>
+      <c r="J19" t="n">
+        <v>10</v>
+      </c>
+      <c r="K19" t="n">
+        <v>8</v>
+      </c>
+      <c r="L19" t="n">
+        <v>9</v>
+      </c>
+      <c r="M19" t="n">
+        <v>8</v>
+      </c>
+      <c r="N19" t="n">
+        <v>9</v>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>- death - murder - loss - grief - aging - dementia - living skeletons - deadbeat dads - devastation - heartwarming - crying - trauma - depression - sobbing - remember - tears - skeletons - breathtaking - guitar tutorial - chills - cathartic - abuse - power - colorful - vibrant - coming of age - innovative animations - soundtrack - dreams - family - forgiveness - visual effects - cinematography - feels - cultural - emotional - heartstrings - heartwarming - heartwrenching - beautiful - heartwarming - heartwrenching - heartwarming - heartwrenching - heartwarming - heartwrenching - heartwarming - heartwrenching - heartwarming - heartwrenching - heartwarming -</t>
+        </is>
+      </c>
+      <c r="P19" t="n">
+        <v>210460015</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>617909171</v>
+      </c>
+      <c r="R19" t="n">
+        <v>828369186</v>
+      </c>
+      <c r="S19" t="n">
+        <v>50802605</v>
+      </c>
+      <c r="T19" t="inlineStr">
+        <is>
+          <t>Walt Disney Studios Motion Pictures</t>
+        </is>
+      </c>
+      <c r="U19" t="inlineStr">
+        <is>
+          <t>PG</t>
+        </is>
+      </c>
+      <c r="V19" t="inlineStr">
+        <is>
+          <t>music</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Bohemian Rhapsody</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>2018</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Bryan Singer</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>135</v>
+      </c>
+      <c r="F20" t="n">
+        <v>1.87</v>
+      </c>
+      <c r="G20" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Bohemian Rhapsody is a divisive film that has received mixed reviews from users on Letterboxd. While some praise Rami Malek's performance as Freddie Mercury and the energetic Live Aid concert sequence, others criticize the film for its inaccuracies, lack of depth in portraying Mercury's queerness, and overall formulaic and exploitative nature. The movie is seen as a missed opportunity to delve deeper into the complexities of Queen and their iconic frontman. Despite its flaws, the film's soundtrack of Queen's music remains a highlight for many viewers.</t>
+        </is>
+      </c>
+      <c r="I20" t="n">
+        <v>2</v>
+      </c>
+      <c r="J20" t="n">
+        <v>4</v>
+      </c>
+      <c r="K20" t="n">
+        <v>3</v>
+      </c>
+      <c r="L20" t="n">
+        <v>2</v>
+      </c>
+      <c r="M20" t="n">
+        <v>1</v>
+      </c>
+      <c r="N20" t="n">
+        <v>2</v>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>- abominable - exploitative - inept - subpar - lacking - lost - disrespectful - incoherent - insipid - formulaic - tragic - manipulative - painful - self-conscious - simplified - lowest-common-denominator - charmless - haphazard - controversies - musical - charmed - controversies - musical - musical - musical - musical - musical - musical - musical - musical - musical - musical - musical - musical - musical - musical - musical - musical - musical - musical - musical - musical - musical - musical - musical - musical - musical - musical - musical - musical - musical - musical - musical - musical - musical - musical - musical - musical - musical - musical - musical - musical - musical - musical - musical -</t>
+        </is>
+      </c>
+      <c r="P20" t="n">
+        <v>216668042</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>694141269</v>
+      </c>
+      <c r="R20" t="n">
+        <v>910813521</v>
+      </c>
+      <c r="S20" t="n">
+        <v>51061119</v>
+      </c>
+      <c r="T20" t="inlineStr">
+        <is>
+          <t>Twentieth Century Fox</t>
+        </is>
+      </c>
+      <c r="U20" t="inlineStr">
+        <is>
+          <t>PG-13</t>
+        </is>
+      </c>
+      <c r="V20" t="inlineStr">
+        <is>
+          <t>music</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Priscilla</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>2023</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Sofia Coppola</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>110</v>
+      </c>
+      <c r="F21" t="n">
+        <v>4.04</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.73</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Priscilla is a film that delves into the relationship between Priscilla Presley and Elvis Presley, exploring themes of grooming, isolation, and the loss of innocence. Directed by Sofia Coppola, the movie humanizes Elvis's character and offers a critical perspective on his behavior. The performances, particularly by Cailee Spaeny, are praised for their depth and grace. The film is visually remarkable and emotionally impactful, leaving viewers with a lot to think about. Despite some mixed reviews, Priscilla is seen as a thought-provoking and important addition to the biopic genre.</t>
+        </is>
+      </c>
+      <c r="I21" t="n">
+        <v>8</v>
+      </c>
+      <c r="J21" t="n">
+        <v>7</v>
+      </c>
+      <c r="K21" t="n">
+        <v>9</v>
+      </c>
+      <c r="L21" t="n">
+        <v>6</v>
+      </c>
+      <c r="M21" t="n">
+        <v>7</v>
+      </c>
+      <c r="N21" t="n">
+        <v>8</v>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>- car - elvis - man - subtitles - Lana Del Rey - Austin Butler - disagreement - men - Stitch - cancel plans - individuality - prisoner - Sofia Coppola - women - asexual - Jacob Elordi - Tom Hanks - intellectual - Cailee Spaeny - beautiful cage - All Too Well - Nate Jacobs - loneliness - control - passion - justice - toothless - emotional core - grooming - predatory behavior - American royalty - childhood - dark fairytale - lana del rey vinyl - cat eyes - empathy - trigger warning - gasped - basketball player - y/n - bad happened - piece of shit - demise of innocence - visual - dark - honest - critical - remarkable - phenomenal - unrealistic expectations - muted - dreamy -</t>
+        </is>
+      </c>
+      <c r="P21" t="n">
+        <v>20960939</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>12063055</v>
+      </c>
+      <c r="R21" t="n">
+        <v>33023994</v>
+      </c>
+      <c r="S21" t="n">
+        <v>132139</v>
+      </c>
+      <c r="T21" t="inlineStr">
+        <is>
+          <t>A24</t>
+        </is>
+      </c>
+      <c r="U21" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="V21" t="inlineStr">
+        <is>
+          <t>music</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Correção nas informações regionais e atualizações no excel
</commit_message>
<xml_diff>
--- a/letterboxd_scraping/movie_info.xlsx
+++ b/letterboxd_scraping/movie_info.xlsx
@@ -568,7 +568,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Everything Everywhere All at Once is a visually dazzling, emotionally resonant, and wildly imaginative film that combines elements of martial arts, sci-fi, comedy, and family drama. With stellar performances, creative storytelling, and a unique multiverse concept, it has left audiences in awe and deeply moved. Despite some mixed reviews, it has been praised for its originality, humor, and heartfelt moments, making it a must-watch for those seeking a truly unique cinematic experience.</t>
+          <t>Everything Everywhere All at Once is a visually stunning, emotionally resonant, and wildly imaginative film that explores themes of family, identity, and the multiverse. With a mix of martial arts, comedy, and heartfelt moments, the movie keeps audiences engaged and entertained throughout. The performances, particularly from Michelle Yeoh, are praised for their depth and authenticity. While some find the film to be overwhelming or lacking in certain areas, many viewers appreciate its creativity and originality, making it a standout cinematic experience.</t>
         </is>
       </c>
       <c r="I2" t="n">
@@ -591,7 +591,7 @@
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>- multiverse - martial arts - family drama - visually dazzling - heartfelt - creative - ambitious - original - funny - emotional - chaotic - kinetic - daring - expertly choreographed - endlessly creative - laugh-out-loud funny - genuine emotional core - intelligent filmmaking - lowbrow humor - existential - philosophical - action-packed - moving - thought-provoking - authentic Asian identity - Michelle Yeoh - Jamie Lee Curtis - Stephanie Hsu - Ke Huy Quan - visually dynamic - technically dazzling - thematically resonant - audacious - sublime - hilarious - tiresome - surreal - zany - whimsical - absurd - heartfelt - melancholic - immature - inventive - dense - expansive - wacky - high-concept - sentimental - ridiculous - intellectual</t>
+          <t>- multiverse - martial arts - family drama - visually dazzling - heartfelt - creative - original - ambitious - funny - emotional - chaotic - kinetic - daring - expertly choreographed - endlessly creative - laugh-out-loud funny - genuine emotional core - intelligent filmmaking - lowbrow humor - existential - philosophical - action-packed - moving - thought-provoking - authentic Asian identity - Michelle Yeoh - Jamie Lee Curtis - Stephanie Hsu - Ke Huy Quan - visually dynamic - technically dazzling - audacious - sublime - hilarious - tiresome - silly - sincere - zany - epic - expansive - magic trick - grounded - breathless climax - acrobatic action scenes - pastiche - heartfelt moments - multiverse gimmick - existential questions -</t>
         </is>
       </c>
       <c r="P2" t="n">
@@ -650,7 +650,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Spider-Man: Into the Spider-Verse is hailed as the best Spider-Man film ever made, with stunning animation that captivates viewers. The film is praised for its creativity, humor, and understanding of the character of Spider-Man. Fans appreciate the diverse representation of Spider-People from different dimensions and the fresh take on the superhero genre. The movie's visuals, soundtrack, and storytelling are all highlighted as exceptional, making it a standout in the world of animated and superhero films.</t>
+          <t>Spider-Man: Into the Spider-Verse is hailed as the best Spider-Man film ever made, with stunning animation that captivates viewers. The film is praised for its creativity, humor, and understanding of the character of Spider-Man. It reinvigorates the superhero genre and is considered a masterpiece in animation. The diverse cast of Spider-People adds depth to the story, making it a visually breathtaking and emotionally resonant experience. The film's soundtrack and score are also highlighted as exceptional, contributing to its overall impact. Overall, Spider-Man: Into the Spider-Verse is celebrated as a groundbreaking and unforgettable cinematic achievement.</t>
         </is>
       </c>
       <c r="I3" t="n">
@@ -673,7 +673,7 @@
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>- groundbreaking - visually stunning - creative - understanding - funny - animated - reinvigorates - diverse - hyper-popular - expressive - colorful - action-packed - emotional - visually daring - visually inventive - visually refreshing - visually vibrant - visually mesmerizing - visually original - visually distinctive - visually kinetic - visually jaw-dropping - visually well-drawn - original - invigorating - talented - moving - bewildering - vibrant - confident - witty - relatable - beloved - fresh - beautiful - fun - mature - hypnotic - mesmerizing - striking - terrific - engaging - sympathetic - hilarious - heartwarming - emotional - jaw-dropping - life-changing - awe-inspiring - exhilarating - hilarious - goofy - powerful - clear - dynamic - expressive - rhyth</t>
+          <t>- groundbreaking - visually stunning - creative - understanding - funny - animated - reinvigorates - diverse - hyper-popular - expressive - colorful - action-packed - emotional - visually inventive - fresh - vibrant - inventive - original - invigorating - relatable - beloved - kinetic - jaw-dropping - top-tier storytelling - well-drawn - well-executed - unique - well-written - enjoyable - masterpiece - game-changing - iconic - legendary - visually breathtaking - visually interesting - visually unique - visually arresting - visually fresh - visually vibrant - visually striking - visually dazzling - visually mesmerizing - visually hypnotic - visually beautiful - visually awe-inspiring - visually overwhelming - visually impressive - visually captivating - visually engaging - visually appealing - visually stunning - visually mind-blow</t>
         </is>
       </c>
       <c r="P3" t="n">
@@ -732,7 +732,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>The Dark Knight is hailed as the best superhero movie ever made, with Heath Ledger's performance as the Joker being a standout. The film is considered a masterpiece by many, with intense action sequences and a dark, realistic approach to the Batman story. Despite some flaws, it remains a cultural landmark and a game-changer in the world of superhero films. Christopher Nolan's direction, Hans Zimmer's score, and the performances of the cast, especially Ledger, make this movie unforgettable and influential in pop culture.</t>
+          <t>The Dark Knight is hailed as the best superhero movie ever made, with Heath Ledger's performance as the Joker being a standout. The film is praised for its thrilling and riveting scenes, as well as its exploration of themes like chaos and order. Despite some flaws, it is considered a cinematic masterpiece that has left an unforgettable mark on pop culture.</t>
         </is>
       </c>
       <c r="I4" t="n">
@@ -742,20 +742,20 @@
         <v>8</v>
       </c>
       <c r="K4" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L4" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="M4" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="N4" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>- masterpiece - best superhero movie - heath ledger - joker - iconic - thrilling - intense - game-changer - cultural landmark - exhilarating - riveting - homoerotic tension - Cillian Murphy - cinematic excellence - anarchy - chaos - considerate - iconic quotes - masterpiece - brilliant - disturbing - intense - phenomenal - realistic - thrilling - unforgettable - influential - action-packed - dark - serious - tense - perfection - flawless - masterpiece - best Batman movie - best Nolan movie - best sequel - favorite movie - masterpiece - dark and realistic - mature storytelling - triumph - iconic - thrilling - intense - masterpiece - masterpiece - masterpiece - masterpiece - masterpiece</t>
+          <t>- masterpiece - iconic - influential - intense - thrilling - dark - realistic - game-changer - unforgettable - cinematic excellence - riveting - exhilarating - brilliant - genius - legendary - perfection - intense thriller - smart - layered - complex - deep - impactful - profound - thought-provoking - nihilistic - brutal - chaotic - poetic - bold - daring - epic - monumental - masterful - captivating - engaging - suspenseful - dark humor - intense action - iconic performances - unforgettable scenes - cultural landmark - timeless - classic - masterpiece - flawless - perfection - best superhero movie - best Batman movie - best Nolan movie - best sequel - favorite movie - iconic villain - memorable quotes - intense opening sequence - dense - serious - masterpiece - masterpiece - masterpiece</t>
         </is>
       </c>
       <c r="P4" t="n">
@@ -814,7 +814,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Inception is a visually stunning and complex heist film that delves into the subconscious mind. With a brilliant cast and masterful direction from Christopher Nolan, the movie explores themes of guilt, grief, and the power of dreams. The intricate plot, mind-bending visuals, and Hans Zimmer's iconic score make it a modern masterpiece that continues to captivate audiences. The film's ambiguous ending leaves viewers questioning reality and the nature of dreams. Overall, Inception is a thrilling and thought-provoking cinematic experience that has stood the test of time.</t>
+          <t>Inception is a complex and visually stunning film directed by Christopher Nolan. The movie follows Dom Cobb, a master thief who enters people's dreams to steal their secrets. With a brilliant cast and a mind-bending plot, Inception is a cerebral pop-masterpiece that combines thought-provoking storytelling with sumptuous aesthetics. The film explores themes of dreams, reality, and the power of the mind, leaving viewers questioning what is real and what is not. With a captivating score by Hans Zimmer and impressive editing, Inception is a brilliant and unrivaled piece of filmmaking that continues to captivate audiences.</t>
         </is>
       </c>
       <c r="I5" t="n">
@@ -837,7 +837,7 @@
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>- complex - heist - science fiction - study - cerebral - thought-provoking - layered - enthralling - brilliant - filmmaking - rent-free - gay - lesbian - fanfic - spinning - dream - 14 year old boys - homoerotic - dialogue - dreams - killing allegations - alarm clock - score - personal - emotional - intense - lucid dreaming - filmmaking - catharsis - action - dreamy - dream within a dream - inception - masterful - therapy - love - meta - character study - love - pop-rationalist - zingy - sad - mindbender - hot</t>
+          <t>- complex - heist - science fiction - study - man - free - past - cerebral - thought-provoking - layered - story-telling - sumptuous - aesthetics - flawless - editing - sound design - effects - musical score - pitch-perfect - cast - brilliant - unrivaled - filmmaking - rent free - gay - lesbian - solidarity - fanfic - totem - spinning - dreaming - beat - allegations - alarm clock - score - personal - technical feat - collaborative vision - design - fake worlds - feelings - workaholic - craft - time - loved ones - fabricated - simulated - catharsis - world-changing therapy - film editing - blown away - trust - people - dreams - lucid dreaming - filmmaking - remarkable -</t>
         </is>
       </c>
       <c r="P5" t="n">
@@ -896,7 +896,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Spider-Man: Across the Spider-Verse is a visually stunning, emotionally impactful, and creatively ambitious masterpiece of animated cinema. It pushes the boundaries of storytelling and animation, leaving viewers in awe with its vibrant colors, intricate details, and heartfelt moments. The film is a treat for fans of Spider-Man, offering a fresh take on the beloved character while introducing new elements and characters. Despite some minor criticisms, the overwhelming consensus is that this movie is a must-watch for any superhero or animation enthusiast.</t>
+          <t>Spider-Man: Across the Spider-Verse is being hailed as an overwhelming viewing experience, with stunning animation, humor, and a vibrant soundtrack. Viewers are left in awe of the visuals and storytelling, with many considering it a masterpiece of animated cinema. The film is praised for its creativity, heart, and ability to redefine superhero storytelling. Despite some minor criticisms, the general consensus is overwhelmingly positive, with many eagerly anticipating the next installment.</t>
         </is>
       </c>
       <c r="I6" t="n">
@@ -919,7 +919,7 @@
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>- overwhelming - outstanding - banger - lit - incredible - joy - perfect - holy shit - magical - mind-blowing - breathtaking - balance - goosebumps - staggering - ambitious - sensational - thought-provoking - masterpiece - vibrant - kinetic - maximalist - revolutionary - beautiful - humanize - stunning - peak - revolutionary - beautiful - funny - astounding - iconic - unforgettable - expressive - artistic - visually beautiful - joy - immeasurable - cool - joyous</t>
+          <t>- overwhelming - outstanding - banger - lit - incredible - joy - perfect - holy shit - magical - mind-blowing - breathtaking - balance - goosebumps - staggering - ambitious - sensational - thought-provoking - masterpiece - vibrant - kinetic - maximalist - revolutionary - beautiful - humanize - stunning - peak - revolutionary - beautiful - funny - astounding - iconic - unforgettable - expressive - visually beautiful - artistic - visually stunning - fleshed out - visually beautiful - joy - immeasurable - cool - cliffhangers</t>
         </is>
       </c>
       <c r="P6" t="n">
@@ -978,7 +978,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Barbie, directed by Greta Gerwig, is a visually gorgeous and complex film that delves into themes of womanhood, gender roles, and self-discovery. While some viewers found it to be historically inaccurate and lacking in substance, others praised it for its note-perfect performances, meta commentary, and feminist messaging. The film has been described as a triumph of design, a triumph of manufactured storytelling, and a triumph of existentialism. Overall, Barbie has been a divisive yet thought-provoking cinematic experience that has left audiences with a mix of emotions and reactions.</t>
+          <t>Barbie, directed by Greta Gerwig, is a visually gorgeous and complex film that delves into themes of womanhood, gender roles, and self-discovery. While some viewers found it to be historically inaccurate and lacking in depth, others praised it for its note-perfect performances, meta commentary, and feminist messaging. The film has been described as a triumph of design, a triumph of manufactured storytelling, and a triumph of existentialism. Overall, Barbie has been a divisive yet thought-provoking cinematic experience that has left audiences with a mix of emotions and reactions.</t>
         </is>
       </c>
       <c r="I7" t="n">
@@ -1001,7 +1001,7 @@
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>- broken - dark humor - existential - funny - historical inaccuracy - scissor - coming-of-age - note-perfect performances - meaningful - acting classes - Ryan Gosling - Ken - existential crisis - visually gorgeous - complex - big-budget - John Waters-inspired - feminist - meta jokes - reverse sexism - liberal feminism - patriarchal society - matriarchal society - existentialism - self-discovery - vibrant - cheeky - feminist parable - representation matters - joyful - insightful - gender roles - identity - self-worth - existential romp - satirical - meta commentary - campy - nuanced - adult - dystopia - fairytale imagination - satire - meta commentary - campiness - existential dread - glitz - glamor - existential dread -</t>
+          <t>- meta - funny - feminist - existential - visually gorgeous - complex - big-budget - surreal - thought-provoking - jubilant - moving - underdeveloped - self-discovery - vibrant - cheeky - satirical - campy - nuanced - adult - empowering - diverse - clever - heartfelt - joyful - existential dread - glitz - glamor - dreamy - empowering - surrealistic - clever - insightful - satirical - meta-commentary - absurd - shallow - disappointing - visually stunning - hilarious - emotional - feminist - existential - thought-provoking - jubilant - moving - underdeveloped - self-discovery - vibrant - cheeky - satirical - campy - nuanced - adult - empowering - diverse - clever - heartfelt -</t>
         </is>
       </c>
       <c r="P7" t="n">
@@ -1060,7 +1060,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Everything Everywhere All at Once is a visually stunning, emotionally resonant, and wildly imaginative film that explores themes of family, identity, and the multiverse. With a mix of martial arts, comedy, and heartfelt moments, the movie keeps audiences engaged and entertained throughout. The performances, particularly from Michelle Yeoh, are praised for their depth and authenticity. While some find the film to be overwhelming or lacking in emotional payoff, many viewers appreciate its creativity and originality. Overall, it's a unique and ambitious cinematic experience that leaves a lasting impact on those who watch it.</t>
+          <t>"Everything Everywhere All at Once" is a visually stunning and emotionally resonant film that combines elements of martial arts, sci-fi, comedy, and family drama. With a mix of heartfelt moments and absurd humor, the movie explores themes of multiverses, family relationships, and the meaning of life. Featuring standout performances and creative storytelling, this film has left a lasting impact on viewers, making it a must-watch for those seeking a unique cinematic experience.</t>
         </is>
       </c>
       <c r="I8" t="n">
@@ -1083,7 +1083,7 @@
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>- multiverse - martial arts - family drama - visually dazzling - heartfelt - creative - ambitious - original - funny - emotional - Michelle Yeoh - action-packed - thought-provoking - Asian identity - zany - moving - existential - everything bagel - absurd - sincere - cinematic - groundbreaking - innovative - imaginative - hilarious - chaotic - kinetic - daring - expertly choreographed - heartfelt - poignant - audacious - technically dazzling - thematic - resonant - audacious - visionary - masterpiece - symphony of chaos - honest - compassionate - multiverse gimmick - genuine - emotional core - genuine amount of honesty - compassion - multiverse - existential questions - thematic - existential - philosophical - emotional payoffs - human level - grounded - visually dynamic - ambitious -</t>
+          <t>- multiverse - martial arts - family drama - visually dazzling - heartfelt - creative - ambitious - original - funny - emotional - chaotic - kinetic - daring - expertly choreographed - endlessly creative - laugh-out-loud funny - genuine emotional core - intelligent filmmaking - lowbrow humor - existential - thought-provoking - visionary - masterpiece - symphony of chaos - honest - compassionate - multiverse gimmick - trending trope - genuine amount of honesty - compassion - Asian identity - Michelle Yeoh - strong performances - authentic - magic trick - grounded - everything has meaning - breathless climax - acrobatic action scenes - emotional resonance - familial rifts - convoluted relationship - fun sci-fi kung fu - Reddit - unbearable - manipulative -</t>
         </is>
       </c>
       <c r="P8" t="n">
@@ -1142,7 +1142,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Interstellar is a visually stunning and emotionally heavy film that explores themes of love, time, and survival. The movie follows a team of explorers traveling through a wormhole in space to ensure humanity's survival. With breathtaking visuals, a powerful score, and strong performances, the film takes viewers on a journey through time and space. While some find it to be a masterpiece, others criticize its ambitious storytelling and emotional depth. Overall, Interstellar is a thought-provoking and visually captivating experience that leaves a lasting impact on its audience.</t>
+          <t>Interstellar is a visually stunning and emotionally heavy film that explores themes of love, time, and the unknown. The movie follows Cooper, played by Matthew McConaughey, on a journey through space to ensure humanity's survival. With breathtaking visuals and a powerful score by Hans Zimmer, the film delves into the complexities of relationships, family, and the mysteries of the universe. While some viewers found the film to be overly ambitious or flawed in its execution, many praised it as a cinematic masterpiece that evokes deep emotions and leaves a lasting impact. Overall, Interstellar is a thought-provoking and visually captivating experience that has left a lasting impression on audiences.</t>
         </is>
       </c>
       <c r="I9" t="n">
@@ -1165,7 +1165,7 @@
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>- emotional - visually stunning - ambitious - masterpiece - thought-provoking - intense - sci-fi - space exploration - love transcends time - breathtaking - rollercoaster - visually monumental - family drama - heartbreaking - awe-inspiring - epic - transcendent - profound - ambitious storytelling - complex - beautifully shot - powerful - cathartic - intense performances - jaw-dropping - goosebumps - compelling - overwhelming - awe-inducing - visually striking - emotional journey - visually stunning - masterpiece - cosmic awe - emotional transcendence - muddled - aggravating - conflict between science and faith - visually iconic - intense storytelling - complex characters - phenomenal - forgiveness - forgiveness - forgiveness - forgiveness</t>
+          <t>- emotional - visually stunning - ambitious - masterpiece - cathartic - thought-provoking - intense - sci-fi - space exploration - love transcends time - visually breathtaking - powerful - Nolan's best - Hans Zimmer score - rollercoaster - epic - family drama - human odyssey - jaw-dropping - heartbreaking - profound - visually monumental - mind-enriching - awe-inspiring - overwhelming - cosmic awe - emotional transcendence - muddled - aggravating - conflict between science and faith - intense performances - visually stunning - euphoric wonder - transcends time and space - poetic - overwhelming - perfection</t>
         </is>
       </c>
       <c r="P9" t="n">
@@ -1224,7 +1224,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Dune is a visually stunning and meticulously crafted adaptation of the iconic science fiction novel, featuring a chosen one named Paul who must navigate a complex universe filled with political intrigue and mystical powers. The film immerses viewers in a world of epic scale and grandeur, with impressive world-building and a captivating score by Hans Zimmer. While some find the film to be methodical and lacking in emotional depth, others praise its faithful adaptation and breathtaking visuals. Overall, Dune is a monumental cinematic achievement that leaves audiences eagerly anticipating the next installment.</t>
+          <t>Dune is a visually stunning and meticulously crafted adaptation of the beloved sci-fi novel, featuring a chosen one named Paul who must navigate a dangerous universe to secure the future of his family and people. The film immerses viewers in a world of intricate world-building, epic scale, and political intrigue, all set against the backdrop of a desert planet with a precious resource. While some find the film to be a masterpiece and a cinematic achievement, others feel it is overly long, lacking in emotional depth, and dominated by a loud and relentless score. With a mix of praise for its grandeur and criticism for its pacing, Dune has left audiences divided but intrigued for the upcoming sequel.</t>
         </is>
       </c>
       <c r="I10" t="n">
@@ -1247,7 +1247,7 @@
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>- chosen one - dehydrated - orange - zendaya dreams - TikTok - documentary - sand on titties - worldbuilding - candy crush - PAUL - Anakin - Hans Zimmer - moaning - Seven - monumental - global warming - desert power - enormous scale - brutalist spectacle - sandworm - floating fatass - ms. lawton - duncan idaho - dilfs - alien language - boring - epic - timothée chalamet - Avengers - wet dreams - sandworm screen time - oscar isaac - incomplete masterpiece - Hans Zimmer score - sandworms - Dune 2 - sci-fi masterpiece - Alaskan Bull Worm - epic scale - Dune hive - epic sci-fi - sand in the ass -</t>
+          <t>- chosen one - dehydrated - orange - zendaya dreams - TikTok - documentary-like - sand on titties - worldbuilding - candy crush - PAUL - Anakin - Hans Zimmer music video - timothee chalamet moaning - box scene - monumental - global warming - desert power - immersive - brutalist spectacle - psychedelia - floating fatass Baron Harkonnen - duncan idaho - dilfs - alien language - boring - epic - timothee chalamet action star - BIG BEAUTIFUL SPACE MOVIE - Jason Momoa - industrial design - thousand-yard-stares - The Sandlot - worming - epic scale - epic cast - epic directing - epic soundtrack - epic setting -</t>
         </is>
       </c>
       <c r="P10" t="n">
@@ -1306,7 +1306,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Spider-Man: Into the Spider-Verse is hailed as the best Spider-Man film ever made, with stunning animation that captivates viewers. The film is praised for its creativity, humor, and understanding of the character of Spider-Man. It reinvigorates the superhero genre and is considered a masterpiece in animation. The diverse cast of Spider-People adds depth to the story, making it a visually breathtaking and emotionally resonant experience. The film is celebrated for its unique style, engaging storytelling, and memorable characters, making it a standout in the world of superhero movies.</t>
+          <t>Spider-Man: Into the Spider-Verse is hailed as the best Spider-Man film ever made, with stunning animation that captivates viewers. The film is praised for its creativity, humor, and understanding of the character of Spider-Man. It reinvigorates the superhero genre and is considered a masterpiece in animation. The diverse cast of Spider-People adds depth to the story, making it a visually breathtaking and emotionally resonant experience. The film's soundtrack and score are also highlighted as exceptional, contributing to its overall impact. Overall, Spider-Man: Into the Spider-Verse is celebrated as a groundbreaking and unforgettable cinematic achievement.</t>
         </is>
       </c>
       <c r="I11" t="n">
@@ -1329,7 +1329,7 @@
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>- groundbreaking - visually stunning - creative - understanding - funny - animated - reinvigorates - diverse - hyper-popular - expressive - colorful - action-packed - emotional - visually daring - inventive - fresh - vibrant - unique - heartfelt - jaw-dropping - original - invigorating - well-drawn - relatable - beloved - kinetic - vibrant - well-executed - enjoyable - masterpiece - visually interesting - hypnotic - mesmerizing - striking - mature - fresh - beautiful - fun - powerful - clear - goofy - hilarious - engaging - sympathetic - exhilarating - hilarious - witty - emotional - heartwarming - electric - awe-inspiring - life-changing - iconic - legendary - unforgettable - impactful - influential - daring - confident - impressive - powerful - clear</t>
+          <t>- best spider-man film - funny - creative - wonderfully animated - understanding of the character - visually stunning - visually daring - visually inventive - visually unique - visually vibrant - visually breathtaking - visually original - visually striking - visually mesmerizing - visually refreshing - visually fresh - visually kinetic - visually jaw-dropping - visually distinctive - visually influential - visually well-drawn - visually comic book-like - visually immersive - visually engaging - visually expressive - visually colorful - visually textured - visually rhythmic - visually expressive - visually psychedelic - visually Lichtenstein-esque - visually pop art-stylings - visually near-psychedelic - visually dense - visually detailed - visually vibrant - visually beautiful - visually fresh - visually original - visually inventive - visually daring - visually stunning - visually mesmer</t>
         </is>
       </c>
       <c r="P11" t="n">
@@ -1388,7 +1388,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Spider-Man: Into the Spider-Verse is hailed as the best Spider-Man film ever made, with stunning animation that is likened to a drug, injecting viewers with its beauty. The film is praised for its creativity, humor, and understanding of the character of Spider-Man. It is considered a groundbreaking achievement in animation and a reinvigoration of the superhero genre. The diverse cast of Spider-People is celebrated, with standout characters like Spider-Man Noir and Spider-Gwen. The film is lauded for its visuals, soundtrack, and emotional depth, making it a must-watch for fans of all ages.</t>
+          <t>Spider-Man: Into the Spider-Verse is hailed as the best Spider-Man film ever made, with stunning animation that captivates viewers. The film is praised for its creativity, humor, and understanding of the character of Spider-Man. It reinvigorates the superhero genre and is considered a masterpiece in animation. The diverse cast of Spider-People adds depth to the story, making it a visually breathtaking and emotionally resonant experience. The film's soundtrack and score are also highly praised, adding to its overall impact. Overall, Spider-Man: Into the Spider-Verse is a groundbreaking and unforgettable cinematic achievement.</t>
         </is>
       </c>
       <c r="I12" t="n">
@@ -1411,7 +1411,7 @@
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>- groundbreaking - visually stunning - creative - funny - understanding - reinvigorates - diverse - hyper-popular - expressive - colorful - action-packed - emotional - heartwarming - inclusive - fresh - vibrant - inventive - kinetic - relatable - beloved - original - invigorating - well-drawn - peak - jaw-dropping - awe-inspiring - mesmerizing - hypnotic - striking - mature - beautiful - fun - fresh - hilarious - engaging - sympathetic - exhilarating - hilarious - emotional - powerful - clear - goofy - confident - daring - impressive - unique - refreshing - inventive - vibrant - well-executed - enjoyable - dazzling - hypnotic - mesmerizing - striking - fresh - beautiful - fun - mature - hilarious - engaging - sympathetic -</t>
+          <t>- groundbreaking - visually stunning - creative - understanding - funny - animated - reinvigorates - diverse - hyper-popular - expressive - colorful - action-packed - emotional - visually daring - visually inventive - visually refreshing - vibrant - fresh - beautiful - fun - mature - inventive - imaginative - jaw-dropping - original - invigorating - kinetic - vibrant - well-drawn - relatable - beloved - unique - well-written - well-executed - enjoyable - visually impressive - visually unique - visually captivating - visually mesmerizing - visually breathtaking - visually striking - visually fresh - visually original - visually stunning - visually vibrant - visually inventive - visually dazzling - visually hypnotic - visually mesmerizing - visually beautiful - visually awe-inspiring - visually jaw-dropping - visually</t>
         </is>
       </c>
       <c r="P12" t="n">
@@ -1470,7 +1470,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Spider-Man: Across the Spider-Verse is being hailed as a visually stunning, emotionally impactful, and incredibly ambitious animated masterpiece. Viewers are overwhelmed by the creativity, humor, and heart of the film, with many praising its unique storytelling and groundbreaking animation. The movie has left audiences in awe, with some calling it the best Spider-Man film ever made and a true cinematic achievement. Despite some minor criticisms, the general consensus is overwhelmingly positive, with viewers eagerly anticipating the next installment in the series.</t>
+          <t>Spider-Man: Across the Spider-Verse is being hailed as an overwhelming viewing experience, with stunning animation, humor, and a vibrant soundtrack. Viewers are left in awe of the visuals and storytelling, with some even calling it a masterpiece. The film is praised for its creativity, emotional moments, and the way it redefines superhero storytelling. Despite some minor criticisms, the general consensus is overwhelmingly positive, with many eagerly anticipating the next installment.</t>
         </is>
       </c>
       <c r="I13" t="n">
@@ -1493,7 +1493,7 @@
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>- overwhelming - outstanding - banger - lit - incredible - joy - perfect - holy shit - magical - mind-blowing - breathtaking - balance - good - favorite - fried - incredible - masterpiece - sensational - thrilling - ambitious - beautiful - vibrant - kinetic - revolutionary - humanize - maximalist - stunning - emotional - vibing - satisfying - revolutionary - unbelievable - cringe - inject - weightless - vibrant - insane - beautiful - unforgettable - expressive - joyful - visually beautiful - artistic - fleshed out - giddiness - immeasurable - joy - cool - cliffhangers</t>
+          <t>- overwhelming - outstanding - banger - lit - incredible - joy - perfect - holy shit - magical - mind-blowing - breathtaking - balance - surprising - goosebumps - staggering - ambitious - vital - contemporary - revolutionary - sensational - jaw-dropping - heartfelt - thought-provoking - masterpiece - beautiful - vibrant - kinetic - maximalist - emotional - humanize - existential - funny - visually stunning - imaginative - funny - visually beautiful - funny - joyful - visually beautiful - joy - immeasurable - cool - joyous</t>
         </is>
       </c>
       <c r="P13" t="n">
@@ -1545,21 +1545,21 @@
         <v>125</v>
       </c>
       <c r="F14" t="n">
-        <v>4.76</v>
+        <v>4.75</v>
       </c>
       <c r="G14" t="n">
-        <v>0.49</v>
+        <v>0.5</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Spirited Away is a visually stunning and emotionally resonant masterpiece that captivates viewers with its magical world and rich storytelling. The film follows the journey of Chihiro, a young girl who finds herself in a mysterious and fantastical realm filled with gods, witches, and spirits. As Chihiro navigates this strange new world, she learns valuable lessons about courage, kindness, and the power of love. With its imaginative animation, memorable characters, and universal themes, Spirited Away has earned its reputation as one of the best animated films of all time.</t>
+          <t>Spirited Away is a visually stunning and emotionally resonant masterpiece that captivates viewers with its magical world and rich storytelling. The film follows the journey of Chihiro, a young girl who finds herself in a mysterious and fantastical realm filled with gods, witches, and spirits. As Chihiro navigates this strange world, she learns valuable lessons about courage, empathy, and the power of kindness. With its imaginative animation, memorable characters, and universal themes, Spirited Away has earned its reputation as one of the best animated films of all time.</t>
         </is>
       </c>
       <c r="I14" t="n">
         <v>9</v>
       </c>
       <c r="J14" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="K14" t="n">
         <v>8</v>
@@ -1568,14 +1568,14 @@
         <v>9</v>
       </c>
       <c r="M14" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="N14" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>- magical - immersive - imaginative - emotional - visually stunning - masterpiece - transformative - enchanting - nostalgic - whimsical - captivating - profound - beautiful - mesmerizing - timeless - intricate - rich - detailed - fantastical - unique - creative - thought-provoking - charming - moving - powerful - heartwarming - iconic - legendary - cinematic - masterful - legendary - unforgettable - whimsical - enchanting - mesmerizing - breathtaking - charming - delightful - profound - whimsical - heartwarming - captivating - magical - transformative - immersive - emotional - visually stunning - masterpiece - enchanting - nostalgic - imaginative - profound - charming - captivating - iconic - legendary - cinematic - breathtaking - powerful - moving - unique - creative - thought-provoking - rich</t>
+          <t>- imaginative - magical - transformative - emotional - visually stunning - immersive - enchanting - nostalgic - whimsical - profound - masterful - captivating - mesmerizing - fantastical - intricate - detailed - rich - beautiful - unique - thought-provoking - charming - touching - moving - profound - timeless - universal - ethereal - whimsy - bittersweet - melancholic - heartwarming - legendary - iconic - legendary - masterpiece - genius - creative - original - surreal - dreamlike - impactful - astonishing - impeccable - immaculate - enchanting - unforgettable - cinematic - fantastical - mythical - charming - delightful - heartwarming - emotional - whimsical - mesmerizing - transformative - immersive - magical - profound - beautiful - stunning - captivating - enchant</t>
         </is>
       </c>
       <c r="P14" t="n">
@@ -1634,7 +1634,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Ratatouille is a heartwarming Pixar film about a talented rat named Remy who dreams of becoming a chef. The movie explores themes of passion, identity, and the pursuit of dreams. With stunning animation, a charming Parisian setting, and a memorable score, Ratatouille is considered by many to be one of Pixar's best films. The story follows Remy's journey as he navigates the culinary world, proving that anyone can achieve greatness, no matter their background. The film's emotional moments, lovable characters, and messages of perseverance make it a timeless classic that resonates with audiences of all ages.</t>
+          <t>Ratatouille is a heartwarming Pixar film about a talented rat named Remy who dreams of becoming a chef. The movie explores themes of passion, identity, and the pursuit of one's dreams. With stunning animation, a charming Parisian setting, and a memorable score by Michael Giacchino, Ratatouille is considered by many to be one of Pixar's best films. The story follows Remy's journey as he navigates the culinary world, proving that anyone can achieve greatness, regardless of their background. The film's emotional moments, lovable characters, and messages of perseverance make it a timeless classic that continues to resonate with audiences.</t>
         </is>
       </c>
       <c r="I15" t="n">
@@ -1657,7 +1657,7 @@
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>- heartwarming - inspirational - comedic - emotional - culinary - Parisian - animated - masterpiece - rewatchable - thought-provoking - visually stunning - charming - lovable characters - relatable - comforting - magical - creative - engaging - touching - iconic - heartening - delightful - genius - feel-good - classic - memorable - entertaining - heartening - enchanting - captivating - heartwarming - whimsical - imaginative - brilliant - impactful - powerful - moving - beautiful - heartening - cinematic - timeless - exceptional - artistic - heartwarming - culinary genius - lovable rat - Parisian charm - animated gem - culinary delight - heartwarming tale - heartwarming message - heartwarming story - heartwarming characters - heartw</t>
+          <t>- heartwarming - inspirational - comedic - emotional - culinary - Parisian - animated - masterpiece - rewatchable - thought-provoking - charming - creative - lovable - visually stunning - enchanting - magical - nostalgic - impactful - engaging - delightful - genius - relatable - comforting - iconic - memorable - entertaining - heartening - touching - heartening - beautiful - captivating - imaginative - powerful - moving - profound - impressive - brilliant - unique - classic - heartwarming - funny - adorable - cinematic - dynamic - engaging - whimsical - delightful - exceptional - extraordinary - enchanting - captivating - brilliant - innovative - heartwarming - heartwarming - heartwarming - heartwarming - heartwarming - heartwarming - heart</t>
         </is>
       </c>
       <c r="P15" t="n">
@@ -1716,7 +1716,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Fantastic Mr. Fox is a stop-motion puppet animation film directed by Wes Anderson that follows the story of Mr. Fox, voiced by George Clooney, as he assembles a team for elaborate heists. The film features a diverse group of characters, including a tall alcoholic rat voiced by Willem Dafoe. With vibrant colors, quirky dialogue, and a heartwarming story about family, this movie is a unique and visually stunning masterpiece that has captivated audiences and become a favorite for many.</t>
+          <t>Fantastic Mr. Fox is a stop-motion puppet animation film directed by Wes Anderson that follows the story of Mr. Fox, voiced by George Clooney, as he assembles a team for elaborate heists. The film features a diverse group of characters, including a tall alcoholic rat voiced by Willem Dafoe. With vibrant colors, quirky dialogue, and a heartwarming story about family, this movie is a unique and visually stunning masterpiece that has captivated audiences with its charm and humor.</t>
         </is>
       </c>
       <c r="I16" t="n">
@@ -1739,7 +1739,7 @@
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>- stop-motion - animation - Wes Anderson - quirky - charming - heist - furry - colorful - unique - Wes Anderson style - feel good - Wes Anderson dialogue - Wes Anderson aesthetic - Wes Anderson commentary - Wes Anderson universe - Wes Anderson genius - Wes Anderson ranked - Wes Anderson magnum opus - Wes Anderson perfection - Wes Anderson adaptation - Wes Anderson filmmaking - Wes Anderson style - Wes Anderson humor - Wes Anderson characters - Wes Anderson visual - Wes Anderson heart - Wes Anderson art - Wes Anderson control - Wes Anderson distinctive - Wes Anderson innovative - Wes Anderson intricate - Wes Anderson vibrant - Wes Anderson beautiful - Wes Anderson iconic - Wes Anderson iconic - Wes Anderson existential - Wes Anderson existential crisis - Wes Anderson humor - Wes Anderson themes - Wes Anderson storytelling -</t>
+          <t>- stop-motion - animation - heist - furry - orange - Wes Anderson - Willem Dafoe - George Clooney - humor - quirky - unique - charm - love - family - dialogue - visual - detail - feel-good - joy - intimate - perfection - art - vibrant - sarcastic - colorful - heartwarming - whimsical - iconic - existential - existential crisis - fall season - rewatchable - masterpiece - different - fantastic - vibrant - intricate - innovative - universal - emotional - nostalgic - delightful - vibrant - quirky - deadpan - candid - unique - surreal - mesmerizing - surreal - whimsical - whimsical - whimsical - whimsical - whimsical - whimsical - whimsical - whimsical - whimsical - whimsical</t>
         </is>
       </c>
       <c r="P16" t="n">
@@ -1798,30 +1798,30 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Barbie, directed by Greta Gerwig, has received mixed reviews from users on Letterboxd. Some praise the film for its humor, performances, and exploration of female coming-of-age themes. Others criticize it for being historically inaccurate and failing to deliver meaningful commentary on gender and feminism. The movie is described as visually gorgeous, complex, and big-budget, with standout performances from Margot Robbie and Ryan Gosling. Overall, Barbie is seen as a unique and divisive film that tackles existential themes and societal issues within the context of a toy commercial.</t>
+          <t>Barbie, directed by Greta Gerwig, has received mixed reviews from users on Letterboxd. Some viewers found it to be a historically inaccurate yet funny film, with standout performances from Margot Robbie and Ryan Gosling. Others praised the film for its feminist themes and meta-commentary on gender roles. However, some critics felt that the movie fell short in delivering meaningful commentary and was ultimately a shallow, corporate product. Despite the divisive opinions, Barbie was commended for its vibrant visuals, clever humor, and unique take on the iconic toy brand.</t>
         </is>
       </c>
       <c r="I17" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J17" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K17" t="n">
         <v>9</v>
       </c>
       <c r="L17" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M17" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N17" t="n">
         <v>8</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>- meta - funny - feminist - existential - visually gorgeous - complex - big-budget - surreal - vibrant - cheeky - jubilant - moving - thoughtful - layered - emotional - note-perfect performances - hoot - divisive - spirited - hopeful - insightful - satirical - campy - nuanced - adult - imaginative - joyful - unapologetically woman - existential dystopia - childlike happiness - disappointing - shallow - flat - lame - absurd - surrealistic - clever - empowering - glitzy - glamorous - existential dread - dreamy - judgmental - hopeful</t>
+          <t>- broken - concerning - historically inaccurate - funny - introspective - note-perfect - meaningful - visually gorgeous - complex - big-budget - inspired - existential - postmodernist - liberal feminism - meta jokes - reverse sexism - existential crisis - out there - feminist - jubilant - moving - underdeveloped - self-discovery - vibrant - cheeky - profound - overedited - commercial - authentic - pedantic - messy - try-hard - high concept - clever - fun - toothless - insightful - divisive - spirited - hopeless - inclusive - financial - biting - representationally inclusive - vital - deconstruction - satirical - existential romp - hilarious - heartfelt - feminist - antifeminist - thematic - layered - existential dystopia - nuanced - adult</t>
         </is>
       </c>
       <c r="P17" t="n">
@@ -1873,14 +1873,14 @@
         <v>133</v>
       </c>
       <c r="F18" t="n">
-        <v>4.78</v>
+        <v>4.77</v>
       </c>
       <c r="G18" t="n">
-        <v>0.47</v>
+        <v>0.48</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Parasite is a masterful film that delves into the complexities of class divide and societal issues. With a mix of genres, it keeps viewers on the edge of their seats while delivering a powerful message. The film's unique storytelling and exceptional performances make it a must-see masterpiece that has left audiences in awe.</t>
+          <t>Parasite is a gripping and thrilling film that delves into the complexities of class divide and societal issues. With masterful storytelling and brilliant performances, it keeps the audience on the edge of their seats. The film has been hailed as a masterpiece and a defining work of the decade, showcasing Bong Joon-ho's unique talent for creating genre-defying cinema. The movie is a must-see, offering a thought-provoking and unforgettable viewing experience.</t>
         </is>
       </c>
       <c r="I18" t="n">
@@ -1903,7 +1903,7 @@
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>- house on a hill - garden - underground - con-men - grifters - forgers - imposters - thriller - bloody napkin scene - tent won't leak - morse code - crazy rich asians - garden party - basement - stone - cake - knife - seizure - car-key - sausage skewer - smell - murder - best hook - live orchestra - minimalist architecture - North Korean news anchors - cinephile - best foreign film - best picture - lemons into lemonade - ketchup - pure movie joy - self isolator - nuanced performance - flood scene - smells good - conspiracy - trauma recovery cake - Palme d'Or - best movie - genre-defying - masterpiece - social discrepancy - best of the decade - fate -</t>
+          <t>- house on a hill - garden - underground house - con-men - grifters - forgers - imposters - stink - cum peach - killer peach - high expectations - HOLY FUCK - Min - Mr. Park - laughing - sarcastic - bloody napkin scene - thrilling - Jessica - Illinois Chicago - best hook - live orchestra - minimalist architecture porn - North Korean news anchors - SCREAMING - CRYING - CINEPHILE - foreign film - best picture - lemons into lemonade - ketchup - wonderful - movie joy - self isolator - Academy - small dick - flood scene - smells good - Twitter - conspiracy - trauma recovery cake - Palme d'Or - best movie - genre piece - class relationships - capitalist</t>
         </is>
       </c>
       <c r="P18" t="n">
@@ -1962,7 +1962,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Everything Everywhere All at Once is a visually dazzling, emotionally resonant, and wildly imaginative film that combines martial arts, family drama, and sci-fi elements in a unique and ambitious way. With stellar performances, creative action sequences, and a heartfelt exploration of familial relationships, this movie has left a lasting impact on viewers, sparking discussions and emotional reactions. Despite some divisive opinions, it has been praised for its originality, humor, and thematic depth, making it a standout film of the year.</t>
+          <t>"Everything Everywhere All at Once" is a visually stunning and emotionally resonant film that combines elements of martial arts, sci-fi, comedy, and family drama. With a mix of heartfelt moments and absurd humor, the movie explores themes of multiverses, family relationships, and the meaning of life. Featuring standout performances from the cast, including Michelle Yeoh and Jamie Lee Curtis, the film has been praised for its creativity, originality, and technical prowess. Despite some divisive opinions, many viewers have found it to be a groundbreaking and unforgettable cinematic experience.</t>
         </is>
       </c>
       <c r="I19" t="n">
@@ -1985,7 +1985,7 @@
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>- multiverse madness - heartfelt - visually dazzling - original - creative - funny - emotional - action-packed - ambitious - thought-provoking - Michelle Yeoh - martial arts - family drama - existential - zany - sci-fi - kung fu - Reddit - visually dynamic - moving - imaginative - touching - melancholic - immature - inventive - dense - expansive - wacky - high-concept - sentimental - ridiculous - intellectual - heartfelt - visually dazzling - original - creative - funny - emotional - action-packed - ambitious - thought-provoking - Michelle Yeoh - martial arts - family drama - existential - zany - sci-fi - kung fu - Reddit - visually dynamic - moving - imaginative - touching - melancholic - immature - inventive - dense -</t>
+          <t>- multiverse madness - heartfelt - visually dazzling - creative - funny - original - emotional - ambitious - kinetic - daring - expertly choreographed - action-packed - complex - moving - thought-provoking - authentic - Asian identity - Michelle Yeoh - visionary - masterpiece - symphony of chaos - honest - compassionate - genuine - zany - hilarious - thrilling - beautiful - spiritual - epic - expansive - mind-bending - roller coaster - magic trick - grounded - meaningful - creative - sincere - emotional - familial - resonant - convoluted - relationship - fun - sci-fi - kung fu - Reddit - unbearable - manipulative - ugly - stupid - imbecile - embarrassing - bloated - artificial - sensorial inadequacy - sketchy</t>
         </is>
       </c>
       <c r="P19" t="n">
@@ -2044,7 +2044,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>La La Land is a film that has divided audiences, with some finding it to be a magical and uplifting experience, while others have been left feeling depressed and disappointed. The movie, directed by Damien Chazelle, follows the intertwined lives of Mia, an aspiring actress, and Sebastian, a passionate jazz musician, as they pursue their dreams and navigate their love for each other. The film is praised for its vibrant cinematography, captivating performances by Emma Stone and Ryan Gosling, and mesmerizing musical numbers. Despite its mixed reviews, La La Land continues to be a film that evokes strong emotions and leaves a lasting impact on viewers.</t>
+          <t>La La Land is a film that evokes a wide range of emotions from viewers, from pure magic to deep sadness. It is a celebration of dreams and love, set against the backdrop of Los Angeles. The film follows the intertwined lives of Mia, an aspiring actress, and Sebastian, a passionate jazz musician. With captivating performances, mesmerizing musical numbers, and vibrant cinematography, La La Land is a cinematic gem that leaves a lasting impact on those who watch it. Despite its bittersweet ending, the film continues to be a favorite for many, invoking feelings of joy, nostalgia, and heartbreak.</t>
         </is>
       </c>
       <c r="I20" t="n">
@@ -2057,7 +2057,7 @@
         <v>9</v>
       </c>
       <c r="L20" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M20" t="n">
         <v>8</v>
@@ -2067,7 +2067,7 @@
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>- enchanting - charming - magical - emotional - bittersweet - impactful - mesmerizing - captivating - vibrant - celebratory - exuberant - electrifying - tender - romantic - heartbreaking - awe-inspiring - sublime - bold - rewarding - difficult - beautiful - triumphant - dreamy - nostalgic - hopeful - bittersweet - flawless - stunning - amazing - enchanting - charming - joyous - celebratory - golden age - contemporary - joy - love - passion - dream - sacrifice - whimsical - whimsy - musical - comedy - dramedy - cinema - art - masterpiece - magic - dreamlike - nostalgic - vibrant - colorful - energetic - emotional - heartfelt - mesmerizing - captivating - breathtaking - dazzling - romantic - inspiring - impactful</t>
+          <t>- magical - emotional - impactful - bittersweet - mesmerizing - romantic - nostalgic - vibrant - celebratory - joyous - melancholic - captivating - enchanting - triumphant - dreamy - hopeful - dramedy - tragic - catchy - flawless - stunning - amazing - emotional - beautiful - flawless - stunning - amazing - celebratory - joyous - melancholic - captivating - enchanting - triumphant - dreamy - hopeful - emotional - beautiful - flawless - stunning - amazing - celebratory - joyous - melancholic - captivating - enchanting - triumphant - dreamy - hopeful - emotional - beautiful - flawless - stunning - amazing - celebratory - joyous - melancholic - captivating - enchanting - triumphant - dreamy -</t>
         </is>
       </c>
       <c r="P20" t="n">
@@ -2126,30 +2126,30 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Knives Out is a clever and entertaining murder mystery film with a stellar cast, led by Daniel Craig and Ana de Armas. The script is sharp and funny, with standout performances from the ensemble cast. The film subverts expectations and keeps the audience engaged throughout. Overall, it's a must-watch for fans of the genre and a crowd-pleaser that delivers on all fronts.</t>
+          <t>Knives Out is a clever and entertaining murder mystery film with a stellar cast, led by the brilliant Ana de Armas. The movie is filled with humor, suspense, and unexpected twists, making it a crowd-pleaser that keeps audiences engaged. Daniel Craig's performance as Benoit Blanc is a standout, and the film's unique take on the genre is refreshing. Overall, Knives Out is a must-watch for fans of whodunnit films and offers a fun and enjoyable viewing experience.</t>
         </is>
       </c>
       <c r="I21" t="n">
         <v>9</v>
       </c>
       <c r="J21" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="K21" t="n">
         <v>10</v>
       </c>
       <c r="L21" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="M21" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="N21" t="n">
         <v>9</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>- clever - funny - entertaining - ensemble - mystery - whodunnit - Daniel Craig - Ana de Armas - Chris Evans - Rian Johnson - donut - cozy - ensemble cast - twist - humor - original - engaging - suspenseful - intricate - modern - self-aware - crowd-pleaser - commentary - meta - brilliant - captivating - homage - masterful - memorable - tight script - human decency - special - favorite - rewatchable - mad genius - perfect - RIP Christopher Plummer</t>
+          <t>- clever - funny - entertaining - ensemble - mystery - detective - donut - cozy - twist - original - whodunnit - cast - Daniel Craig - Ana de Armas - Chris Evans - Michael Shannon - Toni Collette - Jamie Lee Curtis - Rian Johnson - humor - suspense - thriller - modern - homage - nostalgia - family - dark comedy - ensemble cast - brilliant - engaging - intricate - plot twists - memorable - dialogue - cinematography - commentary - rewatchable - favorite - masterpiece - iconic - classic - must-watch - cleverly-written - stellar - captivating - engaging - crowd-pleaser - fun - hilarious - charming - suspenseful - brilliant screenplay - exceptional - unique - refreshing - brilliant performances - dynamic - layered - intriguing -</t>
         </is>
       </c>
       <c r="P21" t="n">
@@ -2208,7 +2208,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Joker is a divisive film that has been both praised and criticized. Some viewers found it to be a bold reinvention of superhero cinema, while others felt it was a shallow and pretentious attempt at social commentary. Joaquin Phoenix's performance as Arthur Fleck/Joker has been widely acclaimed, but the film's handling of mental illness and societal issues has been a point of contention. Overall, Joker has sparked discussions about its themes, style, and impact on audiences.</t>
+          <t>- Joker is a divisive film that has been praised for Joaquin Phoenix's performance and visual elements, but criticized for its lack of depth, handling of mental illness, and political themes. It is seen as a bold reinvention of superhero cinema, but also as a toxic rallying cry for incels. The film has been compared to other works like Taxi Driver and The King of Comedy, with some viewers finding it provocative and others finding it pretentious and shallow. Overall, opinions on Joker vary widely, with some praising it as a masterpiece and others dismissing it as overrated and lacking substance.</t>
         </is>
       </c>
       <c r="I22" t="n">
@@ -2231,7 +2231,7 @@
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>- vapid - shallow - disappointing - predictable - hollow - misguided - pretentious - controversial - unsettling - disturbing - nihilistic - grim - violent - intense - chilling - fascinating - remarkable - fascinating - unsettling - remarkable - interesting - cinema - crime thriller - visually stunning - chilling music - intense - remarkable - fascinating - unsettling - remarkable - fascinating - unsettling - remarkable - fascinating - unsettling - remarkable - fascinating - unsettling - remarkable - fascinating - unsettling - remarkable - fascinating - unsettling - remarkable - fascinating - unsettling - remarkable - fascinating - unsettling - remarkable - fascinating - unsettling - remarkable - fascinating - unsettling - remarkable - fascinating - unsettling - remarkable - fascinating - unsettling - remarkable - fascinating - unsettling - remarkable - fascinating - unsettling - remarkable - fascinating - unsettling - remarkable</t>
+          <t>- vapid - shallow - disappointing - predictable - hollow - misguided - pretentious - controversial - unsettling - grim - nihilistic - intense - chilling - remarkable - fascinating - fascinating - interesting - cinema - crime thriller - visually stunning - impressive - remarkable - captivating - intriguing - unsettling - intense - disappointing - predictable - shallow - hollow - misguided - pretentious - controversial - unsettling - grim - nihilistic - intense - chilling - remarkable - fascinating - fascinating - interesting - cinema - crime thriller - visually stunning - impressive - remarkable - captivating - intriguing - unsettling - intense - disappointing - predictable - shallow - hollow - misguided - pretentious - controversial - unsettling - grim - nihilistic - intense - chilling - remarkable - fascinating - fascinating - interesting - cinema - crime thriller</t>
         </is>
       </c>
       <c r="P22" t="n">
@@ -2290,30 +2290,30 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Pulp Fiction is a cult classic that has left a lasting impact on cinema history. With its sharp dialogue, colorful characters, and unique storytelling, Quentin Tarantino's masterpiece continues to captivate audiences. The film is a mix of different genres, filled with important life lessons and iconic moments. While some viewers may find it overrated or boring, others praise it as a bona-fide landmark in cinematic history. The movie is known for its memorable characters, witty dialogue, and interconnected storylines that come together in a masterpiece of filmmaking. Ultimately, Pulp Fiction remains a must-watch for cinephiles and casual viewers alike.</t>
+          <t>Pulp Fiction is a cult classic that has left a lasting impact on cinema history. With its sharp dialogue, colorful characters, and unique storytelling, Quentin Tarantino's masterpiece continues to captivate audiences. The film is a mix of different genres, filled with important life lessons and iconic moments. While some viewers may find it overrated or boring, others praise it as a bona-fide landmark in cinematic history. Mia Wallace's character steals the show for many, with her dancing, milkshake-drinking, and overall presence. Despite mixed reviews, Pulp Fiction remains a must-watch for cinephiles and casual viewers alike.</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J23" t="n">
+        <v>0</v>
+      </c>
+      <c r="K23" t="n">
+        <v>7</v>
+      </c>
+      <c r="L23" t="n">
+        <v>0</v>
+      </c>
+      <c r="M23" t="n">
         <v>6</v>
       </c>
-      <c r="K23" t="n">
-        <v>8</v>
-      </c>
-      <c r="L23" t="n">
-        <v>7</v>
-      </c>
-      <c r="M23" t="n">
-        <v>8</v>
-      </c>
       <c r="N23" t="n">
         <v>9</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>- iconic - dialogue-driven - interconnected - cult classic - masterpiece - groundbreaking - original - memorable characters - dark humor - pop culture references - witty - Quentin Tarantino - Samuel L. Jackson - Uma Thurman - John Travolta - nonlinear narrative - kaleidoscopic - brilliant screenplay - rewatchable - classic - influential - Tarantino-esque - quotable - genius - electrifying - thought-provoking - reflection - iconic scenes - cult following - legendary - cinematic history - unique - edgy - darkly comedic - ensemble cast - interconnected storylines - non-linear storytelling - witty dialogue - memorable quotes - masterstroke - brilliant humor - character-driven - impactful - timeless - influential - iconic moments - unforgettable - cinematic landmark - brilliant writing - sharp dialogue -</t>
+          <t>- iconic - groundbreaking - witty - dialogue-driven - interconnected - cult classic - masterpiece - original - memorable characters - pop culture references - dark humor - violent - Quentin Tarantino - Samuel L. Jackson - John Travolta - Uma Thurman - Bruce Willis - Ving Rhames - nonlinear narrative - kaleidoscopic - brilliant screenplay - iconic quotes - rewatchable - classic - cinematic history - influential - unique - Tarantino style - character-driven - intense - clever - edgy - stylish - engaging - entertaining - quotable - genius - thought-provoking - non-linear storytelling - masterstroke - electrifying - feast - frequent consumption - legendary - impactful - unforgettable - must-watch - timeless - brilliant humor - interconnected stories - iconic scenes - cultural impact</t>
         </is>
       </c>
       <c r="P23" t="n">
@@ -2372,7 +2372,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>The Batman is a dark, gritty, and visually stunning film that showcases a unique portrayal of Bruce Wayne as a disturbed and gothic figure. The movie delves into the detective side of Batman, with a focus on clues and investigation. The Riddler is portrayed as a twitch streamer, adding a modern twist to the character. The film has been praised for its atmospheric cinematography, haunting score, and standout performances from Robert Pattinson, Zoe Kravitz, and Paul Dano. Overall, The Batman is seen as a refreshing take on the superhero genre, blending elements of noir, thriller, and crime drama to create a compelling and immersive experience.</t>
+          <t>The Batman is a dark, gritty, and visually stunning film that showcases a unique portrayal of Bruce Wayne as a disturbed and gothic figure. The movie delves into Batman's detective skills and features a standout performance by Robert Pattinson. With influences from films like Se7en and Zodiac, The Batman offers a fresh take on the superhero genre with a focus on character development and style. Despite its lengthy runtime, the film is praised for its immersive storytelling and masterful technical achievements. The Riddler is portrayed as a twisted and creepy character, while Catwoman adds a touch of badassery. Overall, The Batman is considered a standout entry in the Batman franchise and a must-watch for fans of the character.</t>
         </is>
       </c>
       <c r="I24" t="n">
@@ -2395,7 +2395,7 @@
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>- disgusting - goth - emo - detective - sexy - gay - hilarious - thrilling - dark - gritty - violent - brooding - immersive - noir - masterpiece - engrossing - engrossing - engrossing - engrossing - engrossing - engrossing - engrossing - engrossing - engrossing - engrossing - engrossing - engrossing - engrossing - engrossing - engrossing - engrossing - engrossing - engrossing - engrossing - engrossing - engrossing - engrossing - engrossing - engrossing - engrossing - engrossing - engrossing - engrossing - engrossing - eng</t>
+          <t>- disgusting - goth - detective - virgin - fantastic - sexy - emo - silly - gay - hilarious - twitch streamer - studied in film school - bangs - haunting - sex for the eyes - bold - pacing issues - Zodiac - Se7en - Saw - mesmerizing - gotham city - brooding - immersive - noir - masterful - conflicted - stunning - dark - gritty - terrifying - breathtaking - chilling - stunning - atmospheric - psychological - unforgettable - immersive - complex - visionary - interesting - intricate - best batman movie - fine - conflicted - brooding - hot - horny - silly - sexy - boring - thriller - crime - detective - sexy - Spanish - vengeance - transformation - hope - endurance - fight - metamorphism</t>
         </is>
       </c>
       <c r="P24" t="n">
@@ -2454,30 +2454,30 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Knives Out is a clever and entertaining murder mystery film with a stellar cast, led by Daniel Craig and Ana de Armas. The script is sharp and funny, with standout performances from the ensemble cast. The film subverts expectations and keeps the audience engaged throughout. Overall, it's a must-watch for fans of the genre and a crowd-pleaser that delivers on all fronts.</t>
+          <t>Knives Out is a clever and entertaining murder mystery film with a stellar cast, led by Daniel Craig and Ana de Armas. The script is sharp and funny, with standout performances from the ensemble cast. The film subverts expectations and keeps the audience engaged throughout. Overall, it's a must-watch for fans of the genre and those looking for a fun and engaging movie experience.</t>
         </is>
       </c>
       <c r="I25" t="n">
         <v>9</v>
       </c>
       <c r="J25" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="K25" t="n">
         <v>10</v>
       </c>
       <c r="L25" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="M25" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="N25" t="n">
         <v>9</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>- clever - funny - entertaining - ensemble - mystery - whodunnit - donut - cozy - Daniel Craig - Ana de Armas - Chris Evans - Rian Johnson - ensemble cast - twist - humor - detective - family - suspense - original - homage - meta - dialogue - cinematography - commentary - rewatchable - favorite - masterpiece - brilliant - engaging - crowd-pleaser - memorable - twisty - cleverly-written - stellar - captivating - exceptional - special - unique - thrilling - satisfying - modern - classic - homage - homage - homage - homage - homage - homage - homage - homage - homage - homage - homage - homage - homage - homage - homage - homage - homage - homage - homage - homage - homage - homage -</t>
+          <t>- clever - funny - entertaining - ensemble cast - whodunnit - mystery - donut monologue - Daniel Craig - Ana de Armas - Chris Evans - Rian Johnson - twists - family dynamics - cozy - suspenseful - modern twist - original - engaging - crowd-pleaser - dark humor - clever screenplay - ensemble film - brilliant performances - memorable characters - intricate plot - masterclass - homage to classic mysteries - human decency - compassion - meta - self-aware - quotable - rewatchable - favorite - special - unique - brilliant - genius - iconic - memorable - stellar - exceptional - masterpiece - thrilling - satisfying - twisty - hilarious - charming - captivating - intriguing - cleverly-constructed - surprising - delightful - fun - cozy -</t>
         </is>
       </c>
       <c r="P25" t="n">
@@ -2536,7 +2536,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>The Dark Knight is hailed as the best superhero movie ever made, with Heath Ledger's performance as the Joker being a standout. The film is praised for its intense action sequences, complex characters, and thought-provoking themes. Despite some flaws, it remains a cinematic masterpiece that continues to captivate audiences.</t>
+          <t>The Dark Knight is hailed as the best superhero movie ever made, with Heath Ledger's performance as the Joker being a standout. The film is considered a masterpiece, with intense action sequences and a dark, realistic approach to the Batman story. Despite some flaws, it remains a cultural landmark and a game-changer in the superhero genre. Ledger's portrayal of the Joker is unforgettable, elevating the film to legendary status. Overall, The Dark Knight is a thrilling and thought-provoking cinematic experience that continues to captivate audiences.</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2546,20 +2546,20 @@
         <v>8</v>
       </c>
       <c r="K26" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L26" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="M26" t="n">
         <v>9</v>
       </c>
       <c r="N26" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>- masterpiece - best superhero movie - heath ledger - iconic - thrilling - intense - game-changer - influential - cinematic excellence - unforgettable - riveting - exhilarating - homoerotic tension - brilliant - thought-provoking - nihilistic - poetic - masterful - cultural landmark - intense thriller - realistic - dark - flawless - action-packed - perfection - dense - serious - dark and realistic - mature storytelling - triumph - unmatched - iconic villain - legendary - intense action - dark and gritty - impactful - unforgettable performance - cinematic history - phenomenal - genius - timeless - classic - epic - influential - masterpiece - thrilling - intense - iconic - unforgettable - riveting - exhilarating - brilliant - thought-provoking - masterful - cultural landmark - intense thriller -</t>
+          <t>- masterpiece - heath ledger - iconic - thrilling - intense - superhero - influential - game-changer - cinematic excellence - unforgettable - dark - realistic - complex - deep - Heath Ledger's Joker - Christopher Nolan - Hans Zimmer - Christian Bale - Cillian Murphy - action-packed - suspenseful - Joker's chaos - Batman's heroism - morally complex - iconic quotes - cultural landmark - nihilistic - brilliant - disturbing - Joker's impact - intense thriller - best chase sequence - phenomenal - emotional impact - flawless action - tense - serious - dense - masterpiece - best Batman movie - best superhero movie - best sequel - favorite movie - unforgettable - dark knight - watchful protector - silent guardian - realistic - mature storytelling - triumph - iconic - thrilling - intense - superhero</t>
         </is>
       </c>
       <c r="P26" t="n">
@@ -2611,14 +2611,14 @@
         <v>133</v>
       </c>
       <c r="F27" t="n">
-        <v>4.78</v>
+        <v>4.77</v>
       </c>
       <c r="G27" t="n">
-        <v>0.47</v>
+        <v>0.48</v>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Parasite is a masterful film that delves into the complexities of class divide and societal issues. With a mix of genres, it keeps viewers on the edge of their seats while delivering a powerful message. The film has been praised for its exceptional storytelling, brilliant performances, and thought-provoking themes. It has been hailed as a masterpiece and a must-see for all movie lovers.</t>
+          <t>Parasite is a gripping and thrilling film that delves into the complexities of class divide and societal issues. With masterful storytelling and brilliant performances, it keeps the audience on the edge of their seats. The film has been hailed as a masterpiece and a defining work of the decade, showcasing Bong Joon-ho's unique talent for creating genre-defying cinema. The movie is both entertaining and thought-provoking, leaving a lasting impact on viewers.</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -2628,10 +2628,10 @@
         <v>7</v>
       </c>
       <c r="K27" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="L27" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M27" t="n">
         <v>9</v>
@@ -2641,7 +2641,7 @@
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>- house on a hill - garden - sunlight - house underground - con-men - grifters - forgers - imposters - stink - cum peach - killer peach - high expectations - HOLY FUCK - Min - Mr. Park - romantic relationships - powerful figures - dismissive - bloody napkin scene - top 3 scenes - thrilling - Jessica - Illinois Chicago - cousin - best hook - live orchestra - minimalist architecture porn - North Korean news anchors - rare compliment - SCREAMING - CRYING - CINEPHILE - foreign film - BEST PICTURE - Bong - lemons into lemonade - eating the rich - ketchup - wonderful couple of hours - self isolator - Academy - small dick - peach - nuanced performance - emotional</t>
+          <t>- gripping - thrilling - suspenseful - darkly comedic - thought-provoking - genre-defying - masterful - social commentary - class warfare - intense - twisty - satirical - nuanced - impactful - mesmerizing - engaging - unique - brilliant - cinematic masterpiece - must-see - unforgettable - powerful - compelling - layered - shocking - anxiety-inducing - edge-of-your-seat - jaw-dropping - batshit crazy - depressing - incredible - fun - gripping - thought-provoking - genre-defying - masterful - social commentary - intense - satirical - impactful - mesmerizing - engaging - unique - brilliant - cinematic masterpiece - must-see - unforgettable - powerful - compelling - layered - shocking - anxiety-inducing - edge-of-your-seat -</t>
         </is>
       </c>
       <c r="P27" t="n">
@@ -2700,7 +2700,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Fight Club is a divisive film that has been viewed in various ways by different audiences. Some see it as the best movie ever made, while others view it as a critique of toxic masculinity. The film explores themes of consumerism, masculinity, and identity, with some viewers finding it deep and thought-provoking, while others see it as overrated. The character of Tyler Durden has become iconic, with some even considering him a fashion icon. Overall, Fight Club remains a complex and intriguing film that continues to spark discussion and debate among viewers.</t>
+          <t>Fight Club is a divisive film that has been viewed in various ways by different audiences. Some see it as the best movie ever made, while others view it as a critique of toxic masculinity. The film explores themes of consumerism, masculinity, and identity, with some viewers finding it deep and thought-provoking, while others see it as overrated and misunderstood. The character of Tyler Durden has become a fashion icon, and the film has sparked discussions about its homoerotic subtext. Overall, Fight Club remains a complex and intriguing film that continues to provoke discussion and debate among viewers.</t>
         </is>
       </c>
       <c r="I28" t="n">
@@ -2723,7 +2723,7 @@
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>- masterpiece - toxic masculinity - satire - gay - imaginary friend - Brad Pitt - Tyler Durden - homoerotic subtext - cult film - misunderstood - consumerism - societal critique - Fincher - twist - self-destruction - iconic - dark - immersive - cinematography - performances - narrative - atmosphere - complex - edgy - favorite - comfort movie - archetype - profound - plot - stylish - flawless - direction - dark humor - societal commentary - modern classic - cinematic art</t>
+          <t>- masterpiece - commentary - toxic masculinity - satire - gay - imaginary friend - hallucination - insomnia - soap - jared leto - fashion icon - queer - violence - misunderstood - overrated - cult - satire - consumerism - masculinity - psychological - twist - propaganda - end scene - top 100 - perfectionist - archetype - comfort movie - dark - immersive - atmospheric</t>
         </is>
       </c>
       <c r="P28" t="n">
@@ -2782,7 +2782,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>La La Land is a film that has divided audiences, with some finding it to be a magical and uplifting experience, while others have been left feeling depressed and disappointed. The movie, directed by Damien Chazelle, follows the intertwined lives of Mia, an aspiring actress, and Sebastian, a passionate jazz musician, as they navigate their dreams and love in the vibrant backdrop of Los Angeles. With captivating performances by Emma Stone and Ryan Gosling, mesmerizing musical numbers, and stunning cinematography, La La Land is a celebration of art, dreams, and the complexities of relationships. Despite its flaws and criticisms, the film continues to evoke strong emotions and remains a favorite for many viewers.</t>
+          <t>La La Land is a film that evokes a wide range of emotions from viewers, from pure magic to deep sadness. It is a celebration of dreams and love, set against the backdrop of Los Angeles. The film follows the intertwined lives of Mia, an aspiring actress, and Sebastian, a passionate jazz musician. With captivating performances, mesmerizing musical numbers, and vibrant cinematography, La La Land is a cinematic gem that leaves a lasting impact on those who watch it. Despite some criticisms, the film continues to be praised for its beauty and emotional depth.</t>
         </is>
       </c>
       <c r="I29" t="n">
@@ -2795,7 +2795,7 @@
         <v>9</v>
       </c>
       <c r="L29" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M29" t="n">
         <v>8</v>
@@ -2805,7 +2805,7 @@
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>- enchanting - charming - magical - bittersweet - emotional - impactful - mesmerizing - captivating - vibrant - celebratory - nostalgic - romantic - bold - rewarding - joyous - breathtaking - electric - sublime - masterful - beautiful - triumphant - dreamy - hopeful - tragic - catchy - flawless - stunning - amazing - enchanting - charming - golden age - contemporary - joy - blissful</t>
+          <t>- magical - emotional - bittersweet - impactful - joyous - melancholic - romantic - nostalgic - mesmerizing - captivating - celebratory - vibrant - enchanting - triumphant - dreamy - hopeful - dramedy - tragic - catchy - beautiful - flawless - stunning - amazing - incredible - goddamn - flawless - stunning - amazing - incredible - celebratory - vibrant - enchanting - triumphant - dreamy - hopeful - mesmerizing - captivating - celebratory - vibrant - enchanting - triumphant - dreamy - hopeful - mesmerizing - captivating - celebratory - vibrant - enchanting - triumphant - dreamy - hopeful - mesmerizing - captivating - celebratory - vibrant - enchanting - triumphant - dreamy - hopeful -</t>
         </is>
       </c>
       <c r="P29" t="n">
@@ -2864,7 +2864,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Interstellar is a visually stunning and emotionally heavy film that explores themes of love, time, and survival. The movie follows a team of explorers traveling through a wormhole in space to ensure humanity's survival. With a mix of awe-inspiring visuals, a powerful score, and strong performances, the film takes viewers on a breathtaking journey through time and space. While some viewers found it to be a masterpiece and a cinematic achievement, others criticized its over-explanation and plot inconsistencies. Overall, Interstellar is a thought-provoking and ambitious film that leaves a lasting impact on its audience.</t>
+          <t>Interstellar is a visually stunning and emotionally heavy film that explores themes of love, time, and the unknown. The movie follows Cooper, played brilliantly by Matthew McConaughey, on a journey through space to ensure humanity's survival. The film has received mixed reviews, with some praising its ambition and technical execution, while others criticize its writing and plot. Overall, Interstellar is a cinematic masterpiece that leaves a lasting impact on viewers.</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -2887,7 +2887,7 @@
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>- emotional - visually stunning - ambitious - masterpiece - thought-provoking - space opera - family drama - breathtaking - powerful - science-fiction - rollercoaster - intense - epic - profound - awe-inspiring - transcendent - beautifully shot - heartbreaking - compelling - ambitious - visually monumental - mind-enriching - captivating - immersive - intense - overwhelming - awe-inspiring - stunning - masterclass - mesmerizing - jaw-dropping - euphoric - cosmic - transcendent - poetic - complex - intricate - challenging - muddled - aggravating - phenomenal - forgiveness - perfection</t>
+          <t>- emotional - visually stunning - ambitious - cathartic - intense - thought-provoking - masterpiece - sci-fi - space exploration - love transcends time - visually breathtaking - rollercoaster - epic - Hans Zimmer score - family drama - human odyssey - profound - science-fantasy - ambitious storytelling - visually spectacular - emotional journey - awe-inspiring - complex - overwhelming - cosmic awe - muddled - aggravating - conflict between science and faith - intense performances - mind-bending - visually stunning - phenomenal - forgiveness - unforgettable - captivating - transcendent - poetic - perfection</t>
         </is>
       </c>
       <c r="P30" t="n">
@@ -2946,7 +2946,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Oppenheimer is a visually stunning and technically masterful film that explores the life of J. Robert Oppenheimer, the father of the atomic bomb. Christopher Nolan's direction creates a complex narrative structure that keeps the audience engaged. Cillian Murphy delivers a mesmerizing performance, while Robert Downey Jr. and Emily Blunt shine in their supporting roles. The film's immersive sound design and score add to the intense experience. Despite some mixed reviews, Oppenheimer is seen as a significant achievement in filmmaking.</t>
+          <t>Oppenheimer is a visually stunning and technically masterful film that explores the life of J. Robert Oppenheimer, the father of the atomic bomb. Christopher Nolan's direction immerses the audience in a complex narrative that jumps between timelines, with standout performances from Cillian Murphy and Robert Downey Jr. The film delves into themes of morality, bureaucracy, and the consequences of scientific discovery. While some find it to be Nolan's best work to date, others criticize its length and pacing. Overall, Oppenheimer is a thought-provoking and intense cinematic experience that leaves a lasting impact on viewers.</t>
         </is>
       </c>
       <c r="I31" t="n">
@@ -2969,7 +2969,7 @@
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>- atomic - immersive - heart-pounding - stud - Best Supporting Actor - score - sound design - nuclear - ridiculous - josh peck - cigarettes - JFK - bone structure - IMAX - happy - funny - Rodrick Rules - communist - intense - harrowing - dense - psychological - personal - grand - moral - cosmic - mature - ambiguous - surreal - subjective - sublime - visual spectacle - soundscape - epic - awe-inspiring - masterclass - technical marvel - historical terror - moral torment - Oscar-worthy - mesmerizing - captivating - breathtaking - profound - beautiful - terrifying - surreal - experimental - surrealist - sublime - introspective - twisty - complex - monumental - speechless - electric - immersive - ambitious - clinical - emotional - insecure -</t>
+          <t>- atomic - immersive - heart-pounding - stud - best supporting actor - score - sound design - nuclear - funny - summer blockbuster - Rodrick Rules - communist - harrowing - psychological - dense - intense - anxiety - dread - master class - filmmaking - visually stunning - awe-inspiring - moral torment - Oscar-worthy - cinematography - thunderous sound - intricate editing - magnificent score - character study - breathtaking - epic visuals - personal - surreal - subjective - experimental - visually stunning - aesthetic masterclass - sublime - personal - technical master - clinical - emotional - insecure</t>
         </is>
       </c>
       <c r="P31" t="n">
@@ -3021,14 +3021,14 @@
         <v>125</v>
       </c>
       <c r="F32" t="n">
-        <v>4.76</v>
+        <v>4.75</v>
       </c>
       <c r="G32" t="n">
-        <v>0.49</v>
+        <v>0.5</v>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Spirited Away is a visually stunning and emotionally resonant masterpiece that captivates viewers with its magical world and rich storytelling. The film follows the journey of a young girl named Chihiro as she navigates a mysterious and fantastical realm filled with gods, witches, and spirits. Through themes of courage, growth, and empathy, Spirited Away explores the power of love and the importance of kindness in the face of adversity. With its intricate animation, memorable characters, and enchanting soundtrack, Spirited Away is hailed as one of the best animated films of all time, leaving a lasting impact on audiences of all ages.</t>
+          <t>Spirited Away is a visually stunning and emotionally resonant masterpiece that captivates viewers with its magical world and rich storytelling. The film follows the journey of Chihiro, a young girl who finds herself in a mysterious and fantastical realm filled with gods, witches, and spirits. As Chihiro navigates this strange world, she learns valuable lessons about courage, empathy, and the power of kindness. With its imaginative animation, memorable characters, and universal themes, Spirited Away has earned its reputation as one of the best animated films of all time.</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -3051,7 +3051,7 @@
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>- magical - immersive - masterpiece - imaginative - visually stunning - emotional - transformative - enchanting - whimsical - nostalgic - captivating - beautiful - mesmerizing - fantastical - thought-provoking - timeless - intricate - detailed - rich - unique - charming - bittersweet - melancholic - legendary - creative - original - awe-inspiring - cinematic poetry - heartwarming - powerful - moving - profound - universal - ethereal - whimsy - surreal - unforgettable - whimsical - dreamlike - enchantment - mesmerizing - captivating - charming - delightful - heartwarming - magical realism - fantastical journey - emotional depth - visually breathtaking - imaginative storytelling - masterful craftsmanship - cultural exploration - thematic richness - character development - moral lessons - spiritual growth -</t>
+          <t>- magical - immersive - transformative - visually stunning - emotional - imaginative - masterpiece - enchanting - nostalgic - whimsical - captivating - profound - beautiful - mesmerizing - fantastical - rich - intricate - detailed - unique - creative - thought-provoking - charming - touching - powerful - moving - legendary - iconic - timeless - universal - ethereal - surreal - whimsy - depth - depth - depth - depth - depth - depth - depth - depth - depth - depth - depth - depth - depth - depth - depth - depth - depth - depth - depth - depth - depth - depth - depth - depth - depth - depth - depth - depth - depth - depth - depth - depth - depth - depth - depth - depth - depth - depth</t>
         </is>
       </c>
       <c r="P32" t="n">
@@ -3110,7 +3110,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Ratatouille is a heartwarming Pixar film about a talented rat named Remy who dreams of becoming a chef. The movie explores themes of passion, identity, and the pursuit of one's dreams. With stunning animation, a charming Parisian setting, and a memorable score by Michael Giacchino, Ratatouille is considered by many to be one of Pixar's best films. The story follows Remy's journey as he navigates the culinary world, proving that anyone can achieve greatness, regardless of their background. The film's emotional moments, lovable characters, and messages of perseverance make it a timeless classic that continues to resonate with audiences.</t>
+          <t>Ratatouille is a heartwarming Pixar film about a talented rat named Remy who dreams of becoming a chef. The movie explores themes of passion, identity, and the pursuit of dreams. With stunning animation, a charming Parisian setting, and a memorable score by Michael Giacchino, Ratatouille is considered by many to be one of Pixar's best films. The story follows Remy's journey as he navigates the culinary world, proving that anyone can achieve greatness, regardless of their background. The film's emotional moments, lovable characters, and messages of perseverance make it a timeless classic that continues to resonate with audiences.</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -3133,7 +3133,7 @@
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>- ratatouille - masterpiece - heartwarming - inspirational - paris - cooking - chef - dream - passion - animation - Pixar - emotional - favorite - comfort - creative - genius - culinary - artistry - friendship - charming - delightful - magical - beautiful - score - talented - dreamer - success - perseverance - nostalgia - classic - rewatchable - funny - lovable - unique - cinematic - storytelling - imaginative - creative - visually stunning - enchanting - soulful - touching - memorable - impactful - brilliant - underrated - underrated - underrated</t>
+          <t>- heartwarming - inspirational - comedic - emotional - culinary - Parisian - animated - masterpiece - rewatchable - thought-provoking - charming - delightful - creative - nostalgic - visually stunning - lovable characters - relatable - touching - magical - genius - captivating - enchanting - feel-good - iconic - memorable - cinematic - impactful - profound - entertaining - heartening - artistic - heartening - ASMR-inducing - comforting - classic - revolutionary - powerful - resonant - beautiful - engaging - dynamic - witty - imaginative - soulful - moving - brilliant - unique - whimsical - endearing - heartening - exceptional - extraordinary - impressive - heartwarming - heartwarming - heartwarming - heartwarming - heartwarming</t>
         </is>
       </c>
       <c r="P33" t="n">
@@ -3192,7 +3192,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Fantastic Mr. Fox is a stop-motion puppet animation film directed by Wes Anderson that has received high praise from viewers. The film features a star-studded cast including George Clooney, Willem Dafoe, and Meryl Streep. Viewers have highlighted the unique characters, quirky dialogue, and vibrant visuals of the film. Many have expressed their love for the movie, calling it a masterpiece and a feel-good experience. The film is described as a heist movie for furries, with elements of humor, charm, and heartwarming moments. Overall, Fantastic Mr. Fox is considered a standout film in Wes Anderson's filmography and a must-watch for animation fans.</t>
+          <t>Fantastic Mr. Fox is a stop-motion puppet animation film directed by Wes Anderson that follows the story of Mr. Fox, voiced by George Clooney, as he assembles a team for elaborate heists. The film features a diverse group of characters, including a tall alcoholic rat voiced by Willem Dafoe. With vibrant colors, quirky dialogue, and a heartwarming story about family, this movie is a unique and visually stunning masterpiece that has captivated audiences with its charm and humor.</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -3215,7 +3215,7 @@
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>- stop-motion - animation - Wes Anderson - quirky - charming - heist - furry - colorful - unique - dialogue - Willem Dafoe - George Clooney - family - feel-good - perfection - vibrant - intricate - heartwarming - iconic - existential - visual - art - fantastic - humor - rewatchable - happy ending - fall season - existential crisis - different - vibrant - joyful - mesmerizing - masterpiece - genius - distinctive - innovative - universal themes - vibrant colors - intricate world - emotional beats - star power - intimate - surreal - surreal - surreal - surreal - surreal - surreal - surreal - surreal - surreal - surreal - surreal - surreal - surreal - surreal - surreal - surreal - surreal - surreal - surreal - surreal - surreal -</t>
+          <t>- stop-motion - animation - Wes Anderson - quirky - charming - heist - furry - vibrant - colorful - unique - feel-good - dialogue - humor - Wes Anderson style - perfection - iconic - George Clooney - Willem Dafoe - family - heartwarming - existential - visual - intricate - art - different - fantastic - fall season - rewatchable</t>
         </is>
       </c>
       <c r="P34" t="n">
@@ -3267,14 +3267,14 @@
         <v>95</v>
       </c>
       <c r="F35" t="n">
-        <v>4.4</v>
+        <v>4.41</v>
       </c>
       <c r="G35" t="n">
-        <v>0.65</v>
+        <v>0.63</v>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Inside Out is a groundbreaking Pixar film that delves into the complexities of emotions within an 11-year-old girl's mind. With a unique concept and heartfelt storytelling, it explores the importance of balance between joy and sadness. The film resonates with audiences of all ages, offering a deep understanding of the human experience and the significance of emotional intelligence. With memorable characters like Bing Bong and a touching message about the value of all emotions, Inside Out is a true masterpiece that leaves a lasting impact on viewers.</t>
+          <t>Inside Out is a deeply emotional and visually stunning masterpiece from Pixar, exploring the complexities of human emotions through the lens of an 11-year-old girl's mind. The film delves into the importance of balance between joy and sadness, delivering a powerful message about the necessity of all emotions in life. With a unique concept and heartfelt storytelling, Inside Out resonates with audiences of all ages, making it a standout in Pixar's impressive filmography.</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3297,7 +3297,7 @@
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>- emotional - heartwarming - innovative - creative - insightful - touching - nostalgic - existential - complex - visually stunning - empathetic - funny - original - masterpiece - balanced - relatable - educational - entertaining - magical - beautiful - iconic - iconic - iconic - iconic - iconic - iconic - iconic - iconic - iconic - iconic - iconic - iconic - iconic - iconic - iconic - iconic - iconic - iconic - iconic - iconic - iconic - iconic - iconic - iconic - iconic - iconic - iconic - iconic - iconic - iconic - iconic - iconic - iconic - iconic - iconic - iconic - iconic - iconic - iconic - iconic - iconic - iconic - iconic - iconic - iconic - iconic - iconic - iconic - iconic - iconic - iconic - iconic -</t>
+          <t>- emotional - heartwarming - innovative - creative - insightful - touching - relatable - nostalgic - profound - existential - iconic - deep - beautiful - vibrant - likable - well-written - unique - magical - existential - complex - empathetic - funny - entertaining - original - visually stunning - masterpiece - visually scrumptious - expansive metaphor - complex storytelling - unpredictable resolution - emotional terrorism - comforting - heartbreaking - relatable - insightful - profound - existential - beautiful - vibrant - emotional - heartwarming - touching - relatable - nostalgic - insightful - profound - existential - emotional - heartwarming - touching - relatable - nostalgic - insightful - profound - existential - emotional - heartwarming - touching - relatable - nostalgic - insightful - profound - existential</t>
         </is>
       </c>
       <c r="P35" t="n">
@@ -3356,20 +3356,20 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Coco is a visually stunning and emotionally captivating animated film that explores themes of family, memory, and the power of music. Set in a vibrant world inspired by Mexican culture, the movie follows a young boy named Miguel on a journey to the Land of the Dead. With catchy songs, heartfelt moments, and a richly detailed storyline, Coco has left audiences in tears and awe, solidifying its place as one of Pixar's best films. It's a celebration of life, love, and the importance of remembering those who have passed on.</t>
+          <t>Coco is a visually stunning and emotionally captivating animated film that explores themes of family, memory, and the power of music. Set in a vibrant world inspired by Mexican culture, the movie follows a young boy named Miguel on a journey to the Land of the Dead. With a heartfelt story, catchy songs, and rich cultural details, Coco has left a lasting impact on audiences, making it a modern classic and one of Pixar's best films.</t>
         </is>
       </c>
       <c r="I36" t="n">
         <v>9</v>
       </c>
       <c r="J36" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="K36" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L36" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="M36" t="n">
         <v>8</v>
@@ -3379,7 +3379,7 @@
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>- death - murder - loss - grief - aging - dementia - living skeletons - deadbeat dads - devastated - heartwarming - crying - trauma - depression - breathtaking - spooky - scary - skeletons - Poco Loco - beautiful - best film - chills - remember me - crying in spanish - guitar tutorial - cinematic parallels - animated children - rules - family - Christian perspective - moved - emotional - cathartic - rebuke - abuse - power - entertainment industry - skeleton movie - coming of age - vibrant - colorful - metaphysical - forgiveness - gratifying - visual effects - cinematography - tears - teary-eyed - heartstrings - remember - music - culture - Mexican - vibrant - fantasy - Land of the Dead - predictable - heartwarming -</t>
+          <t>- emotional - heartwarming - visually stunning - culturally rich - vibrant - bittersweet - captivating - moving - beautiful - impactful - fantasy - gripping - catchy songs - unique - personal identity - tearjerker - celebration - legacy - memorable - engaging - colorful - fantastical - innovative - authentic - heartfelt - soulful - cathartic - breathtaking - adorable - delightful - charming - hilarious - hilarious - funny - sad - powerful - mesmerizing - enchanting - magical - creative - inspiring - nostalgic - relatable - masterpiece - cinematic - unforgettable - dynamic - must-watch - top-tier - brilliant - dynamic - fantastic - raw - unique - tender - elegiac - warm - fuzzy - classic - modern classic - emotional climax - drained - tear jerker -</t>
         </is>
       </c>
       <c r="P36" t="n">
@@ -3431,14 +3431,14 @@
         <v>125</v>
       </c>
       <c r="F37" t="n">
-        <v>4.76</v>
+        <v>4.75</v>
       </c>
       <c r="G37" t="n">
-        <v>0.49</v>
+        <v>0.5</v>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Spirited Away is a visually stunning and emotionally resonant masterpiece that captivates viewers with its magical world and rich storytelling. The film follows the journey of a young girl named Chihiro as she navigates a mysterious and fantastical realm filled with gods, witches, and spirits. Through themes of courage, growth, and empathy, Spirited Away explores the power of love and the importance of kindness in the face of adversity. With its intricate animation, memorable characters, and enchanting soundtrack, Spirited Away is hailed as one of the best animated films of all time, leaving a lasting impact on audiences of all ages.</t>
+          <t>Spirited Away is a visually stunning and emotionally resonant masterpiece that captivates viewers with its magical world and rich storytelling. The film follows the journey of Chihiro, a young girl who finds herself in a mysterious and fantastical realm filled with gods, witches, and spirits. As Chihiro navigates this strange world, she learns valuable lessons about courage, empathy, and the power of kindness. With its imaginative animation, memorable characters, and universal themes, Spirited Away has earned its reputation as one of the best animated films of all time.</t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -3448,7 +3448,7 @@
         <v>8</v>
       </c>
       <c r="K37" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L37" t="n">
         <v>8</v>
@@ -3461,7 +3461,7 @@
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>- magical - immersive - masterpiece - imaginative - visually stunning - emotional - transformative - enchanting - whimsical - nostalgic - captivating - mesmerizing - thought-provoking - beautiful - rich - intricate - fantastical - unique - creative - charming - touching - profound - timeless - universal - heartwarming - legendary - iconic - unforgettable - cinematic poetry - ethereal - surreal - whimsy - bittersweet - melancholic - magical realism - enchantment - dreamlike - imaginative world-building - Miyazaki magic - Studio Ghibli brilliance - animated perfection - cinematic treasure - emotional journey - spiritual awakening - visual feast - cultural exploration - ethical exploration - environmental themes - psychological depth - heartwarming relationships - character growth - courage - empathy - kindness -</t>
+          <t>- magical - immersive - transformative - visually stunning - emotional - imaginative - masterpiece - enchanting - nostalgic - whimsical - captivating - profound - beautiful - impactful - mesmerizing - intricate - thought-provoking - charming - fantastical - rich - unique - legendary - timeless - cinematic - detailed - expressive - universal - heartwarming - ethereal - enchanting - whimsical - surreal - legendary - unforgettable - whimsical - dreamlike - whimsical - whimsical - whimsical</t>
         </is>
       </c>
       <c r="P37" t="n">
@@ -3520,7 +3520,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Ratatouille is a heartwarming Pixar film about a talented rat named Remy who dreams of becoming a chef. The movie explores themes of passion, identity, and the pursuit of one's dreams. With stunning animation, a charming Parisian setting, and a memorable score by Michael Giacchino, Ratatouille is considered by many to be one of Pixar's best films. The story follows Remy's journey as he navigates the culinary world, proving that anyone can achieve greatness, no matter their background. The film's emotional moments, lovable characters, and messages of perseverance make it a timeless classic that continues to resonate with audiences.</t>
+          <t>Ratatouille is a heartwarming Pixar film about a talented rat named Remy who dreams of becoming a chef. The movie explores themes of passion, identity, and the pursuit of dreams. With stunning animation, a charming Parisian setting, and a memorable score by Michael Giacchino, Ratatouille is considered by many to be one of Pixar's best films. The story follows Remy's journey as he navigates the culinary world, proving that anyone can achieve greatness, regardless of their background. The film's emotional moments, lovable characters, and messages of perseverance make it a timeless classic that continues to resonate with audiences.</t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -3543,7 +3543,7 @@
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>- heartwarming - inspirational - culinary - Paris - masterpiece - emotional - animated - chef - dream - comfort - nostalgia - friendship - passion - creativity - family - underdog - perseverance - artistic - charming - delightful - magical - genius - heartening - lovable - classic - rewatchable - visually stunning - witty - soulful - moving - profound - relatable - motivational - enchanting - captivating - whimsical - imaginative - feel-good - iconic - heartening - cinematic - memorable - impactful - brilliant - entertaining - endearing - heartening - funny - touching - beautiful - heartwarming - creative - lovable - charming - delightful - heartening - heartwarming - inspiring - heartwarming - heartwarming - heartwarming</t>
+          <t>- heartwarming - inspirational - comedic - emotional - culinary - Parisian - animated - masterpiece - rewatchable - thought-provoking - charming - creative - lovable - enchanting - nostalgic - visually stunning - engaging - delightful - magical - impactful - memorable - genius - relatable - comforting - entertaining - heartening - heartwrenching - beautiful - touching - heartening - captivating - iconic - heartening - hilarious - imaginative - feel-good - classic - cinematic - brilliant - powerful - moving - whimsical - profound - exceptional - artistic - dynamic - impressive - unique - soulful - resonant - transformative - enchanting - heartening - endearing - heartwarming - heartwarming - heartwarming - heartwarming -</t>
         </is>
       </c>
       <c r="P38" t="n">
@@ -3602,7 +3602,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>The Lord of the Rings: The Fellowship of the Ring is a beloved cinematic masterpiece that captures the essence of J.R.R. Tolkien's epic tale. With breathtaking visuals, unforgettable characters, and a battle between good and evil, this film is a true cinematic wonder. Fans praise the loyalty of Samwise Gamgee, the beauty of Galadriel, and the perfection of the trilogy as a whole. The extended edition adds even more depth to this already incredible story. Overall, this film is a timeless classic that continues to captivate audiences and hold a special place in the hearts of fans around the world.</t>
+          <t>"The Lord of the Rings: The Fellowship of the Ring" is a cinematic masterpiece that captures the essence of J.R.R. Tolkien's epic tale of adventure, friendship, and the battle between good and evil. Directed by Peter Jackson, this film is the first installment of an iconic trilogy that has captivated audiences worldwide. With breathtaking visuals, compelling narratives, unforgettable characters, and a perfect balance of emotion and action, this film is truly a cinematic wonder. From the loyalty of Samwise Gamgee to the iconic line "You shall not pass," this movie has left a lasting impact on viewers, solidifying its place as a classic in the realm of fantasy cinema.</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -3625,7 +3625,7 @@
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>- epic - fantasy - adventure - perfect - stoner - loyalty - journey - crush - himbos - gay - poetic - flawless - magical - astounding - adaptation - beauty - darkness - classical - adventure - meme - fire - crush - burden - fire - dream - loyalty - beauty - perfection - masterclass - effect - horror - hot - love - beginning - epic - enchanting - childhood - adventure - score - characters - world building - pacing - performances - cinematography - emotional - landscapes - fight sequences - characters - story - captivating - intense - action - all-star cast - ride - shire - extended edition - timeless - hold up - balance - satisfying - clear</t>
+          <t>- epic - fantasy - adventure - friendship - loyalty - iconic - masterpiece - timeless - captivating - visually stunning - enchanting - breathtaking - immersive - legendary - classic - perfect - magical - emotional - powerful - impactful - cinematic wonder - near-perfect - sweeping - classical - beautiful - dark - tragic - heroic - stoner Gandalf - heartwarming - courageous - iconic score - masterclass - awe-inspiring - cathartic - extraordinary - thrilling - chilling - bold - horror elements - prologue - captivating epic - intense - thrilling - chills - all-star cast - brilliant - visionary - cult classic - captivating - engrossing - emotional - iconic trilogy - perfect adaptation - flawless - greatest adventure - world-building - pacing - performances - cinematography -</t>
         </is>
       </c>
       <c r="P39" t="n">
@@ -3684,7 +3684,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Donnie Darko is a mind-bending masterpiece that delves into themes of adolescence, time travel, mental illness, and sacrifice. With a stellar performance by Jake Gyllenhaal, the film leaves viewers questioning reality and the nature of existence. The eclectic soundtrack and surreal visuals add to the overall experience, making it a cult classic that continues to intrigue and captivate audiences.</t>
+          <t>Donnie Darko is a mind-bending masterpiece that delves into themes of adolescence, time travel, mental illness, and sacrifice. With a stellar performance by Jake Gyllenhaal, the film leaves viewers questioning reality and the nature of existence. The eclectic soundtrack and surreal visuals add to the overall mysterious and thought-provoking atmosphere of the movie. Despite its complex narrative, Donnie Darko remains a cult classic that continues to captivate audiences with its enigmatic storytelling.</t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -3707,7 +3707,7 @@
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>- masterpiece - time travel - existential - confusing - dark humor - schizophrenia - Jake Gyllenhaal - cult classic - soundtrack - mental illness - sacrifice - adolescence - mind-blowing - trippy - surreal - coming-of-age - enigmatic - teenage angst - Sparkle Motion - Easter Bunny - alternate universe - schizophrenia - existential crisis - Richard Kelly - iconic - 80s - nostalgia - directorial debut - complex plot - dark comedy - dream-like - thought-provoking - cult following - Seth Rogen - furry - Frank the rabbit - existential dread - teenage rebellion - hallucinations - philosophical - mind-bending - indie - psychological thriller - high school - time loop - apocalyptic - atmospheric - enigmatic - haunting - emotional - introspective</t>
+          <t>- masterpiece - time travel - existential - mind-blowing - confusing - Jake Gyllenhaal - schizophrenia - soundtrack - Halloween - cult classic - adolescence - mental illness - Sparkle Motion - rabbit - tangent universe - teenage angst - trippy - surreal - dark humor - science fiction - high school - delusions - eccentricities - Frank the rabbit - existential crisis - coming of age - dream-like - thought-provoking - mind-boggling - Seth Rogen - furry - Richard Kelly - iconic - emotional - soundtrack - 80s - adolescence - schizophrenia - sacrifice - time loop - existential dread - cult following - teenage messiah - hallucinations - alternate universe - mental health - masterpiece - dark comedy - enigmatic - teenage rebellion - philosophical</t>
         </is>
       </c>
       <c r="P40" t="n">
@@ -3766,7 +3766,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>"Soul" is a groundbreaking Pixar film that explores deep themes of purpose, life, and existence in a fresh and innovative way. With stunning animation, a beautiful score, and a mature storyline, it is both heartwarming and thought-provoking. The film follows Joe Gardner, a musician with big dreams, on a journey that challenges the audience to question their own lives and choices. Filled with emotional moments and existential musings, "Soul" is a must-watch for those seeking a unique and profound cinematic experience.</t>
+          <t>"Soul" is a groundbreaking Pixar film that explores deep themes such as purpose, life, and death in a fresh and innovative way. With stunning animation, a beautiful score, and a mature storyline, it is considered one of Pixar's most impressive works to date. The film follows Joe Gardner, a musician with big dreams, on a journey that challenges viewers to question their own existence and find joy in the simple moments of life. It is a heartwarming and thought-provoking experience that resonates with audiences of all ages.</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -3776,10 +3776,10 @@
         <v>8</v>
       </c>
       <c r="K41" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L41" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M41" t="n">
         <v>8</v>
@@ -3789,7 +3789,7 @@
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>- fresh - unique - high concepts - adventure - normal - gifted - jazz - depression - awe - impressive - technical - visually stunning - topping themselves - visually inventive - mature - existential - introspective - hilarious - heartwarming - love letter to life - wonderful - beautiful - love - joy - living - purpose - existential crisis - existentialism - jazz - music - emotional - moving - profound - transcendent - euphoric - masterpiece - grounded - human - naturalism - mature - deep - meaningful - compassion - afterlife - existentialist - purpose - adventure - unique - special - beautiful - core values - character work - fulfilling - possibilities - joys - soulful - emotional - heartbreakingly optimistic - life-affirming - life-changing - celebration</t>
+          <t>- fresh - unique - high concepts - adventure - gifted - normal - broad concept - purpose - jazz - depression - awe - impressive - technical - visually stunning - topping themselves - visually inventive - platitudinous - clever - concepts - untangle - mad - jazz diva - cubist - spiritual - satisfying - explanation - Knicks - jazzed - pants - crippling depression - existential crisis - existentialism - mature - introspective - love letter to life - wonderful - score - trent reznor - atticus ross - talent - tough year - precious moments - tough blob life - beautiful - love letter - existential crisis - existentialism - jazz - jazzing - beautiful moments - cinema therapy - deep - adult - important - mature - original - impactful</t>
         </is>
       </c>
       <c r="P41" t="n">
@@ -3848,7 +3848,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Oppenheimer is a visually stunning and technically masterful film that explores the life of J. Robert Oppenheimer, the father of the atomic bomb. Christopher Nolan's direction immerses the audience in a complex narrative that delves into moral dilemmas and the consequences of scientific discovery. Cillian Murphy delivers a mesmerizing performance, supported by a strong cast including Robert Downey Jr. and Emily Blunt. The film's use of IMAX and sound design creates a heart-pounding experience, although some viewers found it overly long or lacking emotional depth. Overall, Oppenheimer is a monumental achievement in filmmaking that leaves a lasting impact on its audience.</t>
+          <t>Oppenheimer is a visually stunning and technically impressive film that explores the life of J. Robert Oppenheimer, the father of the atomic bomb. With a mix of historical terror and compelling performances, the movie delves into the moral complexities of scientific advancements. While some viewers found it to be a masterpiece and Nolan's best work to date, others felt it was overly long and lacked emotional depth. Overall, Oppenheimer is a thought-provoking and immersive experience that leaves a lasting impact on its audience.</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -3871,7 +3871,7 @@
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>- atomic - immersive - heart-pounding - stud - best supporting actor - score - sound design - nuclear - ridiculous - josh peck - communist - funny - summer blockbuster - Rodrick Rules - blue eyes - god - face of god - winner - phenomenal - sex - understand - Oppenhard - work - obsessed - haunted - tortured - space-time - twilight world - exalted - fixated - moral implications - cosmic weight - maturity - ambiguity - harrowing - psychological tax - monumental achievement - moral torment - Oscar-worthy - cinematography - sound - editing - character study - soundscape - epic visuals - awe-inspiring - breathtaking - awe - awe-inspiring - grand nightmare - synthesized ideas - fission - fusion - grand - synthesized - ideas</t>
+          <t>- atomic - immersive - heart-pounding - stud - best supporting actor - score - sound design - nuclear - funny - summer blockbuster - Rodrick Rules - communist - harrowing - psychological - dense - intense - master class - visually stunning - awe-inspiring - moral torment - Oscar-worthy - cinematography - thunderous - intricate editing - magnificent score - character study - breathtaking - epic visuals - surreal - subjective - experimental - visually stunning - aesthetic masterclass - personal - challenging - introspective - monumental - profound - beautiful - terrifying - surreal - sublime - personal - experimental - complex - technical mastery - historical terror - bureaucratic - surreal - sublime - personal - experimental - complex - technical mastery - historical terror - bureaucratic - surreal - sublime - personal - experimental -</t>
         </is>
       </c>
       <c r="P42" t="n">
@@ -3930,7 +3930,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>1917 is a visually stunning and technically impressive war film that immerses viewers in the brutal realities of World War I. The continuous shot structure, while not truly one take, adds to the immersive experience. The film's cinematography, score, and direction are all top-notch, creating a harrowing and emotional journey for the characters. While some may find the narrative lacking depth, the film's technical achievements and gripping storytelling make it a must-watch for fans of war movies.</t>
+          <t>1917 is a visually stunning and technically impressive war film that immerses viewers in the brutal realities of World War I. The continuous shot structure, while not truly one take, adds to the immersive experience. The film follows two soldiers on a perilous mission to deliver a message that could save thousands of lives. While some find the narrative lacking depth, the film's technical achievements, including Roger Deakins' cinematography and Thomas Newman's score, make it a gripping and emotional cinematic experience. Despite some criticisms, 1917 is praised for its realism and the performances of the cast, particularly George MacKay. Overall, it is considered a cinematic landmark and a must-see for its technical prowess and immersive storytelling.</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -3940,20 +3940,20 @@
         <v>8</v>
       </c>
       <c r="K43" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="L43" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="M43" t="n">
         <v>7</v>
       </c>
       <c r="N43" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>- immersive - technical achievement - visceral - emotional - breathtaking - impressive - intense - harrowing - cinematic - masterclass - gripping - powerful - realistic - immersive - stunning - relentless - beautiful - epic - tense - impactful - engaging - survival thriller - unique - thrilling - heart-racing - impressive blocking - natural performances - grounded perspective - terrifying - brutal - haunting - surreal - immersive - breathtaking cinematography - emotional score - outstanding - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive</t>
+          <t>- immersive - technical marvel - emotional - breathtaking - intense - impressive - naturalistic - grounded - visceral - harrowing - powerful - stunning - gripping - relentless - beautiful - epic - tense - immersive - masterclass - brilliant - immersive - engaging - survival thriller - unique - impactful - visceral - visual - anxiety-inducing - fluid - anxiety-inducing - smooth - breathtaking - emotional - rewarding - cinematic landmark - impressive - thrilling - heart-racing - connective - captivating - incredible - innovative - cool - unique - epic - intense - fluid - anxiety-inducing - smooth - breathtaking - emotional - rewarding - cinematic landmark - impressive - thrilling - heart-racing - connective - captivating - incredible - innovative - cool - unique - epic - intense - fluid -</t>
         </is>
       </c>
       <c r="P43" t="n">
@@ -4012,7 +4012,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Killers of the Flower Moon is a haunting, powerful, and immersive film that delves into the dark history of the Osage murders. Directed by Martin Scorsese, the film showcases stellar performances from Leonardo DiCaprio, Robert De Niro, and Lily Gladstone. It is a deep dive into the banality of evil, exploring themes of greed, violence, and complicity in American history. The film is a masterpiece that leaves a lasting impact on the audience, shedding light on a tragic chapter in American history.</t>
+          <t>Killers of the Flower Moon is a haunting, powerful, and immersive film that delves into the dark history of the Osage murders. Martin Scorsese's direction is sharp, the performances are stellar, and the storytelling is both devastating and impactful. The film sheds light on the atrocities committed against the Osage people, making it a necessary and important watch. Despite its lengthy runtime, it remains a tour de force of cinema that leaves a lasting impact on the viewer.</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -4025,7 +4025,7 @@
         <v>9</v>
       </c>
       <c r="L44" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M44" t="n">
         <v>8</v>
@@ -4035,7 +4035,7 @@
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>- Osage - heavy - struggle - Indigenous - Sisyphean - task - visible - ancestors - pride - Leo - movie - tiktok - clips - car - gangsta - marty - true crime - podcast - quartet - oscar - Lily Gladstone - Leo DiCaprio - grumpy cat faces - haunting - gripping - expertly paced - 4th acts - haunting images - raw - potent - betrayal - Mollie - love - Ernest - teeth - wolves - triumphant - bold - tragic - career bests - Gladstone - brightest - Jesse Plemons - hat - massive - Leo - depth - nuance - De Niro - skin crawl - colossal - oscar campaign - Scorsese - filmmaker - Silence</t>
+          <t>- Osage - heavy - struggle - Indigenous - Sisyphean - task - visible - ancestors - pride - Leo - movie - tiktok - clips - car - true crime - podcast - quartet - Lily Gladstone - Oscar - Leo DiCaprio - Robert De Niro - grumpy cat faces - Mollie - Ernest - betrayal - raw - potent - haunting - gripping - expertly paced - 4th acts - Tulsa - Robbie Robertson - score - balanced - educational - mandatory - viewing - schools - country - cinema - epic - American history - true crime - extravagant - violent - haunting - powerful - immersive - devastating - empathy - Osage - Lily Gladstone - Mollie - complicity - greed - power -</t>
         </is>
       </c>
       <c r="P44" t="n">
@@ -4090,34 +4090,34 @@
         <v>4.58</v>
       </c>
       <c r="G45" t="n">
-        <v>0.89</v>
+        <v>0.9</v>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Schindler's List is a powerful and emotionally devastating film that captures the horrors of the Holocaust through the story of Oskar Schindler, a man who saved many Jews during World War II. Steven Spielberg's direction is masterful, with stunning cinematography and exceptional performances. The film is a haunting depiction of the atrocities committed against the Jewish people, while also offering a message of hope and humanity in the face of darkness. It is considered one of the greatest films ever made, a true masterpiece that leaves a lasting impact on all who watch it.</t>
+          <t>Schindler's List is a powerful and emotionally devastating film that captures the horrors of the Holocaust through the story of Oskar Schindler, a German businessman who becomes an unexpected hero. Steven Spielberg's direction, along with exceptional performances, stunning cinematography, and a haunting score, make this film a masterpiece that transcends the boundaries of cinema. The use of black and white imagery, symbolism, and storytelling create a gripping and unforgettable experience that leaves a lasting impact on the viewer. It is a must-watch film that showcases the best of filmmaking artistry and storytelling.</t>
         </is>
       </c>
       <c r="I45" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J45" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="K45" t="n">
         <v>10</v>
       </c>
       <c r="L45" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="M45" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="N45" t="n">
         <v>10</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>- masterpiece - powerful - moving - iconic - mythic - emotional - important - essential - profound - heartbreaking - somber - devastating - beautiful - sympathetic - perfect - respectful - honoring - true - despicable - chilling - terrifying - cathartic - tragic - astounding - tragic - astounding - gut-wrenching - haunting - resounding - noble - altruistic - sincere - gut-wrenching - compelling - intense - gripping - visually stunning - emotionally charged - poignant - triumphant - gripping - impactful - harrowing - raw - layered - bone deep - cinematic triumph - visually striking - life-changing - speechless</t>
+          <t>- haunting - powerful - masterpiece - moving - important - iconic - profound - gut-wrenching - emotional - somber - intense - gripping - harrowing - poignant - raw - heartbreaking - cinematic triumph - visually stunning - brilliant - captivating - impactful - cathartic - unforgettable - thought-provoking - compelling - mesmerizing - chilling - disturbing - enlightening - enlightening - historical - significant - must-watch - timeless - legendary - mesmerizing - flawless - sincere - resounding - awe-inspiring - resiliency - resounding - awe-inspiring - resiliency - transcendent - gripping - devastating - gut-wrenching - life-changing - powerful storytelling - exceptional performances - visually striking - heart-wrenching - profound - heart-wrenching</t>
         </is>
       </c>
       <c r="P45" t="n">
@@ -4176,30 +4176,30 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>- The Zone of Interest is a chilling and thought-provoking exploration of the banality of evil, focusing on the lives of a Nazi officer and his family living next to a concentration camp. Through its use of sound design and minimalist visuals, the film creates a haunting atmosphere that lingers long after the credits roll. It challenges viewers to confront the uncomfortable reality of complicity and indifference in the face of atrocities. A truly impactful and unforgettable cinematic experience.</t>
+          <t>- The Zone of Interest is a chilling and haunting exploration of the banality of evil, focusing on the lives of a Nazi officer and his wife living next to a concentration camp. Through its use of sound design and minimal visuals, the film creates a sense of unease and discomfort that lingers long after the credits roll. It challenges viewers to confront their own complicity and forces them to question the normalization of atrocities. A powerful and thought-provoking piece of cinema that will leave a lasting impact.</t>
         </is>
       </c>
       <c r="I46" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J46" t="n">
         <v>0</v>
       </c>
       <c r="K46" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L46" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="M46" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N46" t="n">
         <v>9</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>- The Zone of Interest is a film that will stay with you long after the credits roll. It's a haunting experience that challenges the audience to confront the banality of evil and the horrors of genocide in a unique and powerful way.</t>
+          <t>- A chilling exploration of the banality of evil, the horrors of genocide, and the normalization of atrocity. The use of sound design and absence of visuals creates a haunting and unforgettable experience.</t>
         </is>
       </c>
       <c r="P46" t="n">
@@ -4256,7 +4256,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Get Out is a smart, thought-provoking, and terrifying horror film that cleverly blends social commentary with suspense. Directed by Jordan Peele, the film follows a black man who visits his white girlfriend's parents and uncovers sinister secrets. With brilliant performances, symbolism, and a twist that keeps viewers on edge, Get Out is hailed as a modern classic in the horror genre. The film's exploration of race relations and subtle metaphors make it a must-watch for audiences looking for a unique and chilling cinematic experience.</t>
+          <t>Get Out is a smart, thought-provoking, and terrifying horror film that cleverly blends social commentary with suspense. Directed by Jordan Peele, the film follows a black man who visits his white girlfriend's parents and uncovers sinister secrets. With brilliant performances, symbolism, and a twist that keeps you on edge, Get Out is a must-watch for its originality and boldness. White people are portrayed as terrifying in this film, and the movie's themes and metaphors make it a standout in the horror genre. Overall, Get Out is a masterfully crafted film that leaves a lasting impact on its viewers.</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -4279,7 +4279,7 @@
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>- smart - thought-provoking - clever - original - intense - suspenseful - satirical - political - funny - calculated - visually stunning - impeccably acted - scary - iconic - brilliant - genius - psychological - layered - symbolic - unsettling - suspenseful - eerie - twisty - suspenseful - entertaining - compelling - masterfully crafted - bold - smart - economical - creepy - intense - thrilling - unique - effective - thought-provoking - smart - scary - smart - smart - smart - smart - smart - smart - smart - smart - smart - smart - smart - smart - smart - smart - smart - smart - smart - smart - smart - smart - smart - smart - smart - smart - smart - smart - smart - smart - smart</t>
+          <t>- social commentary - horror - satire - intense - psychological - suspenseful - thought-provoking - original - smart - racial themes - unsettling - brilliant - layered - symbolic - creepy - genius - twist - entertaining - unique - thriller - bold - funny - political - calculated - visually stunning - impeccably acted - scary - iconic - psychopathic - intense ending - satisfying - rewatchable - masterful - suspense - eerie - satirical - clever - metaphors - smart dialogue - standout performances - cinematography - social critique - genre blending - suspenseful plot - unsettling atmosphere - disturbing - intense suspense - twist ending - smart horror - jump scares - racial commentary - thought-provoking concepts - smart storytelling - brilliant metaphors - terrifying - over-hyped</t>
         </is>
       </c>
       <c r="P47" t="n">
@@ -4334,7 +4334,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Midsommar is a visually stunning and psychologically intense horror film that takes the audience on a surreal journey into a disturbing pagan cult. Directed by Ari Aster, the film explores themes of grief, trauma, toxic relationships, and self-actualization. With a mix of horror and dark humor, Midsommar follows a group of friends who attend a midsummer festival in a remote Swedish village, only to find themselves trapped in a nightmarish and increasingly violent ritual. Featuring excellent performances, beautiful cinematography, and a haunting score, Midsommar is a unique and disturbing cinematic experience that leaves a lasting impact on viewers.</t>
+          <t>Midsommar is a visually stunning and psychologically intense horror movie that takes the audience on a surreal journey into a disturbing pagan cult. The film explores themes of grief, trauma, toxic relationships, and self-actualization in a unique and disturbing way. With excellent performances, beautiful cinematography, and a haunting score, Midsommar is a chilling and engaging experience that will leave you unsettled and questioning what you just watched.</t>
         </is>
       </c>
       <c r="I48" t="n">
@@ -4357,7 +4357,7 @@
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>- family suicide - therapy - cute couples costume - weed cookie - dark reality - pubic hair pie - floral purge - Charlie and the Chocolate Factory - grief - white men - mixtape - Skarsgård family - Swedish pagan rituals - scary Sweden - relationship endings - boyfriend humor - hot girl summer - influencers at Coachella - formal rigor - mental health stigma - disturbing experience - Midsommar stan community - Director's Cut - relationship breakdown - American students in Europe - trip with the boys - Will Poulter - gaslighting - One Perfect Shot - ritual sacrifice - Ariana Grande - Swedish cult ritual - poppers at a Kate Bush concert - superhero movies - Director's Cut breakdown - uninspired horror - ugly Americans in Europe -</t>
+          <t>- family suicide - therapy - weed cookie - dark reality - pubic hair pie - floral purge - Charlie and the Chocolate Factory - grief - white men - mixtape - Skarsgård family - Swedish pagan rituals - scary Sweden - relationship endings - hot girl summer - influencers at Coachella - formal rigor - mental health stigma - disturbing experience - Midsommar stans - Director's Cut - breakup movies - American students in Europe - trip with the boys - Will Poulter - gaslighting - One Perfect Shot - ritual sacrifice - Ariana Grande - Swedish cult ritual - poppers at a Kate Bush concert - superhero movies - Director's Cut breakdown - uninspired horror - ugly Americans in Europe - Florence Pugh - cult narrative -</t>
         </is>
       </c>
       <c r="P48" t="n">
@@ -4412,11 +4412,11 @@
         <v>4.29</v>
       </c>
       <c r="G49" t="n">
-        <v>0.59</v>
+        <v>0.6</v>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>American Psycho is a darkly comedic and satirical film that follows the wealthy New York banker Patrick Bateman, played brilliantly by Christian Bale, as he hides his psychopathic alter ego from the world. The film delves into the materialistic and hedonistic world of Manhattan in the 1980s, mocking male narcissism and the yuppie generation. With a mix of funny and scary moments, strong visuals, and a stellar performance by Bale, American Psycho is a masterpiece of satire and social commentary that leaves a lasting impression on viewers.</t>
+          <t>American Psycho is a darkly comedic and satirical film that follows the wealthy New York banker, Patrick Bateman, played brilliantly by Christian Bale. The movie delves into the materialistic and hedonistic world of Manhattan in the 1980s, showcasing the shallow and vile nature of its protagonist. With a mix of funny and scary moments, American Psycho critiques the 1980s lifestyle focused on money and looks. Bale's performance as Bateman is captivating, showcasing a man who appears normal on the outside but is truly dangerous on the inside. The film is a masterpiece of satire and social commentary, leaving a lasting impression on viewers.</t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -4439,7 +4439,7 @@
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>- dark comedy - satire - psychological thriller - iconic - quotable - Christian Bale - social commentary - 80s Wall Street - narcissism - materialism - satire - masterpiece - feminist - disturbing - ferocious - unhinged - comfort movie - relatable - captivating - prescient - male vanity - voyeuristic - insane - shallow - vile - sociopath - luxury - wealth - self-obsessed - chainsaw - brutality - iconic scene - skincare routine - obsession - obsession - obsession - obsession - obsession - obsession - obsession - obsession - obsession - obsession - obsession - obsession - obsession - obsession - obsession - obsession - obsession - obsession - obsession - obsession - obsession - obsession - obsession - obsession - obsession - obsession - obsession - obsession - obsession -</t>
+          <t>- brutal - satire - dark comedy - iconic - quotable - twisted - dramatic - cinematic - funny - satirical - masterpiece - mesmerizing - captivating - ferocious - unhinged - social commentary - psychological thriller - prescient - voyeuristic - feminist - comfort movie - relatable - outrageous - shallow - vile - insane - disturbing - surreal - horror - surrealism - dissociation - privilege - ego - misappropriated masculinity - societal critique - behemoth - pop culture - normal - calm - iconic performance - memorable - dangerous</t>
         </is>
       </c>
       <c r="P49" t="n">
@@ -4498,7 +4498,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>The Menu is a darkly comedic satire that takes aim at bougie culture, the restaurant industry, and the cult of celebrity chefs. With a stellar cast including Ralph Fiennes and Anya Taylor-Joy, the film serves up a deliciously wicked banquet of comedy, satire, and terror. While some viewers found it to be a hilarious and entertaining ride, others felt that it fell short in its execution and failed to deliver on its potential. Overall, The Menu is a divisive film that offers a unique and twisted take on the horror-thriller genre.</t>
+          <t>The Menu is a darkly comedic satire that takes aim at bougie culture, the restaurant industry, and the cult of celebrity chefs. With a stellar cast including Ralph Fiennes and Anya Taylor-Joy, the film serves up a deliciously wicked banquet of comedy, satire, and terror. While some viewers found it to be a hilarious and entertaining ride, others felt that it fell short in its execution and failed to deliver on its potential. Overall, The Menu is a divisive film that offers a unique and absurd take on the "eat the rich" genre.</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -4521,7 +4521,7 @@
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>- surprising - dark humor - satire - service industry - bread - weird - cannibalism - humor - eat the rich - cheeseburger - bold - goofy - elite humiliation - high brow foodie culture - edibles - Taco Tuesday - rated R Ratatouille - Jeremy Allen White - movie rating - letterboxd - anti-ideology - satire fail - Anya Taylor-Joy - Ralph Fiennes - foodie culture - social commentary - dark and wicked - catharsis - revenge - erotic response - thriller - horror - comedy - social classes - pretentious - food porn - greasy - juicy - unpleasant - horror - creepy - aggressive - sharp - cheeseburger - imperialism - Midsommar - stunning - shallow - anti-classism</t>
+          <t>- surprising - dark humor - satire - service industry - bread - weird - cannibalism - humor - eat the rich - cheeseburger - bold - goofy - elite humiliation - high brow foodie culture - edibles - Taco Tuesday - rated R Ratatouille - Jeremy Allen White - movie rating - letterboxd - anti-ideology - satire fail - Anya Taylor-Joy - Ralph Fiennes - foodie culture - social commentary - thriller - dark comedy - class satire - pretentious - comedy - ensemble cast - food porn - greasy - juicy - delicious - culinary students - eat the rich - unpleasant - horror - creepy - aggressive - entertaining - sharp - cheeseburger - imperialism - Midsommar - TIFF - stunning - shallow</t>
         </is>
       </c>
       <c r="P50" t="n">
@@ -4580,7 +4580,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>The Shining is a horror masterpiece directed by Stanley Kubrick, known for its chilling atmosphere and iconic performances. Jack Nicholson's portrayal of Jack Torrance is electrifying, while Shelley Duvall's performance as Wendy is intense and realistic. The film explores themes of abuse, isolation, and the descent into madness, all set within the eerie Overlook Hotel. With stunning visuals and a haunting score, The Shining remains a classic in the horror genre, captivating audiences with its psychological terror and supernatural elements.</t>
+          <t>The Shining is a horror masterpiece directed by Stanley Kubrick, known for its chilling atmosphere and iconic performances. Jack Nicholson's portrayal of Jack Torrance is electrifying, while Shelley Duvall's performance as Wendy is intense and realistic. The film explores themes of abuse, isolation, and the descent into madness. With stunning visuals and a haunting score, The Shining remains a classic in the horror genre.</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4603,7 +4603,7 @@
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>- intense - realistic - fear - terror - overlooked - mental abuse - random - bear costume - crazy - hotel - murder - family - mental health - abuse - iconic - funny - bozo mode - masterpiece - domestic abuse - running - vampiric winnie the pooh - hotel stay - trivago - writer - classic - traumatize - horny - twins - maze - axe - drive in theater - snowy - cabin fever - isolation - family bonding - perfection - self-care - bear giving neck - aesthetic - chilling - atmosphere - cabin fever - descent into darkness - domestic horror - family - fire and ice - psychological horror - supernatural - iconic - cold - eerie - blood - extended version - technical masterclass - snowbound - creative - addiction -</t>
+          <t>- intense - realistic - fear - terror - overlooked - mental abuse - random - bear costume - crazy - hotel - murder - family - mental health - abuse - iconic - funny - bozo mode - masterpiece - domestic abuse - running - furry fetish - vampiric winnie the pooh - hotel stay - trivago - writer - self-care - ghost bartenders - perfection - aesthetic - technical - horror - supernatural - psychological - family - cabin fever - snowbound - chilling - atmosphere - claustrophobic - isolation - madness - descent - cold - eerie - symmetrical - spatial geometry - formal exercise - spatial - geometry - spatial geometry - spatial - geometry - spatial geometry - spatial - geometry - spatial geometry - spatial - geometry - spatial geometry</t>
         </is>
       </c>
       <c r="P51" t="n">
@@ -4662,7 +4662,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>La La Land is a film that has divided audiences, with some finding it to be a magical and uplifting experience, while others have been left feeling depressed and disappointed. The movie, directed by Damien Chazelle, follows the intertwined lives of Mia, an aspiring actress, and Sebastian, a passionate jazz musician, as they pursue their dreams and navigate their love for each other. With captivating performances from Emma Stone and Ryan Gosling, mesmerizing musical numbers, and stunning cinematography, La La Land is a celebration of art, dreams, and the complexities of love. Despite its mixed reviews, the film has left a lasting impact on many viewers, evoking a range of emotions from happiness to sadness.</t>
+          <t>La La Land is a film that evokes a wide range of emotions from viewers, from pure magic to deep sadness. It is a celebration of dreams and love, set against the backdrop of Los Angeles. The film's stunning cinematography, captivating performances by Emma Stone and Ryan Gosling, and mesmerizing musical numbers make it a true cinematic gem. While some find it to be a masterpiece that reinvented musicals, others criticize its lack of originality and its portrayal of certain themes. Overall, La La Land is a film that leaves a lasting impact on those who watch it, sparking both joy and tears.</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4685,7 +4685,7 @@
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>- enchanting - charming - magical - bittersweet - emotional - impactful - mesmerizing - captivating - vibrant - celebratory - nostalgic - romantic - breathtaking - electric - sublime - bold - rewarding - joyous - melancholic - beautiful - triumphant - hopeful - dramedy - tragic - catchy - flawless - stunning - amazing - enchanting - charming - joy - celebration - love - dream - passion - sacrifice - musical - comedy - vibrant - contemporary - bliss - cinematic</t>
+          <t>- magical - emotional - impactful - bittersweet - mesmerizing - joyous - melancholic - romantic - nostalgic - vibrant - celebratory - enchanting - captivating - dreamy - hopeful - dramedy - tragic - catchy - beautiful - flawless - stunning - amazing - incredible - goddamn - flawless - stunning - amazing - incredible - goddamn - emotional - impactful - bittersweet - mesmerizing - joyous - melancholic - romantic - nostalgic - vibrant - celebratory - enchanting - captivating - dreamy - hopeful - dramedy - tragic - catchy - beautiful - flawless - stunning - amazing - incredible - goddamn - emotional - impactful - bittersweet - mesmerizing - joyous - melancholic - romantic - nostalgic - vibrant</t>
         </is>
       </c>
       <c r="P52" t="n">
@@ -4744,7 +4744,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>- Whiplash is a gripping and intense film about a young drummer's pursuit of greatness at a cut-throat music conservatory, mentored by an instructor who will stop at nothing to push his students to their limits. The performances by Miles Teller and J.K. Simmons are outstanding, with Simmons delivering a terrifying portrayal of a demanding teacher. The film is a rollercoaster of emotions, leaving viewers on the edge of their seats with its powerful storytelling and electrifying music.</t>
+          <t>- Whiplash is a gripping and intense film about a young drummer's journey to greatness at a cut-throat music conservatory, mentored by an instructor who will stop at nothing to push his students to their limits. The performances by Miles Teller and J.K. Simmons are outstanding, with Simmons delivering a terrifying portrayal of a demanding teacher. The film is a rollercoaster of emotions, leaving viewers on the edge of their seats with its powerful storytelling and electrifying music.</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4767,7 +4767,7 @@
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>- intense - anxiety-inducing - thrilling - passionate - brutal - electrifying - mesmerizing - exhilarating - masterful - powerful - compelling - perfection - sociopathic - adrenaline-fueled - emotional - heart-pounding - engrossing - captivating - energetic - intense - phenomenal - impressive - creative - astounding - dedicated - toxic - brutal - thrilling - terrifying - incredible - relentless - shocking - transformative - captivating - mesmerizing - brutal - intense - exhilarating - electrifying - masterful - passionate - compelling - powerful - anxiety-inducing - thrilling - intense - brutal - electrifying - mesmerizing - exhilarating - captivating - compelling - powerful - masterful - perfection - anxiety-inducing - intense - brutal - electrifying - mesmerizing - exhilar</t>
+          <t>- intense - anxiety-inducing - thrilling - passionate - brutal - electrifying - mesmerizing - exhilarating - masterful - perfection - psychotic - sociopathic - relentless - emotional - captivating - engrossing - energetic - intense - stressful - compelling - powerful - phenomenal - impressive - creative - astounding - nihilistic - dedicated - toxic - brutal - incredible</t>
         </is>
       </c>
       <c r="P53" t="n">
@@ -4826,20 +4826,20 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Coco is a visually stunning and emotionally captivating animated film that explores themes of family, memory, and the power of music. Set in a vibrant world inspired by Mexican culture, the movie follows a young boy named Miguel on a journey to the Land of the Dead. With a heartfelt story, catchy songs, and rich cultural details, Coco has left audiences in tears and awe, solidifying its place as one of Pixar's best films.</t>
+          <t>Coco is a visually stunning and emotionally captivating animated film that celebrates Mexican culture and explores themes of family, memory, and the power of music. It has been praised for its vibrant colors, catchy songs, and heartfelt storytelling. Many viewers have found themselves moved to tears by the film's emotional moments and powerful messages. Overall, Coco is considered a modern classic and one of Pixar's best films to date.</t>
         </is>
       </c>
       <c r="I54" t="n">
         <v>9</v>
       </c>
       <c r="J54" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="K54" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L54" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="M54" t="n">
         <v>8</v>
@@ -4849,7 +4849,7 @@
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>- emotional - heartwarming - visually stunning - tearjerker - family - culture - music - vibrant - bittersweet - fantasy - captivating - memorable - animation - colorful - celebration - Mexican - tradition - legacy - beautiful - catchy songs - gripping - unique - personal identity - cathartic - moving - masterpiece - soulful - impactful - engaging - fantastical - creative - dynamic - innovative - authentic - heartfelt - inspiring - charming - relatable - nostalgic - enchanting - magical - captivating - brilliant - dynamic - must-watch - top-tier - breathtaking - hilarious - hilarious - spooky - scary - skeletons - class systems - rich people - greatness - depression - alebrije - chills - emotional climax - drained - tearjerker - soulful</t>
+          <t>- emotional - heartwarming - visually stunning - culturally rooted - vibrant - bittersweet - captivating - fantasy - rich culture - personable - catchy songs - gripping storyline - modern classic - beautiful lyricism - tear jerker - unique personal identity - emotionally impactful - best animation - heartwarming climax - draining - tear jerker - best Pixar movie - hands down - best Pixar film - heart of sobra</t>
         </is>
       </c>
       <c r="P54" t="n">
@@ -4904,11 +4904,11 @@
         <v>2.05</v>
       </c>
       <c r="G55" t="n">
-        <v>1.28</v>
+        <v>1.27</v>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Bohemian Rhapsody is a divisive film that has received mixed reviews from audiences. While some praise Rami Malek's performance as Freddie Mercury and the music of Queen, others criticize the film for its formulaic and sanitized portrayal of the band's history. Many viewers feel that the movie lacks depth, authenticity, and proper handling of Freddie Mercury's queerness and AIDS diagnosis. Despite its flaws, some viewers still find enjoyment in the film, particularly in the musical scenes and performances. Overall, Bohemian Rhapsody has sparked a range of reactions, from disappointment to admiration.</t>
+          <t>Bohemian Rhapsody is a polarizing film that has received mixed reviews from audiences. While some praise Rami Malek's performance as Freddie Mercury and the film's musical sequences, others criticize its inaccuracies, lack of depth, and formulaic storytelling. The movie has been accused of exploiting queerness and failing to do justice to Freddie Mercury's legacy. Despite its flaws, some viewers find it entertaining and emotionally engaging, while others see it as a missed opportunity to delve deeper into the story of Queen and its iconic frontman.</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4918,16 +4918,16 @@
         <v>4</v>
       </c>
       <c r="K55" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L55" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M55" t="n">
         <v>2</v>
       </c>
       <c r="N55" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
@@ -4990,7 +4990,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Priscilla is a visually stunning and emotionally complex film that delves into the toxic relationship between Priscilla Presley and Elvis Presley. Sofia Coppola's direction captures the isolation and manipulation Priscilla experiences, while Cailee Spaeny delivers a masterful performance. The film critiques Elvis's behavior and the dark side of fame, with subtle moments of beauty and heartbreak throughout. Despite some rushed moments in the third act, Priscilla is a captivating exploration of power dynamics and the loss of innocence.</t>
+          <t>Priscilla is a visually stunning and emotionally complex film that delves into the toxic relationship between Priscilla Presley and Elvis Presley. Sofia Coppola's direction captures the isolation and manipulation Priscilla experiences, while Cailee Spaeny delivers a powerful performance. The film critiques Elvis's behavior and the dark side of fame, with subtle moments of beauty and tragedy throughout. Despite some pacing issues in the third act, Priscilla is a thought-provoking exploration of power dynamics and the loss of innocence.</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -5013,7 +5013,7 @@
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>- car scene with Elvis - heartbreaking - Sofia Coppola masterpiece - Cailee Spaeny performance - Jacob Elordi height - dreamlike - toxic relationship - grooming - beautiful cage - dark fairytale - loneliness - control - predatory relationship - emotional core - subtlety - smart - palpable grace - beautiful nothingness - funny - melancholic - incisive - heartbreaking - innocence - girlhood - bittersweet tragedy - dreamy - nightmare - fragility - subtle - mean - cold - logical - dark - mean - subtle - complicity - women's stories - matter - contrast - rushed - growth</t>
+          <t>- jacob elordi - tall - elvis - grooming - objectification - lana del rey - austin butler - sofia coppola - coming-of-age - dark fairytale - asexual - subtlety - smart - loneliness - control - predatory relationship - passion - justice - cage - humanizes - critical - visual - remarkable - dark - honest - demise - innocence - reality - performances - beautiful - melancholic - melancholy - toxic - beautiful - dreamlike - bittersweet - tragedy - freedom - heartbreak - patient - incisive - innocence - girlhood - growth - Oscar Nom - Barbie - costumes - makeup - performance - production design - women's stories - matter - jail - rushed - contrast -</t>
         </is>
       </c>
       <c r="P56" t="n">
@@ -5072,7 +5072,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Get Out is a smart, thought-provoking, and terrifying horror film that cleverly blends social commentary with suspense. Directed by Jordan Peele, the film follows a black man who visits his white girlfriend's parents and uncovers sinister secrets. With brilliant performances, symbolism, and a twist that keeps viewers on edge, Get Out is hailed as a modern classic in the horror genre. The film's exploration of race relations and subtle metaphors make it a must-watch for audiences looking for a unique and chilling cinematic experience.</t>
+          <t>Get Out is a smart, intense, and thought-provoking horror film that cleverly blends genres and delivers a powerful social commentary. Directed by Jordan Peele, the film follows a black man who visits his white girlfriend's parents and uncovers sinister secrets. With brilliant performances, symbolism, and a twist that keeps viewers on edge, Get Out is a must-watch that leaves a lasting impact. White people are portrayed as terrifying in this film, and the use of metaphors and racial themes adds to the overall chilling experience. The film is praised for its originality, smart writing, and masterful direction, making it a standout in the horror genre.</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -5095,7 +5095,7 @@
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>- smart - clever - thought-provoking - intense - suspenseful - satirical - original - layered - brilliant - genius - political - calculated - visually stunning - impeccably acted - scary - iconic - psychopathic - intense - satisfying - funny - entertaining - bold - important - social commentary - masterful - intense - creepy - psychological - suspenseful - symbolic - unsettling - twist - unsettling - eerie - suspenseful - thrilling - effective - smart - racial themes - terrifying - over-hyped - amazing - masterpiece</t>
+          <t>- smart - political - calculated - funny - intense - visually stunning - impeccably acted - scary - iconic - brilliant - intense - psychological - layered - suspenseful - unsettling - unique - thought-provoking - clever - satirical - original - thrilling - entertaining - smartest - scary - metaphorical - weird - terrifying - intense - amazing - masterpiece</t>
         </is>
       </c>
       <c r="P57" t="n">
@@ -5150,7 +5150,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>The Batman is a dark, gritty, and visually stunning film that showcases a unique portrayal of Bruce Wayne as a disturbed and gothic figure. The movie delves into the detective side of Batman, with a focus on clues and investigation. The Riddler is portrayed as a twitch streamer, adding a modern twist to the character. The film has been praised for its atmospheric cinematography, haunting score, and standout performances from Robert Pattinson, Zoe Kravitz, and Paul Dano. Overall, The Batman is a refreshing take on the superhero genre, blending elements of noir, thriller, and crime drama to create a compelling and immersive experience.</t>
+          <t>The Batman is a dark, gritty, and visually stunning film that showcases a unique portrayal of Bruce Wayne as a disturbed and gothic figure. The movie delves into Batman's detective skills and features a standout performance by Robert Pattinson. With influences from films like Se7en and Zodiac, The Batman offers a fresh take on the superhero genre with a focus on character development and style. Despite its lengthy runtime, the film is praised for its immersive storytelling and masterful technical achievements. Overall, The Batman is considered a standout entry in the Batman franchise and a must-watch for fans of the character.</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -5173,7 +5173,7 @@
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>- disgusting - goth - emo - detective - sexy - gay - hilarious - thrilling - dark - gritty - immersive - engrossing - noir - masterpiece - bold - ambitious - mesmerizing - stunning - breathtaking - conflicted - atmospheric - psychological - haunting - chilling - intense - terrifying - brooding - horny - silly - funny - cringe - boring - predictable - exposition-laden - sprawling - ambitious - transformative - enduring - powerful - rage - corrupt - corrupt - corrupt - corrupt - corrupt - corrupt - corrupt - corrupt - corrupt - corrupt - corrupt - corrupt - corrupt - corrupt - corrupt - corrupt - corrupt - corrupt - corrupt - corrupt - corrupt - corrupt - corrupt - corrupt - corrupt - corrupt - corrupt - corrupt - corrupt - corrupt -</t>
+          <t>- disgusting - goth - detective - virgin - fantastic - sexy - emo - silly - gay - hilarious - twitch streamer - studied in film school - bangs - haunting - sex for the eyes - bold - pacing issues - Zodiac - Se7en - Saw - mesmerizing - best Batman movie - brooding - noir - immersive - dark - gritty - terrifying - breathtaking - stunning - masterful - conflicted - stunning - thrilling - sexy - boring - sexy - Spanish - eye shadow - hope - crime film - sprawling - ambitious - nightmare - monotonous - embarrassing - kiss in the sequel</t>
         </is>
       </c>
       <c r="P58" t="n">
@@ -5210,7 +5210,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Knives Out</t>
+          <t>Midsommar</t>
         </is>
       </c>
       <c r="C59" t="n">
@@ -5218,66 +5218,66 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Rian Johnson</t>
+          <t>Ari Aster</t>
         </is>
       </c>
       <c r="E59" t="n">
-        <v>131</v>
+        <v>147</v>
       </c>
       <c r="F59" t="n">
-        <v>4.33</v>
+        <v>3.8</v>
       </c>
       <c r="G59" t="n">
-        <v>0.6899999999999999</v>
+        <v>1.25</v>
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Knives Out is a clever and entertaining murder mystery film with a stellar cast, led by the brilliant Ana de Armas. The movie is filled with humor, twists, and a unique take on the genre, making it a crowd-pleaser. Daniel Craig's performance as Benoit Blanc is a standout, and the film's script is both smart and funny. Overall, Knives Out is a must-watch for fans of whodunnit films and offers a fresh take on the genre.</t>
+          <t>Midsommar is a visually stunning and psychologically intense horror film that takes the audience on a surreal journey into a disturbing pagan cult. Directed by Ari Aster, the film explores themes of grief, trauma, toxic relationships, and self-actualization. With a mix of disturbing and darkly comedic moments, Midsommar follows a group of friends who attend a midsummer festival in a remote Swedish village, only to find themselves trapped in a nightmarish and increasingly violent ritual. The film has been praised for its cinematography, performances, and unsettling atmosphere, making it a unique and disturbing cinematic experience.</t>
         </is>
       </c>
       <c r="I59" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="J59" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K59" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="L59" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="M59" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="N59" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>- clever - funny - entertaining - ensemble - mystery - detective - donut - cozy - twist - whodunnit - original - modern - hilarious - engaging - stacked cast - brilliant - self-aware - crowd-pleaser - captivating - intricate - homage - meta - suspenseful - ensemble cast - brilliant script - masterful - subversive - engaging - satisfying - memorable - quotable - cozy - twisty - cleverly-constructed - brilliant performances - crowd-pleasing - captivating - entertaining - engaging - original - modern - hilarious - ensemble - mystery - detective - donut - cozy - twist - whodunnit - self-aware - brilliant script - masterful - subversive - satisfying - memorable - quotable - captivating - intricate</t>
+          <t>- family suicide - therapy - couples costume - weed cookie - dark reality - pubic hair pie - floral purge - Charlie and the Chocolate Factory - grief - white men - mixtape - Skarsgård family - Swedish pagan rituals - scary Sweden - relationship endings - boyfriend humor - hot girl summer - influencers at Coachella - formal rigor - mental health stigma - disturbing experience - Midsommar stan community - Directors cut - relationship breakdown - American students in Europe - trip with the boys - Will Poulter - gaslighting - cinematography - cult narrative - horror in sunlight - breakup movie - Ari Aster - superhero movies - Director's Cut breakdown - uninspired horror - Swedish cult - breakup movie - Ari Aster's mind - mental health -</t>
         </is>
       </c>
       <c r="P59" t="n">
-        <v>165363234</v>
+        <v>27426361</v>
       </c>
       <c r="Q59" t="n">
-        <v>147534686</v>
+        <v>20620443</v>
       </c>
       <c r="R59" t="n">
-        <v>312897920</v>
+        <v>48046804</v>
       </c>
       <c r="S59" t="n">
-        <v>26769548</v>
+        <v>6560030</v>
       </c>
       <c r="T59" t="inlineStr">
         <is>
-          <t>Lionsgate Films</t>
+          <t>A24</t>
         </is>
       </c>
       <c r="U59" t="inlineStr">
         <is>
-          <t>PG-13</t>
+          <t>R</t>
         </is>
       </c>
       <c r="V59" t="inlineStr">
@@ -5292,7 +5292,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Midsommar</t>
+          <t>Knives Out</t>
         </is>
       </c>
       <c r="C60" t="n">
@@ -5300,66 +5300,66 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Ari Aster</t>
+          <t>Rian Johnson</t>
         </is>
       </c>
       <c r="E60" t="n">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="F60" t="n">
-        <v>3.8</v>
+        <v>4.33</v>
       </c>
       <c r="G60" t="n">
-        <v>1.25</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Midsommar is a visually stunning and psychologically intense horror film that takes the audience on a surreal journey into a disturbing pagan cult. Directed by Ari Aster, the film follows a group of friends who travel to a remote Swedish village to attend a midsummer festival, only to find themselves trapped in a nightmarish and increasingly violent ritual. With themes of grief, trauma, toxic relationships, and self-actualization, Midsommar is a unique and disturbing experience that leaves viewers both unsettled and intrigued. Featuring excellent performances, beautiful cinematography, and a haunting score, the film explores the darker aspects of human nature in a chilling and thought-provoking way.</t>
+          <t>Knives Out is a clever and entertaining murder mystery film with a stellar cast, led by the brilliant Ana de Armas. The movie is filled with humor, twists, and a unique take on the genre, making it a crowd-pleaser that keeps audiences engaged. Daniel Craig's performance as Benoit Blanc is a standout, and the film's script is both witty and engaging. Overall, Knives Out is a must-watch for fans of whodunnit films and offers a fresh take on the genre.</t>
         </is>
       </c>
       <c r="I60" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J60" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K60" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="L60" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M60" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="N60" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>- suicide - therapy - psychedelic - college - weed - dark - surreal - grief - white men - mixtape - skarsgård family - nightmare - influencers - self-actualization - toxic relationships - gaslighting - mental health stigma - disturbing - relationship-ending - funny - hot girl summer - superhero movies - director's cut - breakup - funny - cult - ritual - horror - daylight horror - swedish - psychedelic - breakup - cult - horror - daylight horror - swedish - psychedelic - breakup - cult - horror - daylight horror - swedish - psychedelic - breakup - cult - horror - daylight horror - swedish - psychedelic - breakup - cult - horror - daylight horror - swedish - psychedelic - breakup - cult - horror - daylight horror</t>
+          <t>- clever - funny - entertaining - ensemble - mystery - detective - donut - cozy - twist - whodunnit - modern - original - engaging - stacked cast - brilliant - self-aware - homage - compassionate - witty - crowd-pleaser - hilarious - captivating - intricate - suspenseful - ensemble cast - brilliant script - subversive - masterclass - memorable - exceptional - special - unique - tight script - earnest - human decency - mad genius - perfect - RIP Christopher Plummer</t>
         </is>
       </c>
       <c r="P60" t="n">
-        <v>27426361</v>
+        <v>165363234</v>
       </c>
       <c r="Q60" t="n">
-        <v>20620443</v>
+        <v>147534686</v>
       </c>
       <c r="R60" t="n">
-        <v>48046804</v>
+        <v>312897920</v>
       </c>
       <c r="S60" t="n">
-        <v>6560030</v>
+        <v>26769548</v>
       </c>
       <c r="T60" t="inlineStr">
         <is>
-          <t>A24</t>
+          <t>Lionsgate Films</t>
         </is>
       </c>
       <c r="U60" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>PG-13</t>
         </is>
       </c>
       <c r="V60" t="inlineStr">
@@ -5389,37 +5389,37 @@
         <v>149</v>
       </c>
       <c r="F61" t="n">
-        <v>4.65</v>
+        <v>4.66</v>
       </c>
       <c r="G61" t="n">
         <v>0.5600000000000001</v>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Based on user reviews on Letterboxd, "Gone Girl" is a twisted and thrilling film that explores the complexities of marriage, deception, and manipulation. The character of Amy Dunne, played by Rosamund Pike, is hailed as a powerful and chilling force to be reckoned with. The film is praised for its dark humor, sharp dialogue, and unexpected twists. Some viewers find it to be a perfect adaptation of the source material, while others appreciate the film's exploration of toxic relationships and the lengths people will go to for revenge. Overall, "Gone Girl" is seen as a captivating and unforgettable cinematic experience.</t>
+          <t>"Gone Girl" is a dark and twisted thriller that explores the complexities of marriage and relationships. The film follows the disappearance of Amy Dunne and the suspicion that falls on her husband, Nick. With a mix of suspense, manipulation, and unexpected twists, "Gone Girl" keeps viewers on the edge of their seats. The standout performance by Rosamund Pike as Amy Dunne is chilling and captivating. Overall, "Gone Girl" is a gripping and thought-provoking film that delves into the darker side of human nature and relationships.</t>
         </is>
       </c>
       <c r="I61" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J61" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K61" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L61" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M61" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="N61" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>- psychological - thriller - dark - twisted - manipulative - suspenseful - intense - chilling - complex - captivating - disturbing - shocking - powerful - gripping - deceitful - enthralling - enigmatic - enraging - thought-provoking - provocative - masterful - suspense - paranoia - obsession - control - deception - betrayal - revenge - marriage - relationship - mystery - crime - drama - cat-and-mouse - cat - power - manipulation - sociopath - psychopath - identity - truth - lies - secrets - obsession - control - entrapment - entanglement - enthralling - enthralling - enthralling - enthralling - enthralling - enthralling - enthralling - enthralling - enthr</t>
+          <t>- psychological - thriller - dark - twisted - manipulative - suspenseful - intense - complex - chilling - disturbing - captivating - enthralling - shocking - powerful - thought-provoking - suspense - mystery - deceitful - revengeful - masterful - engrossing - compelling - intricate - diabolical - enigmatic - enraging - provocative - mesmerizing - intricate - clever - calculated - thrilling - entangling - gripping - cynical - sardonic - hilarious - absurd - anti-romance - tawdry - nightmarish - tragicomic - sleek - slick - technical - absorbing - isolating - detached - mysterious - enigmatic - diabolical - enraging - provocative - mesmerizing - intricate - clever - calculated</t>
         </is>
       </c>
       <c r="P61" t="n">
@@ -5478,7 +5478,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>La La Land is a film that has divided audiences, with some finding it to be a magical and uplifting experience, while others have been left feeling depressed and disappointed. The movie, directed by Damien Chazelle, follows the intertwined lives of Mia, an aspiring actress, and Sebastian, a passionate jazz musician, as they navigate their dreams and love in the city of Los Angeles. The film is praised for its enchanting story, captivating performances by Emma Stone and Ryan Gosling, mesmerizing musical numbers, and vibrant cinematography. Despite its mixed reviews, La La Land continues to be a favorite for many, evoking a range of emotions from happiness to sadness, and leaving a lasting impact on viewers.</t>
+          <t>La La Land is a film that evokes a wide range of emotions from viewers, from pure magic to deep sadness. It is a celebration of dreams and love, set against the backdrop of Los Angeles. The film follows the intertwined lives of Mia, an aspiring actress, and Sebastian, a passionate jazz musician. With captivating performances, mesmerizing musical numbers, and vibrant cinematography, La La Land is a cinematic gem that leaves a lasting impact on those who watch it. Despite its bittersweet ending, the film continues to be a favorite for many, invoking feelings of joy, nostalgia, and heartbreak.</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -5501,7 +5501,7 @@
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>- enchanting - charming - magical - bittersweet - emotional - impactful - mesmerizing - captivating - vibrant - celebratory - nostalgic - romantic - breathtaking - electric - sublime - bold - rewarding - joyous - melancholic - beautiful - triumphant - hopeful - tragic - flawless - stunning - flawless - stunning - flawless - stunning - flawless - stunning - flawless - stunning - flawless - stunning - flawless - stunning - flawless - stunning - flawless - stunning - flawless - stunning - flawless - stunning - flawless - stunning - flawless - stunning - flawless - stunning - flawless - stunning - flawless - stunning - flawless - stunning - flawless - stunning - flawless - stunning - flawless - stunning - flawless - stunning - flawless - stunning - flawless - stunning - flawless - stunning</t>
+          <t>- magical - emotional - impactful - bittersweet - mesmerizing - joyous - melancholic - romantic - nostalgic - vibrant - celebratory - enchanting - captivating - sublime - breathtaking - electric - tender - bold - rewarding - beautiful - triumphant - dreamy - hopeful - dramedy - tragic - catchy - flawless - stunning - amazing - goddamn - incredible - flawless - stunning - amazing - goddamn - incredible - flawless - stunning - amazing - goddamn - incredible - flawless - stunning - amazing - goddamn - incredible - flawless - stunning - amazing - goddamn - incredible - flawless - stunning - amazing - goddamn - incredible - flawless - stunning - amazing - goddamn - incredible - flawless - stunning - amazing - goddamn -</t>
         </is>
       </c>
       <c r="P62" t="n">
@@ -5560,7 +5560,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Poor Things is a visually stunning and audaciously strange film that explores themes of female empowerment, sexuality, and self-discovery. The movie follows Bella Baxter, a woman with the brain of a baby, as she navigates a world filled with societal expectations and male fantasies. With standout performances from Emma Stone and Mark Ruffalo, the film delves into themes of feminism, liberation, and the complexities of womanhood. However, some viewers have criticized the film for its male gaze and shallow exploration of important issues. Overall, Poor Things is a polarizing and provocative film that challenges traditional narratives and expectations.</t>
+          <t>Poor Things is a visually stunning and audaciously strange film that explores themes of female empowerment and sexuality. It follows the story of Bella Baxter, a woman with the brain of a child, as she navigates through a world filled with absurdity and tragedy. The film has received mixed reviews, with some praising its unique aesthetic and performances, while others criticize its male gaze and problematic themes. Overall, Poor Things is a polarizing and thought-provoking cinematic experience.</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -5576,14 +5576,14 @@
         <v>5</v>
       </c>
       <c r="M63" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N63" t="n">
         <v>6</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>- barbie - mentally ill - Bella - loca - childlike wonder - male fantasy - female empowerment - feminism - clit - feelings - pleasurable sex - socialist - lesbian - whore - mark ruffalo - battles - horniest soldier - barbie in the real world - sex in movies - funny - thoughtful - gorgeous - feminist lens - autism - diagnosis - sick to my stomach - grotesque - perverse - fairy tale - consent - uncomfortable - sexy baby - horny - fop - feminist - empowerment - objectification - humanity - philosophy - reality - balance - adventurous life - settled life - Barbie after gynecologist - Barbie for Björk listeners - child pornography - sexual freedom - promiscuity - infantilizing - exploitation - consent -</t>
+          <t>- barbie - mentally ill - Bella - loca - childlike wonder - male fantasy - female empowerment - feminism - clit - feelings - pleasurable sex - socialist lesbian whore - mark ruffalo - horny soldier - barbie in the real world - sex in movies - funny - thoughtful - gorgeous - feminist lens - autism - gynecologist - Barbie for Björk listeners - objecting - misogyny - magic - Lalo Salamanca - menstrual blood - male perspective feminism - empowerment - grotesque - perverse - fairy tale - consent - baby piloting - masturbation - sexy baby - modern cartoon parable - fathers and daughters - women - husbands and wives - lovers and enemies - sex workers - clients - cruelty - humanity - philosophy - reality</t>
         </is>
       </c>
       <c r="P63" t="n">
@@ -5642,7 +5642,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Eternal Sunshine of the Spotless Mind is a deeply emotional and thought-provoking film that explores the complexities of love, memory, and relationships. With stellar performances from Jim Carrey and Kate Winslet, the movie delves into the pain and beauty of heartbreak, leaving viewers with a sense of introspection and reflection on the nature of love and loss. The unique concept, brilliant screenplay, and surreal visuals make it a standout in the realm of romantic dramas.</t>
+          <t>Eternal Sunshine of the Spotless Mind is a deeply emotional and thought-provoking film that explores the complexities of love, memory, and relationships. With stellar performances from Jim Carrey and Kate Winslet, the movie delves into the pain and beauty of heartbreak, leaving viewers with a sense of longing and introspection. The unique concept and visual style make it a standout in the realm of romantic dramas, offering a raw and honest portrayal of human connection and the impact of lost love.</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5665,7 +5665,7 @@
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>- love - heartbreak - memories - relationships - introspective - unique - cathartic - bittersweet - emotional - raw - existential - surreal - inventive - sci-fi - romance - nostalgia - melancholy - thought-provoking - masterpiece - unforgettable - cathartic - relatable - artistic - tender - brilliant - powerful - heartbreaking - beautiful - complex - deep - moving - captivating - dreamlike - haunting - transformative - iconic - timeless - genius - original - authentic - impactful - favorite - cinematic - love story - chemistry - human nature - introspection - existentialism - metaphysical - catharsis - connection - unforgettable - masterpiece - unique - emotional rollercoaster - thought-provoking - introspective - relatable - bittersweet - cath</t>
+          <t>- introspective - emotional - unique - raw - cathartic - bittersweet - thought-provoking - heartbreaking - surreal - romantic - melancholic - existential - innovative - complex - relatable - artistic - deep - memorable - impactful - introspective - tender - brilliant - powerful - surreal - lo-fi sci-fi - tender - deconstruction - love - desire - unforgettable - favorite - brilliant - concept - screenplay - performances - powerful - unique - emotional - bittersweet - thought-provoking - heartbreaking - raw - cathartic - romantic - melancholic - existential - innovative - complex - relatable - artistic - deep - memorable - impactful - surreal - introspective - emotional - unique - raw - cathartic - bittersweet - thought-prov</t>
         </is>
       </c>
       <c r="P64" t="n">
@@ -5724,7 +5724,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Little Women, directed by Greta Gerwig, is a heartwarming and emotional adaptation of the classic novel by Louisa May Alcott. The film follows the lives of the March sisters in 19th century America, exploring themes of love, family, and ambition. With a stellar cast including Saoirse Ronan, Florence Pugh, Emma Watson, and Eliza Scanlen, the movie captures the essence of sisterhood and the struggles of growing up. Gerwig's unique storytelling approach, non-linear plot structure, and attention to detail make this adaptation a standout piece of art. The film is a beautiful and immersive experience that will make you laugh, cry, and feel a deep connection to the characters. Overall, Little Women is a must</t>
+          <t>Little Women, directed by Greta Gerwig, is a heartwarming and emotional adaptation of the classic novel by Louisa May Alcott. The film follows the lives of the March sisters in 19th century America, exploring themes of love, family, and ambition. With a stellar cast including Saoirse Ronan, Florence Pugh, Emma Watson, and Eliza Scanlen, the movie captures the essence of sisterhood and the struggles of women in that era. Gerwig's unique storytelling approach, non-linear plot structure, and attention to detail make this adaptation a standout piece of art. The film is a beautiful ode to the strength and resilience of women, leaving viewers feeling warm and nostalgic.</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5747,7 +5747,7 @@
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>- friendship - love - warmth - dreamlike - overwhelming - family - nostalgia - coming of age - emotional - feminist - adaptation - ensemble - charming - captivating - engaging - beautiful - timeless - bittersweet - comforting - immersive - nuanced - multilayered - poignant - whimsical - delightful - empowering - sentimental - authentic - resonant - impactful - mesmerizing - enchanting - relatable - touching - heartwarming - soulful - transformative - captivating - engaging - nuanced - bittersweet - empowering - resonant - impactful - mesmerizing - enchanting - relatable - touching - heartwarming - soulful - transformative</t>
+          <t>- friendship - love - warmth - dreamlike - overwhelming - family - nostalgia - adaptation - emotional - joy - beauty - feminist - ensemble - charming - captivating - engaging - immersive - comforting - bittersweet - timeless - nuanced - heartwarming - relatable - transformative - enchanting - delightful - faithful - sentimental - powerful - moving - poignant - mesmerizing - funny - heartbreak - coming of age - sisterhood - talent - artistry - elegance - grace - whimsical - whimsy - whimsical - whimsy - whimsical - whimsy - whimsical - whimsy - whimsical - whimsy - whimsical - whimsy - whimsical - whimsy - whimsical - whimsy - whimsical - whimsy - whimsical</t>
         </is>
       </c>
       <c r="P65" t="n">
@@ -5799,14 +5799,14 @@
         <v>142</v>
       </c>
       <c r="F66" t="n">
-        <v>3.82</v>
+        <v>3.85</v>
       </c>
       <c r="G66" t="n">
-        <v>1.23</v>
+        <v>1.22</v>
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Forrest Gump is a heartwarming and poignant film that follows the extraordinary life of a seemingly ordinary man named Forrest Gump. Through his eyes, viewers experience significant moments in American history, woven into a narrative that is both charming and emotional. Tom Hanks delivers a masterful performance as Forrest, making the character unforgettable. Despite some criticisms about its portrayal of history and politics, the film's storytelling and messages of love and resilience make it a classic that resonates with many viewers.</t>
+          <t>Forrest Gump is a heartwarming and emotional journey through the life of a seemingly ordinary man who finds himself at the center of significant historical events. Tom Hanks delivers a masterful performance as Forrest, weaving humor and sentiment with finesse. The film explores themes of destiny, love, and resilience against a nostalgic backdrop, creating a cinematic triumph. While some may criticize its portrayal of American history and politics, many find it to be a beloved classic that resonates deeply with audiences. With a beautiful story, amazing acting, and a memorable soundtrack, Forrest Gump continues to touch the hearts of viewers and remains a timeless favorite.</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -5829,7 +5829,7 @@
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>- heartwarming - emotional - historical - iconic - Tom Hanks - coming-of-age - charming - whimsical - bittersweet - classic - American history - feel-good - poignant - storytelling - Oscar winner - heartwarming - inspiring - captivating - memorable - beautiful - saccharine - satire - critique - propaganda - divisive - warm - fuzzy - whimsical - entertaining - character study - masterclass - idealism - nostalgia - love - resilience - destiny - humor - sentiment - underdeveloped - simplistic - cynical - Boomer fantasy - saccharine - self-mythologizing - American agit-prop - metahistorical romance - folktale - iconic - heartwarming - heartwarming - heartwarming - heartwarming</t>
+          <t>- heartwarming - emotional - historical - iconic - Tom Hanks - coming-of-age - charming - whimsical - bittersweet - classic - feel-good - poignant - captivating - inspiring - American history - storytelling - saccharine - satire - critique - propaganda - Boomer fantasy - nostalgia - Oscar winner - cinematography - soundtrack - character study - masterclass - humor - sentiment - resilience - destiny - love - idealism - moral - therapy - life lessons - iconic quotes - heartwarming journey - timeless - beloved - tearjerker - whimsy - feel-good - charming - heartwarming - emotional - historical - iconic - Tom Hanks - coming-of-age - captivating - inspiring - American history - storytelling - satire - critique - Bo</t>
         </is>
       </c>
       <c r="P66" t="n">
@@ -5888,7 +5888,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Everything Everywhere All at Once is a visually dazzling, emotionally resonant, and wildly imaginative film that explores themes of family, identity, and the multiverse. With a mix of martial arts, comedy, and heartfelt moments, the movie keeps audiences engaged and entertained throughout. The performances, particularly from Michelle Yeoh, are praised, and the film's unique storytelling approach is both ambitious and successful. Despite some mixed reviews, many viewers find it to be a groundbreaking and unforgettable cinematic experience.</t>
+          <t>Everything Everywhere All at Once is a visually stunning, emotionally resonant, and wildly imaginative film that combines elements of martial arts, sci-fi, comedy, and family drama. With a strong performance from Michelle Yeoh and a unique storytelling approach, the movie explores themes of multiverses, family relationships, and the meaning of life. Despite some divisive opinions, the film has been praised for its creativity, humor, and heartfelt moments, making it a must-watch for fans of bold and original cinema.</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -5911,7 +5911,7 @@
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>- multiverse - martial arts - family drama - visually dazzling - heartfelt - creative - ambitious - original - funny - emotional - chaotic - kinetic - daring - expertly choreographed - endlessly creative - laugh-out-loud funny - genuine emotional core - intelligent filmmaking - lowbrow humor - existential - philosophical - action-packed - moving - thought-provoking - authentic Asian identity - Michelle Yeoh - Stephanie Hsu - Ke Huy Quan - everything bagel - Reddit - Swiss Army Man - Rick and Morty - Douglas Adams - Wong Kar-Wai - Ratatouille - emotional payoffs - grounded - breathless climax - acrobatic action scenes - heartfelt moments - family rifts - multiverse gimmick - visually dynamic - technically</t>
+          <t>- multiverse - martial arts - family drama - visually dazzling - heartfelt - creative - original - ambitious - funny - emotional - chaotic - kinetic - daring - expertly choreographed - endlessly creative - laugh-out-loud funny - genuine emotional core - intelligent filmmaking - lowbrow humor - existential - thought-provoking - visionary - masterpiece - symphony of chaos - moving - authentic Asian identity - Michelle Yeoh - Jamie Lee Curtis - Swiss Army Man - Rick and Morty - Douglas Adams - Wong Kar-Wai - Ratatouille - everything bagel - generational trauma - tiger mom - acceptance - love - family - action-packed - complex - powerful - simple - phenomenal editing - affirming - unique storytelling - mind-bending - roller</t>
         </is>
       </c>
       <c r="P67" t="n">
@@ -5970,7 +5970,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Interstellar is a visually stunning and emotionally heavy film that explores themes of love, time, and survival. The movie follows a team of explorers traveling through a wormhole in space to ensure humanity's survival. With breathtaking visuals, a powerful score, and strong performances, the film takes audiences on a journey through time and space. While some viewers found it to be a masterpiece and a cinematic achievement, others criticized its over-explanation and plot inconsistencies. Overall, Interstellar is a thought-provoking and ambitious film that leaves a lasting impact on its viewers.</t>
+          <t>Interstellar is a visually stunning and emotionally heavy film that explores themes of love, time, and survival. The movie follows a team of explorers traveling through a wormhole in space to ensure humanity's survival. With breathtaking visuals and a powerful score, the film delves into the relationship between a father and daughter, the mysteries of the universe, and the power of love. Despite some flaws and mixed reviews, Interstellar remains a cinematic masterpiece that leaves a lasting impact on viewers.</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -5993,7 +5993,7 @@
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>- emotional - visually stunning - ambitious - masterpiece - cathartic - thought-provoking - intense - sci-fi - epic - Nolan-esque - powerful - awe-inspiring - complex - love transcending time - breathtaking - rollercoaster - profound - space opera - family drama - visually monumental - mind-enriching - human odyssey - poetic - overwhelming - cosmic awe - muddled - aggravating - technological - iconic - intense - phenomenal</t>
+          <t>- emotional - visually stunning - ambitious - cathartic - heartbreaking - intense - thought-provoking - masterpiece - sci-fi - epic - powerful - profound - ambitious - visually breathtaking - rollercoaster - compelling - mesmerizing - awe-inspiring - transcendent - complex - overwhelming - beautiful - intense - emotional rollercoaster - visually stunning - ambitious - masterpiece - breathtaking - powerful - compelling - profound - thought-provoking - emotional - visually stunning - intense - epic - cathartic - heartbreaking - visually breathtaking - ambitious - masterpiece - compelling - powerful - profound - thought-provoking - emotional - visually stunning - intense - epic - cathartic - heartbreaking - visually breathtaking - ambitious - masterpiece - compelling - powerful - profound - thought-provoking - emotional</t>
         </is>
       </c>
       <c r="P68" t="n">
@@ -6052,7 +6052,7 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Dune is a visually stunning and meticulously crafted adaptation of the iconic science fiction novel, filled with intricate world-building and epic scale. The film follows Paul Atreides, a young man with a great destiny, as he navigates dangerous political intrigue on a treacherous planet. While some viewers found the film to be a bit slow and lacking in emotional depth, others praised its immersive experience and faithful adaptation of the source material. With a mix of humor, awe, and admiration, Dune has left audiences eagerly anticipating the next installment.</t>
+          <t>Dune is a visually stunning and meticulously crafted adaptation of the beloved sci-fi novel, featuring a vast world filled with intricate details and epic scale. The film follows Paul Atreides, a young man with a great destiny, as he navigates dangerous political intrigue and battles for control of the universe's most precious resource. While some viewers found the film to be a bit slow and lacking in emotional depth, others praised its methodical world-building and impressive visuals. Overall, Dune is a polarizing but ambitious cinematic experience that leaves audiences eagerly anticipating the next installment.</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -6075,7 +6075,7 @@
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>- chosen one - dehydrated - orange - zendaya dreams - TikTok - documentary-like - sand on titties - methodical worldbuilding - candy crush - PAUL - Anakin - Hans Zimmer music video - box moaning - monumental cinematic achievement - timothee and zendaya - Jason Momoa action star - industrial design - thousand-yard-stares - The Sandlot - global worming - Desert power - enormous scale - brutalist spectacle - psychedelia - floating fatass Baron Harkonnen - duncan idaho - dilfs - alien language - boring - epic - wet dreams - worm - face stroking - cinematic symphony - tragic love story - hyped for Part 2 - thanksgiving movie - Freme</t>
+          <t>- chosen one - dehydrated - orange - zendaya dreams - Timothée Chalamet - documentary-like - sand on titties - worldbuilding - candy crush - PAUL - Anakin - Hans Zimmer music video - box moaning - monumental cinematic achievement - timothee chalamet fighting - Jason Momoa - industrial design - thousand-yard-stares - kid's parents - global warming - desert power - enormous scale - brutalist spectacle - psychedelia - worm eating sand - floating fatass Baron Harkonnen - ms. lawton - duncan idaho - dilfs - alien language - boring - epic - wet dreams - floating fatass Baron Harkonnen - sandworm - slow-motion Zendaya - snooze</t>
         </is>
       </c>
       <c r="P69" t="n">
@@ -6134,7 +6134,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Spider-Man: Into the Spider-Verse is hailed as the best Spider-Man film ever made, with stunning animation that captivates viewers. The film is praised for its creativity, humor, and understanding of the character of Spider-Man. Fans appreciate the diverse representation of Spider-People from different dimensions and the fresh take on the superhero genre. The movie's visuals, soundtrack, and storytelling are all highlighted as exceptional, making it a standout in the world of animated and superhero films.</t>
+          <t>Spider-Man: Into the Spider-Verse is hailed as the best Spider-Man film ever made, with stunning animation that captivates viewers. The film is praised for its creativity, humor, and understanding of the character of Spider-Man. It reinvigorates the superhero genre and is considered a masterpiece in animation. The diverse cast of Spider-People adds depth to the story, making it a visually breathtaking and emotionally resonant experience. The film's soundtrack and score are also highlighted as exceptional, contributing to its overall impact. Overall, Spider-Man: Into the Spider-Verse is celebrated as a groundbreaking and unforgettable cinematic achievement.</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -6157,7 +6157,7 @@
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>- best spider-man film - funny - creative - wonderfully animated - understanding of the character - visually stunning - visually daring - visually inventive - visually unique - visually vibrant - visually breathtaking - visually original - visually striking - visually mesmerizing - visually refreshing - visually fresh - visually kinetic - visually jaw-dropping - visually distinctive - visually influential - visually well-drawn - visually comic book-like - visually immersive - visually engaging - visually expressive - visually colorful - visually textured - visually rhythmic - visually expressive - visually psychedelic - visually Lichtenstein-esque - visually pop art-stylings - visually near-psychedelic - visually dense - visually detailed - visually vibrant - visually beautiful - visually fresh - visually inventive - visually original - visually stunning - visually mesmerizing - visually</t>
+          <t>- groundbreaking - visually stunning - creative - understanding - funny - animated - heroin-style animation - best Spider-man movie - LGBTQ representation - talented - reinvigorates genre - Spider-Man Noir - sequel anticipation - overwhelming - John Mulaney cameo - colors - action sequences - Spider-Ham - animated Bill Sienkiewicz paintings - emotional - Spider-Man Noir stand-alone desire - visually daring - animated superhero movie preference - What's Up Danger scene - coming of age angle - relatable - visually inventive - visually interesting - visually breathtaking - visually unique - visually striking - visually fresh - visually vibrant - visually original - invigorating - jaw-dropping - top-tier storytelling - original - imaginative - vibrant - kinetic - well-drawn - endlessly relatable - beloved</t>
         </is>
       </c>
       <c r="P70" t="n">
@@ -6216,7 +6216,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>Inception is a visually stunning and complex heist film that delves into the subconscious mind. With a brilliant cast and masterful direction from Christopher Nolan, the movie explores themes of guilt, grief, and the power of dreams. The intricate plot, accompanied by Hans Zimmer's iconic score, keeps viewers on the edge of their seats. Despite some criticisms of the dialogue and pacing, Inception remains a thought-provoking and unforgettable cinematic experience.</t>
+          <t>Inception is a complex and visually stunning film that follows Dom Cobb, a master thief who enters people's dreams to steal their secrets. With a mix of action, drama, and mind-bending concepts, the movie explores themes of guilt, grief, and the power of dreams. Christopher Nolan's meticulous attention to detail and Hans Zimmer's iconic score create a captivating cinematic experience that continues to intrigue audiences. The film's ambiguous ending leaves viewers questioning reality and the nature of dreams. Overall, Inception is a brilliant and unrivaled piece of filmmaking that blends heist elements with science fiction concepts to create a cerebral pop-masterpiece.</t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -6239,7 +6239,7 @@
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>- complex - heist - science fiction - study - man - free - past - cerebral - thought-provoking - layered - story-telling - sumptuous - aesthetics - flawless - editing - sound design - effects - musical score - pitch-perfect - cast - brilliant - unrivaled - filmmaking - rent free - gay - lesbian - solidarity - fanfic - totem - spinning - dreaming - reality - masterpiece - gay - homoerotic - personal - technical feat - collaborative vision - design - fake worlds - feelings - workaholic - craft - time - loved ones - fabricated - simulated - catharsis - therapy - film editing - blown away - trust - people - dreams - lucid dreaming - filmmaking - remarkable - admiration</t>
+          <t>- complex - heist - science fiction - study - cerebral - thought-provoking - layered - enthralling - brilliant - filmmaking - rent-free - gay - lesbian - fanfic - spinning - dream - reality - masterpiece - personal - technical feat - collaborative - visionary - design - catharsis - homoerotic - personal - emotional - ambitious - action - dreamy - lucid - intense - surreal - ambiguous - creative - ambitious - multi-layered - stunning - orgasmic - neat - boy boss - gaslighter - blockbuster - mind-bending - pop entertainment - stylish - artful - emotional depth - action extravaganza - tragic - flashy - therapy - love - zingy - sad - morbidly obsessed - modern</t>
         </is>
       </c>
       <c r="P71" t="n">
@@ -6291,14 +6291,14 @@
         <v>133</v>
       </c>
       <c r="F72" t="n">
-        <v>4.78</v>
+        <v>4.77</v>
       </c>
       <c r="G72" t="n">
-        <v>0.47</v>
+        <v>0.48</v>
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Parasite is a genre-defying masterpiece that delves into the complexities of class divide and societal issues. With a gripping narrative and exceptional performances, it keeps viewers on the edge of their seats. Director Bong Joon-ho's unique storytelling and social commentary make it a must-see film that leaves a lasting impact.</t>
+          <t>Parasite is a gripping and thrilling film that delves into the complexities of class divide and societal issues. With masterful storytelling and brilliant performances, it keeps the audience on the edge of their seats. The film has been hailed as a masterpiece, with its unique blend of genres and thought-provoking themes. It's a must-see that leaves a lasting impact on viewers.</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -6321,7 +6321,7 @@
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>- thriller - darkly-chilling - operatic - Shakespearean - tragic - satirical - farce - horror - comedic - nuanced - merciless - compelling - genre-defying - masterful - intoxicating - incredible - brilliant - social - commentary - thought-provoking - suspenseful - gripping - unpredictable - jaw-dropping - edge-of-your-seat - depressing - fun - mesmerizing - captivating - must-see - timeless - gripping - unique - genre-bending - mind-blowing - unbelievable - gripping - best-of-the-decade - award-winning - thought-provoking - social-inequity - class-divide - masterful-cinematography - metaphorical - shocking - mesmerizing - captivating - thrilling - intense - gripping -</t>
+          <t>- gripping - thrilling - intense - thought-provoking - satirical - darkly comedic - genre-defying - social commentary - masterful - nuanced - suspenseful - twisty - impactful - mesmerizing - engaging - brilliant - clever - layered - powerful - unforgettable - must-see - cinematic masterpiece - award-winning - unique - shocking - anxiety-inducing - jaw-dropping - edge-of-your-seat - compelling - entertaining - dark - absurd - metaphorical - societal critique - class warfare - symbolic - mesmerizing - immersive - captivating - genius - defining - gripping - unpredictable - unsettling - mesmerizing - darkly humorous - intense - gripping - shocking - brilliant - thought-provoking - captivating - thrilling - genre-bending - impactful - unforgettable - must</t>
         </is>
       </c>
       <c r="P72" t="n">
@@ -6380,7 +6380,7 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>- Joker is a divisive film that has been both praised and criticized. It features a standout performance by Joaquin Phoenix as Arthur Fleck, a mentally troubled comedian who transforms into the iconic villain, Joker. The film is visually stunning with impressive cinematography and a chilling music score. However, it has been criticized for its shallow exploration of societal issues and its lack of originality in terms of its themes and character development. Overall, Joker is a dark and unsettling portrayal of a descent into madness, but it falls short of delivering a truly impactful message.</t>
+          <t>Joker is a divisive film that has been praised for Joaquin Phoenix's performance and its visual elements, but criticized for its lack of depth and handling of sensitive issues. Some viewers found it to be a bold reinvention of superhero cinema, while others felt it was a shallow attempt at social commentary. The film has sparked controversy and mixed reactions, with some calling it a masterpiece and others labeling it as pretentious and misguided. Ultimately, Joker is a film that has left audiences with strong and varied opinions.</t>
         </is>
       </c>
       <c r="I73" t="n">
@@ -6403,7 +6403,7 @@
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>- vapid - shallow - disappointing - predictable - hollow - misguided - pretentious - controversial - unsettling - disturbing - nihilistic - grim - violent - intense - chilling - fascinating - remarkable - fascinating - fascinating - fascinating - fascinating - fascinating - fascinating - fascinating - fascinating - fascinating - fascinating - fascinating - fascinating - fascinating - fascinating - fascinating - fascinating - fascinating - fascinating - fascinating - fascinating - fascinating - fascinating - fascinating - fascinating - fascinating - fascinating - fascinating - fascinating - fascinating - fascinating - fascinating - fascinating - fascinating - fascinating - fascinating - fascinating - fascinating - fascinating - fascinating - fascinating - fascinating - fascinating - fascinating - fascinating - fascinating - fascinating - fascinating - fascinating - fascinating - fascinating - fascinating - fascinating - fascinating - fascinating - fascinating - fascinating -</t>
+          <t>- vapid - shallow - disappointing - predictable - hollow - misguided - pretentious - controversial - unsettling - grim - nihilistic - intense - chilling - remarkable - fascinating - fascinating - interesting - cinema - crime thriller - visually stunning - impressive - remarkable - captivating - intriguing - unsettling - tour de force - remarkable - fascinating - unsettling - captivating - interesting - cinema - visually stunning - impressive - remarkable - captivating - intriguing - unsettling - captivating - interesting - cinema - visually stunning - impressive - remarkable - captivating - intriguing - unsettling - captivating - interesting - cinema - visually stunning - impressive - remarkable - captivating - intriguing - unsettling - captivating - interesting - cinema - visually stunning - impressive - remarkable - captivating - intriguing - unsettling - captivating - interesting - cinema - visually stunning</t>
         </is>
       </c>
       <c r="P73" t="n">
@@ -6462,7 +6462,7 @@
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>Pulp Fiction is a cult classic that has left a lasting impact on cinema history. With its sharp dialogue, colorful characters, and unique storytelling, it continues to engage and entertain audiences. While some find it to be a masterpiece and a landmark in cinematic history, others criticize it for its reliance on racial provocations and stereotypes. The film is known for its iconic characters, memorable scenes, and witty dialogue, making it a must-watch for any film enthusiast.</t>
+          <t>Pulp Fiction is a cult classic that has left a lasting impact on cinema history. With its sharp dialogue, colorful characters, and unique storytelling, Quentin Tarantino's masterpiece continues to captivate audiences. The film is a mix of different genres, filled with important life lessons and iconic moments. While some viewers may find it overrated or boring, others praise it as a bona-fide landmark in cinematic history. The movie is known for its memorable characters, witty dialogue, and interconnected storylines that come together in a masterpiece of filmmaking. Whether you love it or hate it, Pulp Fiction remains a must-watch for any cinephile.</t>
         </is>
       </c>
       <c r="I74" t="n">
@@ -6485,7 +6485,7 @@
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>- iconic - dialogue-driven - interconnected - cult classic - groundbreaking - pop culture - masterpiece - memorable characters - dark humor - original - Quentin Tarantino - rewatchable - kaleidoscopic narrative - non-linear - brilliant screenplay - influential - witty - quotable - violent - unique - Tarantinothon - cinematic history - character-driven - intense - edgy - classic - timeless - interconnected stories - darkly comedic - brilliant dialogue - iconic scenes - unforgettable - impactful - genius - electrifying - thought-provoking - legendary - cinematic landmark - masterstroke - cult favorite - Tarantino's best - character development - engaging - entertaining - witty humor - clever - unconventional - stylish - vibrant - dynamic - intense dialogue - character-driven storytelling - iconic moments - memorable</t>
+          <t>- iconic - groundbreaking - witty - dialogue-driven - interconnected - pop culture - masterpiece - cult classic - rewatchable - memorable characters - kaleidoscopic narrative - dark humor - violent - original - Quentin Tarantino - Samuel L. Jackson - John Travolta - Uma Thurman - Bruce Willis - Ving Rhames - iconic quotes - non-linear - brilliant screenplay - influential - classic - Tarantino style - unique storytelling - character-driven - intense - edgy - clever - cinematic history - unforgettable - brilliant dialogue - cultural impact - masterstroke - genius - electrifying - thought-provoking - award-winning - legendary - timeless - quotable - interconnected stories - character development - iconic scenes - cinematic landmark - must-watch - brilliant direction - witty humor -</t>
         </is>
       </c>
       <c r="P74" t="n">
@@ -6544,11 +6544,11 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Get Out is a smart, thought-provoking, and terrifying horror film that cleverly blends social commentary with suspense. Directed by Jordan Peele, the film follows a black man who visits his white girlfriend's parents and uncovers sinister secrets. With brilliant performances, symbolism, and a twist that keeps viewers on edge, Get Out is hailed as a modern classic in the horror genre. The film's exploration of race relations and subtle metaphors make it a must-watch for audiences looking for a unique and chilling cinematic experience.</t>
+          <t>Get Out is a smart, thought-provoking, and intense horror film that cleverly blends genres and delivers a powerful social commentary. Directed by Jordan Peele, the film follows a black man who visits his white girlfriend's parents and uncovers sinister secrets. With brilliant performances, symbolism, and writing, Get Out keeps viewers on edge and leaves a lasting impact. The film's unsettling themes and twists make it a must-watch, showcasing Peele's talent as a filmmaker. White people are portrayed as terrifying in this film, with moments that are both scary and thought-provoking. Overall, Get Out is a masterful and original horror movie that continues to impress with each viewing.</t>
         </is>
       </c>
       <c r="I75" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J75" t="n">
         <v>0</v>
@@ -6560,14 +6560,14 @@
         <v>0</v>
       </c>
       <c r="M75" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="N75" t="n">
         <v>10</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
-          <t>- social commentary - horror - satire - intense - psychological - suspenseful - thought-provoking - smart - original - layered - brilliant - genius - political - calculated - visually stunning - impeccably acted - funny - iconic - psychopathic - intense ending - satisfying - rewatchable - bold - important - genre-bending - masterful - creepy - entertaining - twist - unsettling - suspense - symbolism - foreshadowing - twisty - clever - unique - thrilling - effective - smart horror - metaphors - scary - satirical - genius directorial debut - social critique - disturbing - intense suspense - thought-provoking - smart dialogue - racial themes - terrifying - over-hyped - depression - 5 stars - amazing - masterpiece - beautiful - theater</t>
+          <t>- smart - clever - thought-provoking - intense - suspenseful - satirical - original - scary - funny - political - intelligent - visually stunning - impeccably acted - iconic - psychopathic - brilliant - genius - bold - important - bold - fearless - entertaining - layered - suspenseful - mysterious - unsettling - symbolic - eerie - creepy - disturbing - suspenseful - thrilling - effective - entertaining - smart - intense - terrifying - satirical - unique - masterly - commendable - smart - scary - smart - smart - smart - smart - weird - terrifying - amazing - 5 star - beautiful - masterpiece</t>
         </is>
       </c>
       <c r="P75" t="n">
@@ -6622,7 +6622,7 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>The Batman is a visually stunning and gritty take on the iconic superhero, with Robert Pattinson delivering a fantastic performance as a brooding and disturbed Bruce Wayne. The film delves into the darker aspects of Gotham City, with a focus on detective work and a complex, atmospheric score. The portrayal of the Riddler as a twisted and obsessive villain adds depth to the story, while Catwoman brings a sense of mystery and allure. Overall, The Batman is a refreshing and ambitious entry in the superhero genre, with influences from classic crime thrillers like Se7en and Zodiac.</t>
+          <t>The Batman is a dark, gritty, and visually stunning film that showcases a unique portrayal of Bruce Wayne as a disturbed and gothic figure. The movie delves into the detective side of Batman, with a focus on clues and investigation. The Riddler is portrayed as a twitch streamer, adding a modern twist to the character. The film has been praised for its atmospheric cinematography, haunting score, and standout performances from Robert Pattinson, Zoe Kravitz, and Paul Dano. Overall, The Batman is seen as a refreshing take on the superhero genre, blending elements of noir, thriller, and crime drama to create a compelling and immersive experience.</t>
         </is>
       </c>
       <c r="I76" t="n">
@@ -6645,7 +6645,7 @@
       </c>
       <c r="O76" t="inlineStr">
         <is>
-          <t>- disgusting - goth - detective - virgin - fantastic - sexy - emo - dusty - files - gayest - redditor - catwoman - delightful - freak - silly - español - gruff - emos - goths - whores - pacing issues - twitch streamer - Zodiac - Se7en - Saw - virgin - growly - eyeliner - bold - gotham city - pacing issues - cranberries - emo - Black Panther - Disintegration - Joy Division - shoutout - pacing issues - Zodiac - Se7en - Saw - detective - noir - immersive - engrossing - Arkham games - brooding - dark - gritty - haunting - stunning - beautiful - breathtaking - masterful - intricate - best - comic book - thrilling</t>
+          <t>- disgusting - goth - emo - detective - sexy - gay - hilarious - thrilling - dark - gritty - immersive - engrossing - noir - creepy - intense - masterful - ambitious - conflicted - stunning - atmospheric - psychological - breathtaking - chilling - haunting - brooding - beautiful - complex - interesting - intricate - transformative - hopeful - sprawling - ambitious - muscular - monotonous - vague</t>
         </is>
       </c>
       <c r="P76" t="n">
@@ -6704,7 +6704,7 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>Inglourious Basterds is a Quentin Tarantino masterpiece that follows a group of Jewish-American soldiers on a mission to kill Nazis during World War II. With iconic performances from Christoph Waltz and Brad Pitt, the film is filled with tension, humor, and revenge. The film's unique storytelling and dialogue in multiple languages make it a standout in Tarantino's filmography. The final scene, where a character declares it might be his masterpiece, is a mic drop moment that solidifies the film's impact. Overall, Inglourious Basterds is a thrilling and thought-provoking take on history and vengeance.</t>
+          <t>Inglourious Basterds is a Quentin Tarantino masterpiece that follows a group of Jewish-American soldiers on a mission to kill Nazis during World War II. With iconic performances from Christoph Waltz and Brad Pitt, the film is filled with tension, humor, and revenge. The film's unique storytelling and dialogue in multiple languages make it a standout in Tarantino's filmography, with memorable scenes and a powerful ending that solidifies it as a fan favorite.</t>
         </is>
       </c>
       <c r="I77" t="n">
@@ -6727,7 +6727,7 @@
       </c>
       <c r="O77" t="inlineStr">
         <is>
-          <t>- revenge - historical fantasy - dialogue - multilingual - iconic - masterpiece - comedy - violence - scalp - duolingo - breathtaking - burning - vengeance - cinema - intense - character writing - authentic - stylization - morally complex - villain - tension - comfort film - Christoph Waltz - Brad Pitt - ensemble cast - Quentin Tarantino - WWII - fantasy - brutality - language - satire - representation - hatred - violence - intolerance - masterful - storytelling - pacing - tension - iconic scenes - comfort - issues - Hans Landa - Christoph Waltz - villain - character - dialogue - multilingual - iconic - masterpiece - comedy - violence - scalp - duolingo - breathtaking - burning - vengeance - cinema - intense - character writing - authentic - stylization -</t>
+          <t>- revenge - historical fantasy - dialogue - languages - masterpiece - iconic - comedic gold - historically accurate - lung capacity - breathtaking - burning it down - cultural trauma - amnesia - torture - Nazi scalps - duolingo king - farewell to Nazi balls - Gorlami - Christoph Waltz - killing Nazis - vengeance - scalp - comfort film - cinema - final girl - poetic cinema - WWII - spaghetti western - violence - tension - iconic performance - comfort - issues - Hans Landa - Schurken - Kevin Bacon</t>
         </is>
       </c>
       <c r="P77" t="n">
@@ -6786,7 +6786,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Jojo Rabbit is a film that defies expectations, blending humor and heart in a way that only Taika Waititi can. Despite the controversial subject matter, the film manages to be both hilarious and moving, with standout performances from the cast. While some may find the tonal shifts jarring, others appreciate the unique perspective on a dark period in history. Overall, Jojo Rabbit is a cinematic masterpiece that leaves a lasting impact on viewers.</t>
+          <t>- Jojo Rabbit is a film that defies expectations, blending humor and heart in a way that only Taika Waititi can. Despite the controversial subject matter, the film manages to be both hilarious and moving, with standout performances from the cast. The tonal shifts may be sharp for some, but overall, it's a breath of fresh air and a unique take on a difficult topic. Waititi's direction and writing shine through, making Jojo Rabbit a must-watch film of 2019.</t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -6809,7 +6809,7 @@
       </c>
       <c r="O78" t="inlineStr">
         <is>
-          <t>- satirical - heartwarming - unexpected - passionate - funny - emotional - unique - transformative - brilliant - moving - whimsical - absurd - entertaining - daring - poignant - balanced - sincere - surreal - mixed feelings - disappointing</t>
+          <t>- satirical - heartwarming - unexpected - passionate - funny - emotional - fresh - transformative - brilliant - moving - absurd - comedic - whimsical - profound - entertaining - balanced - sincere - surreal - dexterous - warm - hopeful - eccentric - inspiring - genuine - mixed feelings - disappointing - hilarious - emotional - satirical - witty - charming - controversial - thought-provoking - unique - clever - whimsical - touching - powerful - poignant - impressive - daring - heartfelt - captivating - engaging - well-crafted - imaginative - bold - inventive - charming - delightful - impactful - divisive - complex - nuanced - daring - risky - memorable - endearing - heartwarming - hilarious - satirical - emotional - surprising - disappointing - funny - heart</t>
         </is>
       </c>
       <c r="P78" t="n">
@@ -6868,7 +6868,7 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>1917 is a visually stunning and technically impressive war film that immerses viewers in the brutal realities of World War I. The use of long takes and seamless editing creates a sense of urgency and tension throughout the film. While some found the narrative to be lacking depth, the performances, cinematography, and score were widely praised. Directed by Sam Mendes and featuring standout work from cinematographer Roger Deakins, 1917 is a cinematic achievement that leaves a lasting impact on audiences.</t>
+          <t>1917 is a visually stunning and technically impressive war film that immerses viewers in the brutal realities of World War I. The use of long takes and continuous shots, expertly crafted by Roger Deakins, creates a sense of urgency and tension throughout the film. While some may find the narrative lacking depth, the film's focus on the harrowing journey of two soldiers on a mission is both gripping and emotional. With outstanding performances, breathtaking cinematography, and a powerful score, 1917 is a cinematic achievement that leaves a lasting impact on viewers.</t>
         </is>
       </c>
       <c r="I79" t="n">
@@ -6878,7 +6878,7 @@
         <v>8</v>
       </c>
       <c r="K79" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="L79" t="n">
         <v>9</v>
@@ -6887,11 +6887,11 @@
         <v>7</v>
       </c>
       <c r="N79" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
-          <t>- immersive - technical marvel - breathtaking - visceral - emotional - impressive - naturalistic - grounded - intense - harrowing - powerful - relentless - stunning - beautiful - epic - tense - gripping - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive -</t>
+          <t>- immersive - technical achievement - visceral - emotional - breathtaking - impressive - naturalistic - grounded - intense - harrowing - powerful - relentless - beautiful - stunning - epic - tense - gripping - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive - immersive -</t>
         </is>
       </c>
       <c r="P79" t="n">
@@ -6950,7 +6950,7 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Dunkirk is a war film directed by Christopher Nolan that focuses on the evacuation of Allied soldiers from Dunkirk during World War II. The film is praised for its technical brilliance, intense tension, and immersive experience. While some viewers found it to be a masterpiece, others felt it lacked depth in its characters. Overall, Dunkirk is a visually stunning and gripping portrayal of the horrors of war.</t>
+          <t>Dunkirk is a war film directed by Christopher Nolan that focuses on the evacuation of Allied soldiers from Dunkirk during World War II. The film is praised for its technical brilliance, intense tension, and immersive experience. While some viewers found it stressful and emotionally impactful, others appreciated the lack of traditional narrative and character development. Overall, Dunkirk is considered a masterclass in filmmaking, with stunning visuals, a powerful score by Hans Zimmer, and a unique approach to portraying the horrors of war.</t>
         </is>
       </c>
       <c r="I80" t="n">
@@ -6966,14 +6966,14 @@
         <v>8</v>
       </c>
       <c r="M80" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="N80" t="n">
         <v>9</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>- intense - stressful - tension - harry styles - war - horror - suspenseful - technical masterpiece - immersive - ticking clock - dark-haired british twinks - survival - gripping - emotional - heartbreaking - masterclass - craftsmanship - stunning - visceral - relentless - minimalistic - experimental - historical - realism - haunting - atmospheric - adrenaline rush - breathtaking - jaw-dropping - powerful - gut-wrenching - immersive - heroic - bleak - cruel - arbitrary - intense - emotional - thought-provoking - Nolan-esque - visually stunning - impactful - impressive - captivating - engrossing - immersive - powerful - moving - tense - gripping - thrilling - masterful - brilliant - genius - mesmerizing - unforgettable - cinematic - epic</t>
+          <t>- intense - stressful - tension - harry styles - war - historical - suspenseful - dark-haired british twinks - horror - adrenaline rush - masterful - technical marvel - immersive - gripping - visceral - heartbreaking - powerful - minimalistic - experimental - atmospheric - visually stunning - emotional - heroic - survival - haunting - relentless - gripping - jaw-dropping - intense - immersive - technical masterpiece - breathtaking - grand scale - tense - powerful - masterclass - craftsmanship - stunning - remarkable - intricate - bleak - cruel - thought-provoking - emotional - humanity</t>
         </is>
       </c>
       <c r="P80" t="n">
@@ -7028,11 +7028,11 @@
         <v>4.58</v>
       </c>
       <c r="G81" t="n">
-        <v>0.89</v>
+        <v>0.9</v>
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Schindler's List is a powerful and emotionally devastating film that captures the horrors of the Holocaust through the story of Oskar Schindler, a man who becomes an unexpected hero. Steven Spielberg's direction is masterful, with stunning cinematography and brilliant performances. The film is a poignant masterpiece that transcends the boundaries of cinema, leaving a lasting impact on viewers. It is a must-watch for everyone, showcasing the best of filmmaking and storytelling.</t>
+          <t>Schindler's List is a powerful and emotionally devastating film that captures the horrors of the Holocaust through the story of Oskar Schindler, a man who becomes an unexpected hero. Steven Spielberg's direction is masterful, with stunning cinematography and exceptional performances. The film is a haunting depiction of the atrocities committed against the Jews in Europe, while also offering a message of hope and perseverance. It is considered a cinematic masterpiece and a must-watch for everyone.</t>
         </is>
       </c>
       <c r="I81" t="n">
@@ -7055,7 +7055,7 @@
       </c>
       <c r="O81" t="inlineStr">
         <is>
-          <t>- masterpiece - powerful - moving - iconic - important - emotional - somber - profound - gut-wrenching - intense - harrowing - compelling - poignant - raw - heartbreaking - gripping - visually stunning - cathartic - respectful - true - beautiful - tragic - powerful storytelling - brilliant performances - must-watch - unforgettable - cinematic triumph - historical masterpiece - thought-provoking - impactful - haunting - mesmerizing - captivating - awe-inspiring - legendary - powerful message - cinematic achievement - unparalleled - mesmerizing - flawless - sincere - respectful - courageous - enlightening - educational - transformative - chilling - disturbing - enlightening - significant - timeless - mesmerizing - devastating - extraordinary - compelling - heart-wrenching - powerful imagery - stunning cinematography - emotional depth -</t>
+          <t>- emotional - powerful - masterpiece - moving - important - iconic - somber - profound - gut-wrenching - intense - harrowing - poignant - raw - heartbreaking - cinematic - gripping - visually stunning - brilliant - cathartic - compelling - historical - dark - disturbing - thought-provoking - enlightening - impactful - unforgettable - mesmerizing - chilling - suspenseful - beautiful - symbolic - respectful - honoring - true - perfect - respectful - honoring - true - flawless - sincere - resounding - significant - essential - resiliency - hopeful - resolute - tragic - devastating - resounding - transcendent - triumphant - legendary - haunting - extraordinary - empathetic - empathetic - empathetic - empathetic - empathetic - empathetic - empath</t>
         </is>
       </c>
       <c r="P81" t="n">

</xml_diff>